<commit_message>
Botafogo x Fluminense 04/11/2017
</commit_message>
<xml_diff>
--- a/Jogos do Botafogo que já fui.xlsx
+++ b/Jogos do Botafogo que já fui.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hfogo_000\Documents\Listas Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hfogo_000\Documents\GitHub\JogosDoBotafogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="115">
   <si>
     <t>Sim</t>
   </si>
@@ -764,7 +764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -929,6 +929,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1226,7 +1229,7 @@
   <dimension ref="A1:AE125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A95" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L112" sqref="L112"/>
+      <selection activeCell="K121" sqref="K121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,34 +1262,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="59"/>
-      <c r="Y1" s="59"/>
-      <c r="Z1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="60"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="59"/>
       <c r="AA1" s="46"/>
       <c r="AB1" s="46"/>
       <c r="AC1" s="46"/>
@@ -1424,14 +1427,14 @@
       </c>
       <c r="O3" s="6">
         <f>COUNTIF(I3:I1007,"Série A")</f>
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="Q3" s="6">
         <f>COUNTIF(J2:J1004,"Nilton Santos")</f>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="R3" s="21">
         <v>2004</v>
@@ -1450,15 +1453,15 @@
       </c>
       <c r="V3" s="41">
         <f>COUNTIF(F3:F1007, "Derrota")</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="W3" s="36">
         <f>SUM(G3:G1001)</f>
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="X3" s="42">
         <f>SUM(H3:H1001)</f>
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="Y3" s="43">
         <f>COUNTIF(K3:K1006,"Sim")</f>
@@ -1466,7 +1469,7 @@
       </c>
       <c r="Z3" s="41">
         <f>COUNTIF(K3:K1006,"Não")</f>
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AA3" s="46"/>
       <c r="AB3" s="46"/>
@@ -1513,7 +1516,7 @@
       </c>
       <c r="M4" s="17">
         <f>COUNTIF(B3:B1005,"Fluminense")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N4" s="8" t="s">
         <v>24</v>
@@ -2371,7 +2374,7 @@
       </c>
       <c r="S16" s="30">
         <f>COUNTIF(E3:E1060, "2017")</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="T16" s="47"/>
       <c r="U16" s="48"/>
@@ -7711,7 +7714,7 @@
     </row>
     <row r="110" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A110" s="56">
-        <f t="shared" ref="A110:A119" si="5">SUM(A109+1)</f>
+        <f t="shared" ref="A110:A120" si="5">SUM(A109+1)</f>
         <v>108</v>
       </c>
       <c r="B110" s="56" t="s">
@@ -8220,17 +8223,40 @@
       <c r="Z119" s="46"/>
     </row>
     <row r="120" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A120" s="46"/>
-      <c r="B120" s="46"/>
-      <c r="C120" s="46"/>
-      <c r="D120" s="46"/>
-      <c r="E120" s="46"/>
-      <c r="F120" s="46"/>
-      <c r="G120" s="46"/>
-      <c r="H120" s="46"/>
-      <c r="I120" s="46"/>
-      <c r="J120" s="46"/>
-      <c r="K120" s="46"/>
+      <c r="A120" s="58">
+        <f t="shared" si="5"/>
+        <v>118</v>
+      </c>
+      <c r="B120" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="C120" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="D120" s="1">
+        <v>43043</v>
+      </c>
+      <c r="E120" s="58">
+        <v>2017</v>
+      </c>
+      <c r="F120" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="G120" s="58">
+        <v>1</v>
+      </c>
+      <c r="H120" s="58">
+        <v>2</v>
+      </c>
+      <c r="I120" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="J120" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="K120" s="58" t="s">
+        <v>49</v>
+      </c>
       <c r="L120" s="46"/>
       <c r="M120" s="46"/>
       <c r="N120" s="46"/>

</xml_diff>

<commit_message>
Botafogo x Atlético Paranaense 11/11/2017
</commit_message>
<xml_diff>
--- a/Jogos do Botafogo que já fui.xlsx
+++ b/Jogos do Botafogo que já fui.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="114">
   <si>
     <t>Sim</t>
   </si>
@@ -360,9 +360,6 @@
   </si>
   <si>
     <t>Avaí</t>
-  </si>
-  <si>
-    <t>Atlético-MG</t>
   </si>
   <si>
     <t>3 x 4</t>
@@ -764,7 +761,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -929,6 +926,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1228,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K121" sqref="K121"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,34 +1262,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
-      <c r="U1" s="60"/>
-      <c r="V1" s="60"/>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="60"/>
-      <c r="Z1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="61"/>
+      <c r="W1" s="61"/>
+      <c r="X1" s="61"/>
+      <c r="Y1" s="61"/>
+      <c r="Z1" s="60"/>
       <c r="AA1" s="46"/>
       <c r="AB1" s="46"/>
       <c r="AC1" s="46"/>
@@ -1427,14 +1427,14 @@
       </c>
       <c r="O3" s="6">
         <f>COUNTIF(I3:I1007,"Série A")</f>
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="P3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="Q3" s="6">
         <f>COUNTIF(J2:J1004,"Nilton Santos")</f>
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="R3" s="21">
         <v>2004</v>
@@ -1453,7 +1453,7 @@
       </c>
       <c r="V3" s="41">
         <f>COUNTIF(F3:F1007, "Derrota")</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="W3" s="36">
         <f>SUM(G3:G1001)</f>
@@ -1461,11 +1461,11 @@
       </c>
       <c r="X3" s="42">
         <f>SUM(H3:H1001)</f>
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="Y3" s="43">
         <f>COUNTIF(K3:K1006,"Sim")</f>
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="Z3" s="41">
         <f>COUNTIF(K3:K1006,"Não")</f>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="M7" s="17">
         <f>COUNTIF(B3:B1003,"Atlético Mineiro")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N7" s="22" t="s">
         <v>12</v>
@@ -2165,7 +2165,7 @@
       </c>
       <c r="M13" s="17">
         <f>COUNTIF(B3:B977,"Atlético Paranaense")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N13" s="47"/>
       <c r="O13" s="47"/>
@@ -2374,7 +2374,7 @@
       </c>
       <c r="S16" s="30">
         <f>COUNTIF(E3:E1060, "2017")</f>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="T16" s="47"/>
       <c r="U16" s="48"/>
@@ -4316,7 +4316,7 @@
         <v>0</v>
       </c>
       <c r="L48" s="51" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M48" s="56">
         <f>COUNTIF(B3:B1000,"Nacional-URU")</f>
@@ -7361,7 +7361,7 @@
         <v>101</v>
       </c>
       <c r="B103" s="27" t="s">
-        <v>112</v>
+        <v>53</v>
       </c>
       <c r="C103" s="27" t="s">
         <v>15</v>
@@ -7514,7 +7514,7 @@
         <v>104</v>
       </c>
       <c r="B106" s="55" t="s">
-        <v>112</v>
+        <v>53</v>
       </c>
       <c r="C106" s="55" t="s">
         <v>17</v>
@@ -7568,7 +7568,7 @@
         <v>81</v>
       </c>
       <c r="C107" s="56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D107" s="1">
         <v>42945</v>
@@ -7667,7 +7667,7 @@
         <v>107</v>
       </c>
       <c r="B109" s="56" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C109" s="56" t="s">
         <v>19</v>
@@ -7714,7 +7714,7 @@
     </row>
     <row r="110" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A110" s="56">
-        <f t="shared" ref="A110:A120" si="5">SUM(A109+1)</f>
+        <f t="shared" ref="A110:A121" si="5">SUM(A109+1)</f>
         <v>108</v>
       </c>
       <c r="B110" s="56" t="s">
@@ -8274,17 +8274,40 @@
       <c r="Z120" s="46"/>
     </row>
     <row r="121" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A121" s="46"/>
-      <c r="B121" s="46"/>
-      <c r="C121" s="46"/>
-      <c r="D121" s="46"/>
-      <c r="E121" s="46"/>
-      <c r="F121" s="46"/>
-      <c r="G121" s="46"/>
-      <c r="H121" s="46"/>
-      <c r="I121" s="46"/>
-      <c r="J121" s="46"/>
-      <c r="K121" s="46"/>
+      <c r="A121" s="59">
+        <f t="shared" si="5"/>
+        <v>119</v>
+      </c>
+      <c r="B121" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="C121" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="D121" s="1">
+        <v>43050</v>
+      </c>
+      <c r="E121" s="59">
+        <v>2017</v>
+      </c>
+      <c r="F121" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="G121" s="59">
+        <v>0</v>
+      </c>
+      <c r="H121" s="59">
+        <v>1</v>
+      </c>
+      <c r="I121" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="J121" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="K121" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="L121" s="46"/>
       <c r="M121" s="46"/>
       <c r="N121" s="46"/>

</xml_diff>

<commit_message>
botafogo x atletico goianiense 16112017
</commit_message>
<xml_diff>
--- a/Jogos do Botafogo que já fui.xlsx
+++ b/Jogos do Botafogo que já fui.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="115">
   <si>
     <t>Sim</t>
   </si>
@@ -366,6 +366,9 @@
   </si>
   <si>
     <t>Nacional-URU</t>
+  </si>
+  <si>
+    <t>Atlético Goianiense</t>
   </si>
 </sst>
 </file>
@@ -414,7 +417,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -746,17 +749,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="6"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -922,10 +914,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1228,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,37 +1289,37 @@
       <c r="AE1" s="46"/>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="56" t="s">
+      <c r="G2" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="I2" s="56" t="s">
+      <c r="I2" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="56" t="s">
+      <c r="J2" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="56" t="s">
+      <c r="K2" s="55" t="s">
         <v>66</v>
       </c>
       <c r="L2" s="25" t="s">
@@ -1427,14 +1419,14 @@
       </c>
       <c r="O3" s="6">
         <f>COUNTIF(I3:I1007,"Série A")</f>
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="P3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="Q3" s="6">
         <f>COUNTIF(J2:J1004,"Nilton Santos")</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R3" s="21">
         <v>2004</v>
@@ -1453,15 +1445,15 @@
       </c>
       <c r="V3" s="41">
         <f>COUNTIF(F3:F1007, "Derrota")</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W3" s="36">
         <f>SUM(G3:G1001)</f>
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="X3" s="42">
         <f>SUM(H3:H1001)</f>
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="Y3" s="43">
         <f>COUNTIF(K3:K1006,"Sim")</f>
@@ -1469,7 +1461,7 @@
       </c>
       <c r="Z3" s="41">
         <f>COUNTIF(K3:K1006,"Não")</f>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AA3" s="46"/>
       <c r="AB3" s="46"/>
@@ -1553,14 +1545,14 @@
       <c r="AE4" s="46"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="56">
+      <c r="A5" s="55">
         <f>SUM(A4+1)</f>
         <v>3</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="55" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="1">
@@ -1578,10 +1570,10 @@
       <c r="H5" s="15">
         <v>1</v>
       </c>
-      <c r="I5" s="56" t="s">
+      <c r="I5" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="56" t="s">
+      <c r="J5" s="55" t="s">
         <v>62</v>
       </c>
       <c r="K5" s="7" t="s">
@@ -1629,14 +1621,14 @@
       <c r="AE5" s="46"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A6" s="56">
+      <c r="A6" s="55">
         <f t="shared" ref="A6:A7" si="0">SUM(A5+1)</f>
         <v>4</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="55" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="1">
@@ -1654,10 +1646,10 @@
       <c r="H6" s="15">
         <v>1</v>
       </c>
-      <c r="I6" s="56" t="s">
+      <c r="I6" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="56" t="s">
+      <c r="J6" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K6" s="7" t="s">
@@ -1705,14 +1697,14 @@
       <c r="AE6" s="46"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" s="56">
+      <c r="A7" s="55">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="55" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="1">
@@ -1730,10 +1722,10 @@
       <c r="H7" s="15">
         <v>1</v>
       </c>
-      <c r="I7" s="56" t="s">
+      <c r="I7" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="56" t="s">
+      <c r="J7" s="55" t="s">
         <v>62</v>
       </c>
       <c r="K7" s="7" t="s">
@@ -1781,14 +1773,14 @@
       <c r="AE7" s="46"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="56">
+      <c r="A8" s="55">
         <f t="shared" ref="A8:A18" si="1">SUM(A7+1)</f>
         <v>6</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="55" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="1">
@@ -1806,10 +1798,10 @@
       <c r="H8" s="15">
         <v>0</v>
       </c>
-      <c r="I8" s="56" t="s">
+      <c r="I8" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="56" t="s">
+      <c r="J8" s="55" t="s">
         <v>62</v>
       </c>
       <c r="K8" s="7" t="s">
@@ -1852,14 +1844,14 @@
       <c r="AE8" s="46"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A9" s="56">
+      <c r="A9" s="55">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="C9" s="55" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="1">
@@ -1877,10 +1869,10 @@
       <c r="H9" s="15">
         <v>2</v>
       </c>
-      <c r="I9" s="56" t="s">
+      <c r="I9" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="56" t="s">
+      <c r="J9" s="55" t="s">
         <v>62</v>
       </c>
       <c r="K9" s="7" t="s">
@@ -1923,14 +1915,14 @@
       <c r="AE9" s="46"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A10" s="56">
+      <c r="A10" s="55">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="55" t="s">
         <v>105</v>
       </c>
       <c r="D10" s="1">
@@ -1948,10 +1940,10 @@
       <c r="H10" s="15">
         <v>2</v>
       </c>
-      <c r="I10" s="56" t="s">
+      <c r="I10" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="56" t="s">
+      <c r="J10" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K10" s="7" t="s">
@@ -1969,7 +1961,7 @@
       <c r="P10" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="Q10" s="55">
+      <c r="Q10" s="54">
         <f>COUNTIF(J3:J1008,"Mário Helênio")</f>
         <v>1</v>
       </c>
@@ -1994,14 +1986,14 @@
       <c r="AE10" s="46"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A11" s="56">
+      <c r="A11" s="55">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="55" t="s">
         <v>61</v>
       </c>
       <c r="D11" s="1">
@@ -2019,10 +2011,10 @@
       <c r="H11" s="15">
         <v>4</v>
       </c>
-      <c r="I11" s="56" t="s">
+      <c r="I11" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="56" t="s">
+      <c r="J11" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K11" s="7" t="s">
@@ -2060,14 +2052,14 @@
       <c r="AE11" s="46"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="56">
+      <c r="A12" s="55">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="56" t="s">
+      <c r="C12" s="55" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="1">
@@ -2085,7 +2077,7 @@
       <c r="H12" s="15">
         <v>0</v>
       </c>
-      <c r="I12" s="56" t="s">
+      <c r="I12" s="55" t="s">
         <v>38</v>
       </c>
       <c r="J12" s="2" t="s">
@@ -2126,14 +2118,14 @@
       <c r="AE12" s="46"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="56">
+      <c r="A13" s="55">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="56" t="s">
+      <c r="C13" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="1">
@@ -2151,7 +2143,7 @@
       <c r="H13" s="15">
         <v>1</v>
       </c>
-      <c r="I13" s="56" t="s">
+      <c r="I13" s="55" t="s">
         <v>38</v>
       </c>
       <c r="J13" s="2" t="s">
@@ -2192,14 +2184,14 @@
       <c r="AE13" s="46"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A14" s="56">
+      <c r="A14" s="55">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="56" t="s">
+      <c r="C14" s="55" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="1">
@@ -2217,7 +2209,7 @@
       <c r="H14" s="15">
         <v>2</v>
       </c>
-      <c r="I14" s="56" t="s">
+      <c r="I14" s="55" t="s">
         <v>38</v>
       </c>
       <c r="J14" s="2" t="s">
@@ -2258,14 +2250,14 @@
       <c r="AE14" s="46"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A15" s="56">
+      <c r="A15" s="55">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="56" t="s">
+      <c r="C15" s="55" t="s">
         <v>33</v>
       </c>
       <c r="D15" s="1">
@@ -2283,10 +2275,10 @@
       <c r="H15" s="15">
         <v>1</v>
       </c>
-      <c r="I15" s="56" t="s">
+      <c r="I15" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J15" s="56" t="s">
+      <c r="J15" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K15" s="7" t="s">
@@ -2324,14 +2316,14 @@
       <c r="AE15" s="46"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="56">
+      <c r="A16" s="55">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C16" s="55" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="1">
@@ -2349,10 +2341,10 @@
       <c r="H16" s="15">
         <v>0</v>
       </c>
-      <c r="I16" s="56" t="s">
+      <c r="I16" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J16" s="56" t="s">
+      <c r="J16" s="55" t="s">
         <v>78</v>
       </c>
       <c r="K16" s="7" t="s">
@@ -2374,7 +2366,7 @@
       </c>
       <c r="S16" s="30">
         <f>COUNTIF(E3:E1060, "2017")</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="T16" s="47"/>
       <c r="U16" s="48"/>
@@ -2390,14 +2382,14 @@
       <c r="AE16" s="46"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A17" s="56">
+      <c r="A17" s="55">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="55" t="s">
         <v>58</v>
       </c>
       <c r="D17" s="1">
@@ -2415,10 +2407,10 @@
       <c r="H17" s="15">
         <v>3</v>
       </c>
-      <c r="I17" s="56" t="s">
+      <c r="I17" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="56" t="s">
+      <c r="J17" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K17" s="7" t="s">
@@ -2451,14 +2443,14 @@
       <c r="AE17" s="46"/>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A18" s="56">
+      <c r="A18" s="55">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="55" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="1">
@@ -2476,10 +2468,10 @@
       <c r="H18" s="15">
         <v>1</v>
       </c>
-      <c r="I18" s="56" t="s">
+      <c r="I18" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="56" t="s">
+      <c r="J18" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K18" s="7" t="s">
@@ -2512,14 +2504,14 @@
       <c r="AE18" s="46"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A19" s="56">
+      <c r="A19" s="55">
         <f t="shared" ref="A19:A24" si="2">SUM(A18+1)</f>
         <v>17</v>
       </c>
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="56" t="s">
+      <c r="C19" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D19" s="1">
@@ -2537,10 +2529,10 @@
       <c r="H19" s="15">
         <v>1</v>
       </c>
-      <c r="I19" s="56" t="s">
+      <c r="I19" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J19" s="56" t="s">
+      <c r="J19" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K19" s="7" t="s">
@@ -2573,14 +2565,14 @@
       <c r="AE19" s="46"/>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A20" s="56">
+      <c r="A20" s="55">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="56" t="s">
+      <c r="C20" s="55" t="s">
         <v>47</v>
       </c>
       <c r="D20" s="1">
@@ -2598,10 +2590,10 @@
       <c r="H20" s="15">
         <v>2</v>
       </c>
-      <c r="I20" s="56" t="s">
+      <c r="I20" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J20" s="56" t="s">
+      <c r="J20" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K20" s="7" t="s">
@@ -2634,14 +2626,14 @@
       <c r="AE20" s="46"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A21" s="56">
+      <c r="A21" s="55">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="B21" s="56" t="s">
+      <c r="B21" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="56" t="s">
+      <c r="C21" s="55" t="s">
         <v>57</v>
       </c>
       <c r="D21" s="1">
@@ -2659,10 +2651,10 @@
       <c r="H21" s="15">
         <v>3</v>
       </c>
-      <c r="I21" s="56" t="s">
+      <c r="I21" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J21" s="56" t="s">
+      <c r="J21" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K21" s="7" t="s">
@@ -2695,14 +2687,14 @@
       <c r="AE21" s="46"/>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A22" s="56">
+      <c r="A22" s="55">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="B22" s="56" t="s">
+      <c r="B22" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="56" t="s">
+      <c r="C22" s="55" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="1">
@@ -2720,10 +2712,10 @@
       <c r="H22" s="15">
         <v>1</v>
       </c>
-      <c r="I22" s="56" t="s">
+      <c r="I22" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J22" s="56" t="s">
+      <c r="J22" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K22" s="7" t="s">
@@ -2756,14 +2748,14 @@
       <c r="AE22" s="46"/>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A23" s="56">
+      <c r="A23" s="55">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="B23" s="56" t="s">
+      <c r="B23" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="56" t="s">
+      <c r="C23" s="55" t="s">
         <v>47</v>
       </c>
       <c r="D23" s="1">
@@ -2781,10 +2773,10 @@
       <c r="H23" s="15">
         <v>2</v>
       </c>
-      <c r="I23" s="56" t="s">
+      <c r="I23" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J23" s="56" t="s">
+      <c r="J23" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K23" s="7" t="s">
@@ -2817,14 +2809,14 @@
       <c r="AE23" s="46"/>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A24" s="56">
+      <c r="A24" s="55">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="B24" s="56" t="s">
+      <c r="B24" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="56" t="s">
+      <c r="C24" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="1">
@@ -2842,10 +2834,10 @@
       <c r="H24" s="15">
         <v>1</v>
       </c>
-      <c r="I24" s="56" t="s">
+      <c r="I24" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="J24" s="56" t="s">
+      <c r="J24" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K24" s="7" t="s">
@@ -2878,14 +2870,14 @@
       <c r="AE24" s="46"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A25" s="56">
+      <c r="A25" s="55">
         <f t="shared" ref="A25:A39" si="3">SUM(A24+1)</f>
         <v>23</v>
       </c>
-      <c r="B25" s="56" t="s">
+      <c r="B25" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="56" t="s">
+      <c r="C25" s="55" t="s">
         <v>17</v>
       </c>
       <c r="D25" s="1">
@@ -2903,10 +2895,10 @@
       <c r="H25" s="15">
         <v>0</v>
       </c>
-      <c r="I25" s="56" t="s">
+      <c r="I25" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J25" s="56" t="s">
+      <c r="J25" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K25" s="7" t="s">
@@ -2939,14 +2931,14 @@
       <c r="AE25" s="46"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A26" s="56">
+      <c r="A26" s="55">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="B26" s="56" t="s">
+      <c r="B26" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="56" t="s">
+      <c r="C26" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D26" s="1">
@@ -2964,10 +2956,10 @@
       <c r="H26" s="15">
         <v>1</v>
       </c>
-      <c r="I26" s="56" t="s">
+      <c r="I26" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J26" s="56" t="s">
+      <c r="J26" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K26" s="7" t="s">
@@ -3000,14 +2992,14 @@
       <c r="AE26" s="46"/>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A27" s="56">
+      <c r="A27" s="55">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="B27" s="56" t="s">
+      <c r="B27" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="56" t="s">
+      <c r="C27" s="55" t="s">
         <v>15</v>
       </c>
       <c r="D27" s="1">
@@ -3025,10 +3017,10 @@
       <c r="H27" s="15">
         <v>1</v>
       </c>
-      <c r="I27" s="56" t="s">
+      <c r="I27" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J27" s="56" t="s">
+      <c r="J27" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K27" s="7" t="s">
@@ -3061,7 +3053,7 @@
       <c r="AE27" s="46"/>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A28" s="56">
+      <c r="A28" s="55">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
@@ -3122,14 +3114,14 @@
       <c r="AE28" s="46"/>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A29" s="56">
+      <c r="A29" s="55">
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="56" t="s">
+      <c r="C29" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D29" s="1">
@@ -3147,10 +3139,10 @@
       <c r="H29" s="15">
         <v>1</v>
       </c>
-      <c r="I29" s="56" t="s">
+      <c r="I29" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J29" s="56" t="s">
+      <c r="J29" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K29" s="7" t="s">
@@ -3183,14 +3175,14 @@
       <c r="AE29" s="46"/>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A30" s="56">
+      <c r="A30" s="55">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="B30" s="56" t="s">
+      <c r="B30" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="56" t="s">
+      <c r="C30" s="55" t="s">
         <v>19</v>
       </c>
       <c r="D30" s="1">
@@ -3208,10 +3200,10 @@
       <c r="H30" s="15">
         <v>0</v>
       </c>
-      <c r="I30" s="56" t="s">
+      <c r="I30" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="J30" s="56" t="s">
+      <c r="J30" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K30" s="7" t="s">
@@ -3244,14 +3236,14 @@
       <c r="AE30" s="46"/>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A31" s="56">
+      <c r="A31" s="55">
         <f t="shared" si="3"/>
         <v>29</v>
       </c>
-      <c r="B31" s="56" t="s">
+      <c r="B31" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="56" t="s">
+      <c r="C31" s="55" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="1">
@@ -3269,10 +3261,10 @@
       <c r="H31" s="15">
         <v>1</v>
       </c>
-      <c r="I31" s="56" t="s">
+      <c r="I31" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J31" s="56" t="s">
+      <c r="J31" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K31" s="7" t="s">
@@ -3305,14 +3297,14 @@
       <c r="AE31" s="46"/>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A32" s="56">
+      <c r="A32" s="55">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="B32" s="56" t="s">
+      <c r="B32" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="56" t="s">
+      <c r="C32" s="55" t="s">
         <v>15</v>
       </c>
       <c r="D32" s="1">
@@ -3330,10 +3322,10 @@
       <c r="H32" s="15">
         <v>1</v>
       </c>
-      <c r="I32" s="56" t="s">
+      <c r="I32" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J32" s="56" t="s">
+      <c r="J32" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K32" s="7" t="s">
@@ -3366,14 +3358,14 @@
       <c r="AE32" s="46"/>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A33" s="56">
+      <c r="A33" s="55">
         <f t="shared" si="3"/>
         <v>31</v>
       </c>
-      <c r="B33" s="56" t="s">
+      <c r="B33" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="56" t="s">
+      <c r="C33" s="55" t="s">
         <v>25</v>
       </c>
       <c r="D33" s="1">
@@ -3391,10 +3383,10 @@
       <c r="H33" s="15">
         <v>2</v>
       </c>
-      <c r="I33" s="56" t="s">
+      <c r="I33" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J33" s="56" t="s">
+      <c r="J33" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K33" s="7" t="s">
@@ -3427,14 +3419,14 @@
       <c r="AE33" s="46"/>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A34" s="56">
+      <c r="A34" s="55">
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="B34" s="56" t="s">
+      <c r="B34" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="56" t="s">
+      <c r="C34" s="55" t="s">
         <v>21</v>
       </c>
       <c r="D34" s="1">
@@ -3452,10 +3444,10 @@
       <c r="H34" s="15">
         <v>1</v>
       </c>
-      <c r="I34" s="56" t="s">
+      <c r="I34" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J34" s="56" t="s">
+      <c r="J34" s="55" t="s">
         <v>36</v>
       </c>
       <c r="K34" s="7" t="s">
@@ -3488,14 +3480,14 @@
       <c r="AE34" s="46"/>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A35" s="56">
+      <c r="A35" s="55">
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="B35" s="56" t="s">
+      <c r="B35" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="56" t="s">
+      <c r="C35" s="55" t="s">
         <v>17</v>
       </c>
       <c r="D35" s="1">
@@ -3513,10 +3505,10 @@
       <c r="H35" s="15">
         <v>0</v>
       </c>
-      <c r="I35" s="56" t="s">
+      <c r="I35" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J35" s="56" t="s">
+      <c r="J35" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K35" s="7" t="s">
@@ -3549,14 +3541,14 @@
       <c r="AE35" s="46"/>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A36" s="56">
+      <c r="A36" s="55">
         <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="B36" s="56" t="s">
+      <c r="B36" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="56" t="s">
+      <c r="C36" s="55" t="s">
         <v>31</v>
       </c>
       <c r="D36" s="1">
@@ -3574,10 +3566,10 @@
       <c r="H36" s="15">
         <v>0</v>
       </c>
-      <c r="I36" s="56" t="s">
+      <c r="I36" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J36" s="56" t="s">
+      <c r="J36" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K36" s="7" t="s">
@@ -3610,14 +3602,14 @@
       <c r="AE36" s="46"/>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A37" s="56">
+      <c r="A37" s="55">
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="B37" s="56" t="s">
+      <c r="B37" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="56" t="s">
+      <c r="C37" s="55" t="s">
         <v>51</v>
       </c>
       <c r="D37" s="1">
@@ -3635,10 +3627,10 @@
       <c r="H37" s="15">
         <v>2</v>
       </c>
-      <c r="I37" s="56" t="s">
+      <c r="I37" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J37" s="56" t="s">
+      <c r="J37" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K37" s="7" t="s">
@@ -3671,14 +3663,14 @@
       <c r="AE37" s="46"/>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A38" s="56">
+      <c r="A38" s="55">
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="B38" s="56" t="s">
+      <c r="B38" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="56" t="s">
+      <c r="C38" s="55" t="s">
         <v>50</v>
       </c>
       <c r="D38" s="1">
@@ -3696,10 +3688,10 @@
       <c r="H38" s="15">
         <v>2</v>
       </c>
-      <c r="I38" s="56" t="s">
+      <c r="I38" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J38" s="56" t="s">
+      <c r="J38" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K38" s="7" t="s">
@@ -3732,14 +3724,14 @@
       <c r="AE38" s="46"/>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A39" s="56">
+      <c r="A39" s="55">
         <f t="shared" si="3"/>
         <v>37</v>
       </c>
-      <c r="B39" s="56" t="s">
+      <c r="B39" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="56" t="s">
+      <c r="C39" s="55" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="1">
@@ -3757,10 +3749,10 @@
       <c r="H39" s="15">
         <v>0</v>
       </c>
-      <c r="I39" s="56" t="s">
+      <c r="I39" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J39" s="56" t="s">
+      <c r="J39" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K39" s="7" t="s">
@@ -3793,14 +3785,14 @@
       <c r="AE39" s="46"/>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A40" s="56">
+      <c r="A40" s="55">
         <f t="shared" ref="A40:A109" si="4">SUM(A39+1)</f>
         <v>38</v>
       </c>
-      <c r="B40" s="56" t="s">
+      <c r="B40" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="56" t="s">
+      <c r="C40" s="55" t="s">
         <v>47</v>
       </c>
       <c r="D40" s="1">
@@ -3818,10 +3810,10 @@
       <c r="H40" s="15">
         <v>2</v>
       </c>
-      <c r="I40" s="56" t="s">
+      <c r="I40" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J40" s="56" t="s">
+      <c r="J40" s="55" t="s">
         <v>36</v>
       </c>
       <c r="K40" s="7" t="s">
@@ -3854,14 +3846,14 @@
       <c r="AE40" s="46"/>
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A41" s="56">
+      <c r="A41" s="55">
         <f t="shared" si="4"/>
         <v>39</v>
       </c>
-      <c r="B41" s="56" t="s">
+      <c r="B41" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C41" s="56" t="s">
+      <c r="C41" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D41" s="1">
@@ -3879,10 +3871,10 @@
       <c r="H41" s="15">
         <v>1</v>
       </c>
-      <c r="I41" s="56" t="s">
+      <c r="I41" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J41" s="56" t="s">
+      <c r="J41" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K41" s="7" t="s">
@@ -3915,14 +3907,14 @@
       <c r="AE41" s="46"/>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A42" s="56">
+      <c r="A42" s="55">
         <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="B42" s="56" t="s">
+      <c r="B42" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="56" t="s">
+      <c r="C42" s="55" t="s">
         <v>13</v>
       </c>
       <c r="D42" s="1">
@@ -3940,10 +3932,10 @@
       <c r="H42" s="15">
         <v>1</v>
       </c>
-      <c r="I42" s="56" t="s">
+      <c r="I42" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J42" s="56" t="s">
+      <c r="J42" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K42" s="7" t="s">
@@ -3976,14 +3968,14 @@
       <c r="AE42" s="46"/>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A43" s="56">
+      <c r="A43" s="55">
         <f t="shared" si="4"/>
         <v>41</v>
       </c>
-      <c r="B43" s="56" t="s">
+      <c r="B43" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="C43" s="56" t="s">
+      <c r="C43" s="55" t="s">
         <v>31</v>
       </c>
       <c r="D43" s="1">
@@ -4001,7 +3993,7 @@
       <c r="H43" s="15">
         <v>0</v>
       </c>
-      <c r="I43" s="56" t="s">
+      <c r="I43" s="55" t="s">
         <v>24</v>
       </c>
       <c r="J43" s="2" t="s">
@@ -4037,14 +4029,14 @@
       <c r="AE43" s="46"/>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A44" s="56">
+      <c r="A44" s="55">
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="B44" s="56" t="s">
+      <c r="B44" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="56" t="s">
+      <c r="C44" s="55" t="s">
         <v>13</v>
       </c>
       <c r="D44" s="1">
@@ -4062,10 +4054,10 @@
       <c r="H44" s="15">
         <v>1</v>
       </c>
-      <c r="I44" s="56" t="s">
+      <c r="I44" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J44" s="56" t="s">
+      <c r="J44" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K44" s="7" t="s">
@@ -4098,14 +4090,14 @@
       <c r="AE44" s="46"/>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A45" s="56">
+      <c r="A45" s="55">
         <f t="shared" si="4"/>
         <v>43</v>
       </c>
-      <c r="B45" s="56" t="s">
+      <c r="B45" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="C45" s="56" t="s">
+      <c r="C45" s="55" t="s">
         <v>17</v>
       </c>
       <c r="D45" s="1">
@@ -4123,10 +4115,10 @@
       <c r="H45" s="15">
         <v>0</v>
       </c>
-      <c r="I45" s="56" t="s">
+      <c r="I45" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J45" s="56" t="s">
+      <c r="J45" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K45" s="7" t="s">
@@ -4159,14 +4151,14 @@
       <c r="AE45" s="46"/>
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A46" s="56">
+      <c r="A46" s="55">
         <f t="shared" si="4"/>
         <v>44</v>
       </c>
-      <c r="B46" s="56" t="s">
+      <c r="B46" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="56" t="s">
+      <c r="C46" s="55" t="s">
         <v>6</v>
       </c>
       <c r="D46" s="1">
@@ -4184,10 +4176,10 @@
       <c r="H46" s="15">
         <v>0</v>
       </c>
-      <c r="I46" s="56" t="s">
+      <c r="I46" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="J46" s="56" t="s">
+      <c r="J46" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K46" s="7" t="s">
@@ -4220,14 +4212,14 @@
       <c r="AE46" s="46"/>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A47" s="56">
+      <c r="A47" s="55">
         <f t="shared" si="4"/>
         <v>45</v>
       </c>
-      <c r="B47" s="56" t="s">
+      <c r="B47" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="C47" s="56" t="s">
+      <c r="C47" s="55" t="s">
         <v>31</v>
       </c>
       <c r="D47" s="1">
@@ -4245,10 +4237,10 @@
       <c r="H47" s="15">
         <v>0</v>
       </c>
-      <c r="I47" s="56" t="s">
+      <c r="I47" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="J47" s="56" t="s">
+      <c r="J47" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K47" s="7" t="s">
@@ -4281,14 +4273,14 @@
       <c r="AE47" s="46"/>
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A48" s="56">
+      <c r="A48" s="55">
         <f t="shared" si="4"/>
         <v>46</v>
       </c>
-      <c r="B48" s="56" t="s">
+      <c r="B48" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C48" s="56" t="s">
+      <c r="C48" s="55" t="s">
         <v>13</v>
       </c>
       <c r="D48" s="1">
@@ -4306,10 +4298,10 @@
       <c r="H48" s="15">
         <v>1</v>
       </c>
-      <c r="I48" s="56" t="s">
+      <c r="I48" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J48" s="56" t="s">
+      <c r="J48" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K48" s="7" t="s">
@@ -4318,7 +4310,7 @@
       <c r="L48" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="M48" s="56">
+      <c r="M48" s="55">
         <f>COUNTIF(B3:B1000,"Nacional-URU")</f>
         <v>1</v>
       </c>
@@ -4342,14 +4334,14 @@
       <c r="AE48" s="46"/>
     </row>
     <row r="49" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A49" s="55">
+      <c r="A49" s="54">
         <f t="shared" si="4"/>
         <v>47</v>
       </c>
-      <c r="B49" s="56" t="s">
+      <c r="B49" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="C49" s="56" t="s">
+      <c r="C49" s="55" t="s">
         <v>31</v>
       </c>
       <c r="D49" s="1">
@@ -4367,17 +4359,22 @@
       <c r="H49" s="15">
         <v>0</v>
       </c>
-      <c r="I49" s="56" t="s">
+      <c r="I49" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J49" s="56" t="s">
+      <c r="J49" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K49" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L49" s="47"/>
-      <c r="M49" s="54"/>
+      <c r="L49" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="M49" s="59">
+        <f>COUNTIF(B4:B1001,"Atlético Goianiense")</f>
+        <v>1</v>
+      </c>
       <c r="N49" s="47"/>
       <c r="O49" s="47"/>
       <c r="P49" s="47"/>
@@ -4398,14 +4395,14 @@
       <c r="AE49" s="46"/>
     </row>
     <row r="50" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A50" s="56">
+      <c r="A50" s="55">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="B50" s="56" t="s">
+      <c r="B50" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="C50" s="56" t="s">
+      <c r="C50" s="55" t="s">
         <v>31</v>
       </c>
       <c r="D50" s="1">
@@ -4423,10 +4420,10 @@
       <c r="H50" s="15">
         <v>0</v>
       </c>
-      <c r="I50" s="56" t="s">
+      <c r="I50" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J50" s="56" t="s">
+      <c r="J50" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K50" s="7" t="s">
@@ -4454,14 +4451,14 @@
       <c r="AE50" s="46"/>
     </row>
     <row r="51" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A51" s="56">
+      <c r="A51" s="55">
         <f t="shared" si="4"/>
         <v>49</v>
       </c>
-      <c r="B51" s="55" t="s">
+      <c r="B51" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="C51" s="55" t="s">
+      <c r="C51" s="54" t="s">
         <v>8</v>
       </c>
       <c r="D51" s="18">
@@ -4479,10 +4476,10 @@
       <c r="H51" s="20">
         <v>3</v>
       </c>
-      <c r="I51" s="55" t="s">
+      <c r="I51" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="J51" s="55" t="s">
+      <c r="J51" s="54" t="s">
         <v>23</v>
       </c>
       <c r="K51" s="11" t="s">
@@ -4510,14 +4507,14 @@
       <c r="AE51" s="46"/>
     </row>
     <row r="52" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A52" s="56">
+      <c r="A52" s="55">
         <f t="shared" si="4"/>
         <v>50</v>
       </c>
-      <c r="B52" s="56" t="s">
+      <c r="B52" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="C52" s="56" t="s">
+      <c r="C52" s="55" t="s">
         <v>13</v>
       </c>
       <c r="D52" s="1">
@@ -4535,10 +4532,10 @@
       <c r="H52" s="15">
         <v>1</v>
       </c>
-      <c r="I52" s="56" t="s">
+      <c r="I52" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J52" s="56" t="s">
+      <c r="J52" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K52" s="7" t="s">
@@ -4566,14 +4563,14 @@
       <c r="AE52" s="46"/>
     </row>
     <row r="53" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A53" s="56">
+      <c r="A53" s="55">
         <f t="shared" si="4"/>
         <v>51</v>
       </c>
-      <c r="B53" s="56" t="s">
+      <c r="B53" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="C53" s="56" t="s">
+      <c r="C53" s="55" t="s">
         <v>31</v>
       </c>
       <c r="D53" s="1">
@@ -4591,10 +4588,10 @@
       <c r="H53" s="15">
         <v>0</v>
       </c>
-      <c r="I53" s="56" t="s">
+      <c r="I53" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J53" s="56" t="s">
+      <c r="J53" s="55" t="s">
         <v>36</v>
       </c>
       <c r="K53" s="7" t="s">
@@ -4622,14 +4619,14 @@
       <c r="AE53" s="46"/>
     </row>
     <row r="54" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A54" s="56">
+      <c r="A54" s="55">
         <f t="shared" si="4"/>
         <v>52</v>
       </c>
-      <c r="B54" s="56" t="s">
+      <c r="B54" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="C54" s="56" t="s">
+      <c r="C54" s="55" t="s">
         <v>6</v>
       </c>
       <c r="D54" s="1">
@@ -4647,10 +4644,10 @@
       <c r="H54" s="15">
         <v>0</v>
       </c>
-      <c r="I54" s="56" t="s">
+      <c r="I54" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J54" s="56" t="s">
+      <c r="J54" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K54" s="7" t="s">
@@ -4678,14 +4675,14 @@
       <c r="AE54" s="46"/>
     </row>
     <row r="55" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A55" s="56">
+      <c r="A55" s="55">
         <f t="shared" si="4"/>
         <v>53</v>
       </c>
-      <c r="B55" s="56" t="s">
+      <c r="B55" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="C55" s="56" t="s">
+      <c r="C55" s="55" t="s">
         <v>33</v>
       </c>
       <c r="D55" s="1">
@@ -4703,10 +4700,10 @@
       <c r="H55" s="15">
         <v>1</v>
       </c>
-      <c r="I55" s="56" t="s">
+      <c r="I55" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J55" s="56" t="s">
+      <c r="J55" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K55" s="7" t="s">
@@ -4734,14 +4731,14 @@
       <c r="AE55" s="46"/>
     </row>
     <row r="56" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A56" s="56">
+      <c r="A56" s="55">
         <f t="shared" si="4"/>
         <v>54</v>
       </c>
-      <c r="B56" s="56" t="s">
+      <c r="B56" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C56" s="56" t="s">
+      <c r="C56" s="55" t="s">
         <v>31</v>
       </c>
       <c r="D56" s="1">
@@ -4759,10 +4756,10 @@
       <c r="H56" s="15">
         <v>0</v>
       </c>
-      <c r="I56" s="56" t="s">
+      <c r="I56" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J56" s="56" t="s">
+      <c r="J56" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K56" s="7" t="s">
@@ -4790,14 +4787,14 @@
       <c r="AE56" s="46"/>
     </row>
     <row r="57" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A57" s="56">
+      <c r="A57" s="55">
         <f t="shared" si="4"/>
         <v>55</v>
       </c>
-      <c r="B57" s="56" t="s">
+      <c r="B57" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="C57" s="56" t="s">
+      <c r="C57" s="55" t="s">
         <v>76</v>
       </c>
       <c r="D57" s="1">
@@ -4815,10 +4812,10 @@
       <c r="H57" s="15">
         <v>3</v>
       </c>
-      <c r="I57" s="56" t="s">
+      <c r="I57" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J57" s="56" t="s">
+      <c r="J57" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K57" s="7" t="s">
@@ -4846,14 +4843,14 @@
       <c r="AE57" s="46"/>
     </row>
     <row r="58" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A58" s="56">
+      <c r="A58" s="55">
         <f t="shared" si="4"/>
         <v>56</v>
       </c>
-      <c r="B58" s="56" t="s">
+      <c r="B58" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="C58" s="56" t="s">
+      <c r="C58" s="55" t="s">
         <v>17</v>
       </c>
       <c r="D58" s="1">
@@ -4871,10 +4868,10 @@
       <c r="H58" s="15">
         <v>0</v>
       </c>
-      <c r="I58" s="56" t="s">
+      <c r="I58" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J58" s="56" t="s">
+      <c r="J58" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K58" s="7" t="s">
@@ -4902,14 +4899,14 @@
       <c r="AE58" s="46"/>
     </row>
     <row r="59" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A59" s="56">
+      <c r="A59" s="55">
         <f t="shared" si="4"/>
         <v>57</v>
       </c>
-      <c r="B59" s="56" t="s">
+      <c r="B59" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C59" s="56" t="s">
+      <c r="C59" s="55" t="s">
         <v>15</v>
       </c>
       <c r="D59" s="1">
@@ -4927,10 +4924,10 @@
       <c r="H59" s="15">
         <v>1</v>
       </c>
-      <c r="I59" s="56" t="s">
+      <c r="I59" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J59" s="56" t="s">
+      <c r="J59" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K59" s="7" t="s">
@@ -4958,14 +4955,14 @@
       <c r="AE59" s="46"/>
     </row>
     <row r="60" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A60" s="56">
+      <c r="A60" s="55">
         <f t="shared" si="4"/>
         <v>58</v>
       </c>
-      <c r="B60" s="56" t="s">
+      <c r="B60" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C60" s="56" t="s">
+      <c r="C60" s="55" t="s">
         <v>21</v>
       </c>
       <c r="D60" s="1">
@@ -4983,10 +4980,10 @@
       <c r="H60" s="15">
         <v>1</v>
       </c>
-      <c r="I60" s="56" t="s">
+      <c r="I60" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J60" s="56" t="s">
+      <c r="J60" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K60" s="7" t="s">
@@ -5014,14 +5011,14 @@
       <c r="AE60" s="46"/>
     </row>
     <row r="61" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A61" s="56">
+      <c r="A61" s="55">
         <f t="shared" si="4"/>
         <v>59</v>
       </c>
-      <c r="B61" s="56" t="s">
+      <c r="B61" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C61" s="56" t="s">
+      <c r="C61" s="55" t="s">
         <v>25</v>
       </c>
       <c r="D61" s="1">
@@ -5039,10 +5036,10 @@
       <c r="H61" s="15">
         <v>2</v>
       </c>
-      <c r="I61" s="56" t="s">
+      <c r="I61" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J61" s="56" t="s">
+      <c r="J61" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K61" s="7" t="s">
@@ -5070,14 +5067,14 @@
       <c r="AE61" s="46"/>
     </row>
     <row r="62" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A62" s="56">
+      <c r="A62" s="55">
         <f t="shared" si="4"/>
         <v>60</v>
       </c>
-      <c r="B62" s="56" t="s">
+      <c r="B62" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="C62" s="56" t="s">
+      <c r="C62" s="55" t="s">
         <v>21</v>
       </c>
       <c r="D62" s="1">
@@ -5095,10 +5092,10 @@
       <c r="H62" s="15">
         <v>1</v>
       </c>
-      <c r="I62" s="56" t="s">
+      <c r="I62" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="J62" s="56" t="s">
+      <c r="J62" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K62" s="7" t="s">
@@ -5126,14 +5123,14 @@
       <c r="AE62" s="46"/>
     </row>
     <row r="63" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A63" s="56">
+      <c r="A63" s="55">
         <f t="shared" si="4"/>
         <v>61</v>
       </c>
-      <c r="B63" s="56" t="s">
+      <c r="B63" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="C63" s="56" t="s">
+      <c r="C63" s="55" t="s">
         <v>19</v>
       </c>
       <c r="D63" s="1">
@@ -5151,10 +5148,10 @@
       <c r="H63" s="15">
         <v>0</v>
       </c>
-      <c r="I63" s="56" t="s">
+      <c r="I63" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="J63" s="56" t="s">
+      <c r="J63" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K63" s="7" t="s">
@@ -5182,14 +5179,14 @@
       <c r="AE63" s="46"/>
     </row>
     <row r="64" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A64" s="56">
+      <c r="A64" s="55">
         <f t="shared" si="4"/>
         <v>62</v>
       </c>
-      <c r="B64" s="56" t="s">
+      <c r="B64" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="C64" s="56" t="s">
+      <c r="C64" s="55" t="s">
         <v>17</v>
       </c>
       <c r="D64" s="1">
@@ -5207,10 +5204,10 @@
       <c r="H64" s="15">
         <v>0</v>
       </c>
-      <c r="I64" s="56" t="s">
+      <c r="I64" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="J64" s="56" t="s">
+      <c r="J64" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K64" s="7" t="s">
@@ -5238,14 +5235,14 @@
       <c r="AE64" s="46"/>
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A65" s="56">
+      <c r="A65" s="55">
         <f t="shared" si="4"/>
         <v>63</v>
       </c>
-      <c r="B65" s="56" t="s">
+      <c r="B65" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="C65" s="56" t="s">
+      <c r="C65" s="55" t="s">
         <v>15</v>
       </c>
       <c r="D65" s="1">
@@ -5263,10 +5260,10 @@
       <c r="H65" s="15">
         <v>1</v>
       </c>
-      <c r="I65" s="56" t="s">
+      <c r="I65" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="J65" s="56" t="s">
+      <c r="J65" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K65" s="7" t="s">
@@ -5294,14 +5291,14 @@
       <c r="AE65" s="46"/>
     </row>
     <row r="66" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A66" s="56">
+      <c r="A66" s="55">
         <f t="shared" si="4"/>
         <v>64</v>
       </c>
-      <c r="B66" s="56" t="s">
+      <c r="B66" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="C66" s="56" t="s">
+      <c r="C66" s="55" t="s">
         <v>13</v>
       </c>
       <c r="D66" s="1">
@@ -5319,10 +5316,10 @@
       <c r="H66" s="15">
         <v>1</v>
       </c>
-      <c r="I66" s="56" t="s">
+      <c r="I66" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="J66" s="56" t="s">
+      <c r="J66" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K66" s="7" t="s">
@@ -5350,14 +5347,14 @@
       <c r="AE66" s="46"/>
     </row>
     <row r="67" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A67" s="56">
+      <c r="A67" s="55">
         <f t="shared" si="4"/>
         <v>65</v>
       </c>
-      <c r="B67" s="56" t="s">
+      <c r="B67" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="C67" s="56" t="s">
+      <c r="C67" s="55" t="s">
         <v>10</v>
       </c>
       <c r="D67" s="1">
@@ -5375,10 +5372,10 @@
       <c r="H67" s="15">
         <v>0</v>
       </c>
-      <c r="I67" s="56" t="s">
+      <c r="I67" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="J67" s="56" t="s">
+      <c r="J67" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K67" s="7" t="s">
@@ -5406,14 +5403,14 @@
       <c r="AE67" s="46"/>
     </row>
     <row r="68" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A68" s="56">
+      <c r="A68" s="55">
         <f t="shared" si="4"/>
         <v>66</v>
       </c>
-      <c r="B68" s="56" t="s">
+      <c r="B68" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="C68" s="56" t="s">
+      <c r="C68" s="55" t="s">
         <v>8</v>
       </c>
       <c r="D68" s="1">
@@ -5431,10 +5428,10 @@
       <c r="H68" s="15">
         <v>3</v>
       </c>
-      <c r="I68" s="56" t="s">
+      <c r="I68" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="J68" s="56" t="s">
+      <c r="J68" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K68" s="7" t="s">
@@ -5462,14 +5459,14 @@
       <c r="AE68" s="46"/>
     </row>
     <row r="69" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A69" s="56">
+      <c r="A69" s="55">
         <f t="shared" si="4"/>
         <v>67</v>
       </c>
-      <c r="B69" s="56" t="s">
+      <c r="B69" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="56" t="s">
+      <c r="C69" s="55" t="s">
         <v>6</v>
       </c>
       <c r="D69" s="1">
@@ -5487,10 +5484,10 @@
       <c r="H69" s="15">
         <v>0</v>
       </c>
-      <c r="I69" s="56" t="s">
+      <c r="I69" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="J69" s="56" t="s">
+      <c r="J69" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K69" s="7" t="s">
@@ -5518,14 +5515,14 @@
       <c r="AE69" s="46"/>
     </row>
     <row r="70" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A70" s="56">
+      <c r="A70" s="55">
         <f t="shared" si="4"/>
         <v>68</v>
       </c>
-      <c r="B70" s="56" t="s">
+      <c r="B70" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="56" t="s">
+      <c r="C70" s="55" t="s">
         <v>4</v>
       </c>
       <c r="D70" s="1">
@@ -5543,10 +5540,10 @@
       <c r="H70" s="15">
         <v>3</v>
       </c>
-      <c r="I70" s="56" t="s">
+      <c r="I70" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="J70" s="56" t="s">
+      <c r="J70" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K70" s="7" t="s">
@@ -5574,14 +5571,14 @@
       <c r="AE70" s="46"/>
     </row>
     <row r="71" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A71" s="56">
+      <c r="A71" s="55">
         <f t="shared" si="4"/>
         <v>69</v>
       </c>
-      <c r="B71" s="56" t="s">
+      <c r="B71" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="C71" s="56" t="s">
+      <c r="C71" s="55" t="s">
         <v>10</v>
       </c>
       <c r="D71" s="1">
@@ -5599,10 +5596,10 @@
       <c r="H71" s="15">
         <v>0</v>
       </c>
-      <c r="I71" s="56" t="s">
+      <c r="I71" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="J71" s="56" t="s">
+      <c r="J71" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K71" s="7" t="s">
@@ -5630,14 +5627,14 @@
       <c r="AE71" s="46"/>
     </row>
     <row r="72" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A72" s="56">
+      <c r="A72" s="55">
         <f t="shared" si="4"/>
         <v>70</v>
       </c>
-      <c r="B72" s="56" t="s">
+      <c r="B72" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="C72" s="56" t="s">
+      <c r="C72" s="55" t="s">
         <v>33</v>
       </c>
       <c r="D72" s="1">
@@ -5655,10 +5652,10 @@
       <c r="H72" s="15">
         <v>1</v>
       </c>
-      <c r="I72" s="56" t="s">
+      <c r="I72" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J72" s="56" t="s">
+      <c r="J72" s="55" t="s">
         <v>36</v>
       </c>
       <c r="K72" s="7" t="s">
@@ -5686,14 +5683,14 @@
       <c r="AE72" s="46"/>
     </row>
     <row r="73" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A73" s="56">
+      <c r="A73" s="55">
         <f t="shared" si="4"/>
         <v>71</v>
       </c>
-      <c r="B73" s="56" t="s">
+      <c r="B73" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="C73" s="56" t="s">
+      <c r="C73" s="55" t="s">
         <v>31</v>
       </c>
       <c r="D73" s="1">
@@ -5711,10 +5708,10 @@
       <c r="H73" s="15">
         <v>0</v>
       </c>
-      <c r="I73" s="56" t="s">
+      <c r="I73" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J73" s="56" t="s">
+      <c r="J73" s="55" t="s">
         <v>36</v>
       </c>
       <c r="K73" s="7" t="s">
@@ -5742,14 +5739,14 @@
       <c r="AE73" s="46"/>
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A74" s="56">
+      <c r="A74" s="55">
         <f t="shared" si="4"/>
         <v>72</v>
       </c>
-      <c r="B74" s="56" t="s">
+      <c r="B74" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C74" s="56" t="s">
+      <c r="C74" s="55" t="s">
         <v>13</v>
       </c>
       <c r="D74" s="1">
@@ -5767,10 +5764,10 @@
       <c r="H74" s="15">
         <v>1</v>
       </c>
-      <c r="I74" s="56" t="s">
+      <c r="I74" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J74" s="56" t="s">
+      <c r="J74" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K74" s="7" t="s">
@@ -5798,14 +5795,14 @@
       <c r="AE74" s="46"/>
     </row>
     <row r="75" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A75" s="56">
+      <c r="A75" s="55">
         <f t="shared" si="4"/>
         <v>73</v>
       </c>
-      <c r="B75" s="56" t="s">
+      <c r="B75" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C75" s="56" t="s">
+      <c r="C75" s="55" t="s">
         <v>75</v>
       </c>
       <c r="D75" s="1">
@@ -5823,10 +5820,10 @@
       <c r="H75" s="15">
         <v>1</v>
       </c>
-      <c r="I75" s="56" t="s">
+      <c r="I75" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J75" s="56" t="s">
+      <c r="J75" s="55" t="s">
         <v>23</v>
       </c>
       <c r="K75" s="7" t="s">
@@ -5854,14 +5851,14 @@
       <c r="AE75" s="46"/>
     </row>
     <row r="76" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A76" s="56">
+      <c r="A76" s="55">
         <f t="shared" si="4"/>
         <v>74</v>
       </c>
-      <c r="B76" s="56" t="s">
+      <c r="B76" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="C76" s="56" t="s">
+      <c r="C76" s="55" t="s">
         <v>77</v>
       </c>
       <c r="D76" s="1">
@@ -5879,7 +5876,7 @@
       <c r="H76" s="15">
         <v>1</v>
       </c>
-      <c r="I76" s="56" t="s">
+      <c r="I76" s="55" t="s">
         <v>38</v>
       </c>
       <c r="J76" s="2" t="s">
@@ -5910,14 +5907,14 @@
       <c r="AE76" s="46"/>
     </row>
     <row r="77" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A77" s="56">
+      <c r="A77" s="55">
         <f t="shared" si="4"/>
         <v>75</v>
       </c>
-      <c r="B77" s="56" t="s">
+      <c r="B77" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C77" s="56" t="s">
+      <c r="C77" s="55" t="s">
         <v>33</v>
       </c>
       <c r="D77" s="1">
@@ -5935,10 +5932,10 @@
       <c r="H77" s="15">
         <v>1</v>
       </c>
-      <c r="I77" s="56" t="s">
+      <c r="I77" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J77" s="56" t="s">
+      <c r="J77" s="55" t="s">
         <v>80</v>
       </c>
       <c r="K77" s="7" t="s">
@@ -5966,14 +5963,14 @@
       <c r="AE77" s="46"/>
     </row>
     <row r="78" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A78" s="56">
+      <c r="A78" s="55">
         <f t="shared" si="4"/>
         <v>76</v>
       </c>
-      <c r="B78" s="56" t="s">
+      <c r="B78" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="C78" s="56" t="s">
+      <c r="C78" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D78" s="1">
@@ -5991,10 +5988,10 @@
       <c r="H78" s="15">
         <v>1</v>
       </c>
-      <c r="I78" s="56" t="s">
+      <c r="I78" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J78" s="56" t="s">
+      <c r="J78" s="55" t="s">
         <v>95</v>
       </c>
       <c r="K78" s="7" t="s">
@@ -6022,35 +6019,35 @@
       <c r="AE78" s="46"/>
     </row>
     <row r="79" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A79" s="56">
+      <c r="A79" s="55">
         <f t="shared" si="4"/>
         <v>77</v>
       </c>
-      <c r="B79" s="56" t="s">
+      <c r="B79" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="C79" s="56" t="s">
+      <c r="C79" s="55" t="s">
         <v>33</v>
       </c>
       <c r="D79" s="1">
         <v>42617</v>
       </c>
-      <c r="E79" s="56">
+      <c r="E79" s="55">
         <v>2016</v>
       </c>
-      <c r="F79" s="56" t="s">
+      <c r="F79" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G79" s="56">
+      <c r="G79" s="55">
         <v>2</v>
       </c>
       <c r="H79" s="15">
         <v>1</v>
       </c>
-      <c r="I79" s="56" t="s">
+      <c r="I79" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J79" s="56" t="s">
+      <c r="J79" s="55" t="s">
         <v>95</v>
       </c>
       <c r="K79" s="7" t="s">
@@ -6078,35 +6075,35 @@
       <c r="AE79" s="46"/>
     </row>
     <row r="80" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A80" s="56">
+      <c r="A80" s="55">
         <f t="shared" si="4"/>
         <v>78</v>
       </c>
-      <c r="B80" s="56" t="s">
+      <c r="B80" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="C80" s="56" t="s">
+      <c r="C80" s="55" t="s">
         <v>31</v>
       </c>
       <c r="D80" s="1">
         <v>42620</v>
       </c>
-      <c r="E80" s="56">
+      <c r="E80" s="55">
         <v>2016</v>
       </c>
-      <c r="F80" s="56" t="s">
+      <c r="F80" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G80" s="56">
+      <c r="G80" s="55">
         <v>1</v>
       </c>
       <c r="H80" s="15">
         <v>0</v>
       </c>
-      <c r="I80" s="56" t="s">
+      <c r="I80" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J80" s="56" t="s">
+      <c r="J80" s="55" t="s">
         <v>95</v>
       </c>
       <c r="K80" s="7" t="s">
@@ -6134,14 +6131,14 @@
       <c r="AE80" s="46"/>
     </row>
     <row r="81" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A81" s="56">
+      <c r="A81" s="55">
         <f t="shared" si="4"/>
         <v>79</v>
       </c>
-      <c r="B81" s="56" t="s">
+      <c r="B81" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="C81" s="56" t="s">
+      <c r="C81" s="55" t="s">
         <v>31</v>
       </c>
       <c r="D81" s="1">
@@ -6150,19 +6147,19 @@
       <c r="E81" s="15">
         <v>2016</v>
       </c>
-      <c r="F81" s="56" t="s">
+      <c r="F81" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G81" s="56">
+      <c r="G81" s="55">
         <v>1</v>
       </c>
       <c r="H81" s="15">
         <v>0</v>
       </c>
-      <c r="I81" s="56" t="s">
+      <c r="I81" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J81" s="56" t="s">
+      <c r="J81" s="55" t="s">
         <v>95</v>
       </c>
       <c r="K81" s="7" t="s">
@@ -6190,14 +6187,14 @@
       <c r="AE81" s="46"/>
     </row>
     <row r="82" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A82" s="56">
+      <c r="A82" s="55">
         <f t="shared" si="4"/>
         <v>80</v>
       </c>
-      <c r="B82" s="56" t="s">
+      <c r="B82" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="C82" s="56" t="s">
+      <c r="C82" s="55" t="s">
         <v>96</v>
       </c>
       <c r="D82" s="1">
@@ -6206,19 +6203,19 @@
       <c r="E82" s="15">
         <v>2016</v>
       </c>
-      <c r="F82" s="56" t="s">
+      <c r="F82" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G82" s="56">
+      <c r="G82" s="55">
         <v>3</v>
       </c>
       <c r="H82" s="15">
         <v>2</v>
       </c>
-      <c r="I82" s="56" t="s">
+      <c r="I82" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J82" s="56" t="s">
+      <c r="J82" s="55" t="s">
         <v>95</v>
       </c>
       <c r="K82" s="7" t="s">
@@ -6246,14 +6243,14 @@
       <c r="AE82" s="46"/>
     </row>
     <row r="83" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A83" s="56">
+      <c r="A83" s="55">
         <f t="shared" si="4"/>
         <v>81</v>
       </c>
-      <c r="B83" s="56" t="s">
+      <c r="B83" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="C83" s="56" t="s">
+      <c r="C83" s="55" t="s">
         <v>10</v>
       </c>
       <c r="D83" s="1">
@@ -6262,19 +6259,19 @@
       <c r="E83" s="15">
         <v>2016</v>
       </c>
-      <c r="F83" s="56" t="s">
+      <c r="F83" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="G83" s="56">
+      <c r="G83" s="55">
         <v>0</v>
       </c>
       <c r="H83" s="15">
         <v>0</v>
       </c>
-      <c r="I83" s="56" t="s">
+      <c r="I83" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J83" s="56" t="s">
+      <c r="J83" s="55" t="s">
         <v>95</v>
       </c>
       <c r="K83" s="7" t="s">
@@ -6302,14 +6299,14 @@
       <c r="AE83" s="46"/>
     </row>
     <row r="84" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A84" s="56">
+      <c r="A84" s="55">
         <f t="shared" si="4"/>
         <v>82</v>
       </c>
-      <c r="B84" s="56" t="s">
+      <c r="B84" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="C84" s="56" t="s">
+      <c r="C84" s="55" t="s">
         <v>50</v>
       </c>
       <c r="D84" s="1">
@@ -6318,19 +6315,19 @@
       <c r="E84" s="15">
         <v>2016</v>
       </c>
-      <c r="F84" s="56" t="s">
+      <c r="F84" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="G84" s="56">
+      <c r="G84" s="55">
         <v>0</v>
       </c>
       <c r="H84" s="15">
         <v>2</v>
       </c>
-      <c r="I84" s="56" t="s">
+      <c r="I84" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J84" s="56" t="s">
+      <c r="J84" s="55" t="s">
         <v>95</v>
       </c>
       <c r="K84" s="7" t="s">
@@ -6358,14 +6355,14 @@
       <c r="AE84" s="46"/>
     </row>
     <row r="85" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A85" s="56">
+      <c r="A85" s="55">
         <f t="shared" si="4"/>
         <v>83</v>
       </c>
-      <c r="B85" s="56" t="s">
+      <c r="B85" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="C85" s="56" t="s">
+      <c r="C85" s="55" t="s">
         <v>75</v>
       </c>
       <c r="D85" s="1">
@@ -6374,19 +6371,19 @@
       <c r="E85" s="15">
         <v>2016</v>
       </c>
-      <c r="F85" s="56" t="s">
+      <c r="F85" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="G85" s="56">
+      <c r="G85" s="55">
         <v>1</v>
       </c>
       <c r="H85" s="15">
         <v>1</v>
       </c>
-      <c r="I85" s="56" t="s">
+      <c r="I85" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J85" s="56" t="s">
+      <c r="J85" s="55" t="s">
         <v>95</v>
       </c>
       <c r="K85" s="7" t="s">
@@ -6414,7 +6411,7 @@
       <c r="AE85" s="46"/>
     </row>
     <row r="86" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A86" s="56">
+      <c r="A86" s="55">
         <f t="shared" si="4"/>
         <v>84</v>
       </c>
@@ -6430,19 +6427,19 @@
       <c r="E86" s="28">
         <v>2017</v>
       </c>
-      <c r="F86" s="56" t="s">
+      <c r="F86" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="G86" s="56">
+      <c r="G86" s="55">
         <v>1</v>
       </c>
       <c r="H86" s="15">
         <v>1</v>
       </c>
-      <c r="I86" s="56" t="s">
+      <c r="I86" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J86" s="56" t="s">
+      <c r="J86" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K86" s="7" t="s">
@@ -6470,14 +6467,14 @@
       <c r="AE86" s="46"/>
     </row>
     <row r="87" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A87" s="56">
+      <c r="A87" s="55">
         <f t="shared" si="4"/>
         <v>85</v>
       </c>
-      <c r="B87" s="56" t="s">
+      <c r="B87" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="C87" s="56" t="s">
+      <c r="C87" s="55" t="s">
         <v>33</v>
       </c>
       <c r="D87" s="1">
@@ -6486,19 +6483,19 @@
       <c r="E87" s="15">
         <v>2017</v>
       </c>
-      <c r="F87" s="56" t="s">
+      <c r="F87" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G87" s="56">
+      <c r="G87" s="55">
         <v>2</v>
       </c>
       <c r="H87" s="15">
         <v>1</v>
       </c>
-      <c r="I87" s="56" t="s">
+      <c r="I87" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="J87" s="56" t="s">
+      <c r="J87" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K87" s="7" t="s">
@@ -6526,35 +6523,35 @@
       <c r="AE87" s="46"/>
     </row>
     <row r="88" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A88" s="56">
+      <c r="A88" s="55">
         <f t="shared" si="4"/>
         <v>86</v>
       </c>
-      <c r="B88" s="56" t="s">
+      <c r="B88" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="C88" s="56" t="s">
+      <c r="C88" s="55" t="s">
         <v>33</v>
       </c>
       <c r="D88" s="1">
         <v>42770</v>
       </c>
-      <c r="E88" s="56">
+      <c r="E88" s="55">
         <v>2017</v>
       </c>
-      <c r="F88" s="56" t="s">
+      <c r="F88" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G88" s="56">
+      <c r="G88" s="55">
         <v>2</v>
       </c>
-      <c r="H88" s="56">
-        <v>1</v>
-      </c>
-      <c r="I88" s="56" t="s">
+      <c r="H88" s="55">
+        <v>1</v>
+      </c>
+      <c r="I88" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J88" s="56" t="s">
+      <c r="J88" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K88" s="7" t="s">
@@ -6582,35 +6579,35 @@
       <c r="AE88" s="46"/>
     </row>
     <row r="89" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A89" s="55">
+      <c r="A89" s="54">
         <f t="shared" si="4"/>
         <v>87</v>
       </c>
-      <c r="B89" s="55" t="s">
+      <c r="B89" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="C89" s="55" t="s">
+      <c r="C89" s="54" t="s">
         <v>31</v>
       </c>
       <c r="D89" s="18">
         <v>42781</v>
       </c>
-      <c r="E89" s="55">
+      <c r="E89" s="54">
         <v>2017</v>
       </c>
-      <c r="F89" s="55" t="s">
+      <c r="F89" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G89" s="55">
-        <v>1</v>
-      </c>
-      <c r="H89" s="55">
-        <v>0</v>
-      </c>
-      <c r="I89" s="55" t="s">
+      <c r="G89" s="54">
+        <v>1</v>
+      </c>
+      <c r="H89" s="54">
+        <v>0</v>
+      </c>
+      <c r="I89" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="J89" s="55" t="s">
+      <c r="J89" s="54" t="s">
         <v>1</v>
       </c>
       <c r="K89" s="11" t="s">
@@ -6638,14 +6635,14 @@
       <c r="AE89" s="46"/>
     </row>
     <row r="90" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A90" s="56">
+      <c r="A90" s="55">
         <f t="shared" si="4"/>
         <v>88</v>
       </c>
-      <c r="B90" s="56" t="s">
+      <c r="B90" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="C90" s="56" t="s">
+      <c r="C90" s="55" t="s">
         <v>31</v>
       </c>
       <c r="D90" s="1">
@@ -6654,19 +6651,19 @@
       <c r="E90" s="15">
         <v>2017</v>
       </c>
-      <c r="F90" s="56" t="s">
+      <c r="F90" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G90" s="56">
+      <c r="G90" s="55">
         <v>1</v>
       </c>
       <c r="H90" s="15">
         <v>0</v>
       </c>
-      <c r="I90" s="56" t="s">
+      <c r="I90" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J90" s="56" t="s">
+      <c r="J90" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K90" s="7" t="s">
@@ -6694,14 +6691,14 @@
       <c r="AE90" s="46"/>
     </row>
     <row r="91" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A91" s="56">
+      <c r="A91" s="55">
         <f t="shared" si="4"/>
         <v>89</v>
       </c>
-      <c r="B91" s="56" t="s">
+      <c r="B91" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C91" s="56" t="s">
+      <c r="C91" s="55" t="s">
         <v>10</v>
       </c>
       <c r="D91" s="1">
@@ -6710,19 +6707,19 @@
       <c r="E91" s="15">
         <v>2017</v>
       </c>
-      <c r="F91" s="56" t="s">
+      <c r="F91" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="G91" s="56">
+      <c r="G91" s="55">
         <v>0</v>
       </c>
       <c r="H91" s="15">
         <v>0</v>
       </c>
-      <c r="I91" s="56" t="s">
+      <c r="I91" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J91" s="56" t="s">
+      <c r="J91" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K91" s="7" t="s">
@@ -6750,14 +6747,14 @@
       <c r="AE91" s="46"/>
     </row>
     <row r="92" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A92" s="56">
+      <c r="A92" s="55">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
-      <c r="B92" s="56" t="s">
+      <c r="B92" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="C92" s="56" t="s">
+      <c r="C92" s="55" t="s">
         <v>8</v>
       </c>
       <c r="D92" s="1">
@@ -6766,19 +6763,19 @@
       <c r="E92" s="15">
         <v>2017</v>
       </c>
-      <c r="F92" s="56" t="s">
+      <c r="F92" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="G92" s="56">
+      <c r="G92" s="55">
         <v>2</v>
       </c>
       <c r="H92" s="15">
         <v>3</v>
       </c>
-      <c r="I92" s="56" t="s">
+      <c r="I92" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J92" s="56" t="s">
+      <c r="J92" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K92" s="7" t="s">
@@ -6806,14 +6803,14 @@
       <c r="AE92" s="46"/>
     </row>
     <row r="93" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A93" s="56">
+      <c r="A93" s="55">
         <f t="shared" si="4"/>
         <v>91</v>
       </c>
-      <c r="B93" s="56" t="s">
+      <c r="B93" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="C93" s="56" t="s">
+      <c r="C93" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D93" s="1">
@@ -6822,19 +6819,19 @@
       <c r="E93" s="15">
         <v>2017</v>
       </c>
-      <c r="F93" s="56" t="s">
+      <c r="F93" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G93" s="56">
+      <c r="G93" s="55">
         <v>3</v>
       </c>
       <c r="H93" s="15">
         <v>1</v>
       </c>
-      <c r="I93" s="56" t="s">
+      <c r="I93" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J93" s="56" t="s">
+      <c r="J93" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K93" s="7" t="s">
@@ -6862,14 +6859,14 @@
       <c r="AE93" s="46"/>
     </row>
     <row r="94" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A94" s="56">
+      <c r="A94" s="55">
         <f t="shared" si="4"/>
         <v>92</v>
       </c>
-      <c r="B94" s="56" t="s">
+      <c r="B94" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C94" s="56" t="s">
+      <c r="C94" s="55" t="s">
         <v>50</v>
       </c>
       <c r="D94" s="1">
@@ -6878,19 +6875,19 @@
       <c r="E94" s="15">
         <v>2017</v>
       </c>
-      <c r="F94" s="56" t="s">
+      <c r="F94" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="G94" s="56">
+      <c r="G94" s="55">
         <v>0</v>
       </c>
       <c r="H94" s="15">
         <v>2</v>
       </c>
-      <c r="I94" s="56" t="s">
+      <c r="I94" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J94" s="56" t="s">
+      <c r="J94" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K94" s="7" t="s">
@@ -6918,14 +6915,14 @@
       <c r="AE94" s="46"/>
     </row>
     <row r="95" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A95" s="56">
+      <c r="A95" s="55">
         <f t="shared" si="4"/>
         <v>93</v>
       </c>
-      <c r="B95" s="56" t="s">
+      <c r="B95" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="C95" s="56" t="s">
+      <c r="C95" s="55" t="s">
         <v>107</v>
       </c>
       <c r="D95" s="1">
@@ -6934,19 +6931,19 @@
       <c r="E95" s="15">
         <v>2017</v>
       </c>
-      <c r="F95" s="56" t="s">
+      <c r="F95" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G95" s="56">
+      <c r="G95" s="55">
         <v>2</v>
       </c>
       <c r="H95" s="15">
         <v>1</v>
       </c>
-      <c r="I95" s="56" t="s">
+      <c r="I95" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="J95" s="56" t="s">
+      <c r="J95" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K95" s="7" t="s">
@@ -6974,14 +6971,14 @@
       <c r="AE95" s="46"/>
     </row>
     <row r="96" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A96" s="56">
+      <c r="A96" s="55">
         <f t="shared" si="4"/>
         <v>94</v>
       </c>
-      <c r="B96" s="56" t="s">
+      <c r="B96" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="C96" s="56" t="s">
+      <c r="C96" s="55" t="s">
         <v>50</v>
       </c>
       <c r="D96" s="1">
@@ -6990,19 +6987,19 @@
       <c r="E96" s="15">
         <v>2017</v>
       </c>
-      <c r="F96" s="56" t="s">
+      <c r="F96" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="G96" s="56">
+      <c r="G96" s="55">
         <v>0</v>
       </c>
       <c r="H96" s="15">
         <v>2</v>
       </c>
-      <c r="I96" s="56" t="s">
+      <c r="I96" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="J96" s="56" t="s">
+      <c r="J96" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K96" s="7" t="s">
@@ -7030,14 +7027,14 @@
       <c r="AE96" s="46"/>
     </row>
     <row r="97" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A97" s="56">
+      <c r="A97" s="55">
         <f t="shared" si="4"/>
         <v>95</v>
       </c>
-      <c r="B97" s="56" t="s">
+      <c r="B97" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="C97" s="56" t="s">
+      <c r="C97" s="55" t="s">
         <v>110</v>
       </c>
       <c r="D97" s="1">
@@ -7046,19 +7043,19 @@
       <c r="E97" s="15">
         <v>2017</v>
       </c>
-      <c r="F97" s="56" t="s">
+      <c r="F97" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G97" s="56">
+      <c r="G97" s="55">
         <v>1</v>
       </c>
       <c r="H97" s="15">
         <v>0</v>
       </c>
-      <c r="I97" s="56" t="s">
+      <c r="I97" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="J97" s="56" t="s">
+      <c r="J97" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K97" s="7" t="s">
@@ -7086,14 +7083,14 @@
       <c r="AE97" s="46"/>
     </row>
     <row r="98" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A98" s="56">
+      <c r="A98" s="55">
         <f t="shared" si="4"/>
         <v>96</v>
       </c>
-      <c r="B98" s="56" t="s">
+      <c r="B98" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="C98" s="56" t="s">
+      <c r="C98" s="55" t="s">
         <v>19</v>
       </c>
       <c r="D98" s="1">
@@ -7102,19 +7099,19 @@
       <c r="E98" s="15">
         <v>2017</v>
       </c>
-      <c r="F98" s="56" t="s">
+      <c r="F98" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G98" s="56">
+      <c r="G98" s="55">
         <v>2</v>
       </c>
       <c r="H98" s="15">
         <v>0</v>
       </c>
-      <c r="I98" s="56" t="s">
+      <c r="I98" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J98" s="56" t="s">
+      <c r="J98" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K98" s="7" t="s">
@@ -7142,14 +7139,14 @@
       <c r="AE98" s="46"/>
     </row>
     <row r="99" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A99" s="56">
+      <c r="A99" s="55">
         <f t="shared" si="4"/>
         <v>97</v>
       </c>
-      <c r="B99" s="56" t="s">
+      <c r="B99" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="C99" s="56" t="s">
+      <c r="C99" s="55" t="s">
         <v>110</v>
       </c>
       <c r="D99" s="1">
@@ -7158,19 +7155,19 @@
       <c r="E99" s="15">
         <v>2017</v>
       </c>
-      <c r="F99" s="56" t="s">
+      <c r="F99" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G99" s="56">
+      <c r="G99" s="55">
         <v>1</v>
       </c>
       <c r="H99" s="15">
         <v>0</v>
       </c>
-      <c r="I99" s="56" t="s">
+      <c r="I99" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J99" s="56" t="s">
+      <c r="J99" s="55" t="s">
         <v>1</v>
       </c>
       <c r="K99" s="7" t="s">
@@ -7198,14 +7195,14 @@
       <c r="AE99" s="46"/>
     </row>
     <row r="100" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A100" s="55">
+      <c r="A100" s="54">
         <f t="shared" si="4"/>
         <v>98</v>
       </c>
-      <c r="B100" s="55" t="s">
+      <c r="B100" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="C100" s="55" t="s">
+      <c r="C100" s="54" t="s">
         <v>47</v>
       </c>
       <c r="D100" s="18">
@@ -7214,19 +7211,19 @@
       <c r="E100" s="20">
         <v>2017</v>
       </c>
-      <c r="F100" s="55" t="s">
+      <c r="F100" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="G100" s="55">
+      <c r="G100" s="54">
         <v>2</v>
       </c>
       <c r="H100" s="20">
         <v>2</v>
       </c>
-      <c r="I100" s="55" t="s">
+      <c r="I100" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="J100" s="55" t="s">
+      <c r="J100" s="54" t="s">
         <v>1</v>
       </c>
       <c r="K100" s="11" t="s">
@@ -7254,14 +7251,14 @@
       <c r="AE100" s="46"/>
     </row>
     <row r="101" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A101" s="56">
+      <c r="A101" s="55">
         <f t="shared" si="4"/>
         <v>99</v>
       </c>
-      <c r="B101" s="56" t="s">
+      <c r="B101" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C101" s="56" t="s">
+      <c r="C101" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D101" s="1">
@@ -7270,22 +7267,22 @@
       <c r="E101" s="15">
         <v>2017</v>
       </c>
-      <c r="F101" s="56" t="s">
+      <c r="F101" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G101" s="56">
+      <c r="G101" s="55">
         <v>3</v>
       </c>
       <c r="H101" s="15">
         <v>1</v>
       </c>
-      <c r="I101" s="56" t="s">
+      <c r="I101" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J101" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="K101" s="56" t="s">
+      <c r="J101" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="K101" s="55" t="s">
         <v>0</v>
       </c>
       <c r="L101" s="46"/>
@@ -7305,14 +7302,14 @@
       <c r="Z101" s="46"/>
     </row>
     <row r="102" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A102" s="56">
+      <c r="A102" s="55">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="B102" s="56" t="s">
+      <c r="B102" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="C102" s="56" t="s">
+      <c r="C102" s="55" t="s">
         <v>50</v>
       </c>
       <c r="D102" s="1">
@@ -7321,22 +7318,22 @@
       <c r="E102" s="15">
         <v>2017</v>
       </c>
-      <c r="F102" s="56" t="s">
+      <c r="F102" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="G102" s="56">
+      <c r="G102" s="55">
         <v>0</v>
       </c>
       <c r="H102" s="15">
         <v>2</v>
       </c>
-      <c r="I102" s="56" t="s">
+      <c r="I102" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J102" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="K102" s="56" t="s">
+      <c r="J102" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="K102" s="55" t="s">
         <v>0</v>
       </c>
       <c r="L102" s="46"/>
@@ -7356,7 +7353,7 @@
       <c r="Z102" s="46"/>
     </row>
     <row r="103" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A103" s="55">
+      <c r="A103" s="54">
         <f t="shared" si="4"/>
         <v>101</v>
       </c>
@@ -7407,14 +7404,14 @@
       <c r="Z103" s="46"/>
     </row>
     <row r="104" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A104" s="55">
+      <c r="A104" s="54">
         <f t="shared" si="4"/>
         <v>102</v>
       </c>
-      <c r="B104" s="55" t="s">
+      <c r="B104" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="C104" s="55" t="s">
+      <c r="C104" s="54" t="s">
         <v>31</v>
       </c>
       <c r="D104" s="18">
@@ -7423,22 +7420,22 @@
       <c r="E104" s="20">
         <v>2017</v>
       </c>
-      <c r="F104" s="55" t="s">
+      <c r="F104" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G104" s="55">
+      <c r="G104" s="54">
         <v>1</v>
       </c>
       <c r="H104" s="20">
         <v>0</v>
       </c>
-      <c r="I104" s="55" t="s">
+      <c r="I104" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="J104" s="55" t="s">
+      <c r="J104" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="K104" s="55" t="s">
+      <c r="K104" s="54" t="s">
         <v>0</v>
       </c>
       <c r="L104" s="46"/>
@@ -7458,14 +7455,14 @@
       <c r="Z104" s="46"/>
     </row>
     <row r="105" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A105" s="56">
+      <c r="A105" s="55">
         <f t="shared" si="4"/>
         <v>103</v>
       </c>
-      <c r="B105" s="56" t="s">
+      <c r="B105" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="C105" s="56" t="s">
+      <c r="C105" s="55" t="s">
         <v>33</v>
       </c>
       <c r="D105" s="1">
@@ -7474,22 +7471,22 @@
       <c r="E105" s="15">
         <v>2017</v>
       </c>
-      <c r="F105" s="56" t="s">
+      <c r="F105" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G105" s="56">
+      <c r="G105" s="55">
         <v>2</v>
       </c>
       <c r="H105" s="15">
         <v>1</v>
       </c>
-      <c r="I105" s="56" t="s">
+      <c r="I105" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J105" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="K105" s="56" t="s">
+      <c r="J105" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="K105" s="55" t="s">
         <v>0</v>
       </c>
       <c r="L105" s="46"/>
@@ -7509,14 +7506,14 @@
       <c r="Z105" s="46"/>
     </row>
     <row r="106" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A106" s="55">
+      <c r="A106" s="54">
         <f t="shared" si="4"/>
         <v>104</v>
       </c>
-      <c r="B106" s="55" t="s">
+      <c r="B106" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="C106" s="55" t="s">
+      <c r="C106" s="54" t="s">
         <v>17</v>
       </c>
       <c r="D106" s="18">
@@ -7525,22 +7522,22 @@
       <c r="E106" s="20">
         <v>2017</v>
       </c>
-      <c r="F106" s="55" t="s">
+      <c r="F106" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G106" s="55">
+      <c r="G106" s="54">
         <v>3</v>
       </c>
       <c r="H106" s="20">
         <v>0</v>
       </c>
-      <c r="I106" s="55" t="s">
+      <c r="I106" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="J106" s="55" t="s">
-        <v>1</v>
-      </c>
-      <c r="K106" s="55" t="s">
+      <c r="J106" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="K106" s="54" t="s">
         <v>49</v>
       </c>
       <c r="L106" s="46"/>
@@ -7560,14 +7557,14 @@
       <c r="Z106" s="46"/>
     </row>
     <row r="107" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A107" s="56">
+      <c r="A107" s="55">
         <f t="shared" si="4"/>
         <v>105</v>
       </c>
-      <c r="B107" s="56" t="s">
+      <c r="B107" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="C107" s="56" t="s">
+      <c r="C107" s="55" t="s">
         <v>112</v>
       </c>
       <c r="D107" s="1">
@@ -7576,22 +7573,22 @@
       <c r="E107" s="15">
         <v>2017</v>
       </c>
-      <c r="F107" s="56" t="s">
+      <c r="F107" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="G107" s="56">
+      <c r="G107" s="55">
         <v>3</v>
       </c>
       <c r="H107" s="15">
         <v>4</v>
       </c>
-      <c r="I107" s="56" t="s">
+      <c r="I107" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J107" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="K107" s="56" t="s">
+      <c r="J107" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="K107" s="55" t="s">
         <v>0</v>
       </c>
       <c r="L107" s="46"/>
@@ -7611,14 +7608,14 @@
       <c r="Z107" s="46"/>
     </row>
     <row r="108" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A108" s="55">
+      <c r="A108" s="54">
         <f t="shared" si="4"/>
         <v>106</v>
       </c>
-      <c r="B108" s="55" t="s">
+      <c r="B108" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="C108" s="55" t="s">
+      <c r="C108" s="54" t="s">
         <v>105</v>
       </c>
       <c r="D108" s="18">
@@ -7627,22 +7624,22 @@
       <c r="E108" s="20">
         <v>2017</v>
       </c>
-      <c r="F108" s="55" t="s">
+      <c r="F108" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="G108" s="55">
+      <c r="G108" s="54">
         <v>1</v>
       </c>
       <c r="H108" s="20">
         <v>2</v>
       </c>
-      <c r="I108" s="55" t="s">
+      <c r="I108" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="J108" s="55" t="s">
-        <v>1</v>
-      </c>
-      <c r="K108" s="55" t="s">
+      <c r="J108" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="K108" s="54" t="s">
         <v>49</v>
       </c>
       <c r="L108" s="46"/>
@@ -7662,14 +7659,14 @@
       <c r="Z108" s="46"/>
     </row>
     <row r="109" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A109" s="56">
+      <c r="A109" s="55">
         <f t="shared" si="4"/>
         <v>107</v>
       </c>
-      <c r="B109" s="56" t="s">
+      <c r="B109" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="C109" s="56" t="s">
+      <c r="C109" s="55" t="s">
         <v>19</v>
       </c>
       <c r="D109" s="1">
@@ -7678,22 +7675,22 @@
       <c r="E109" s="15">
         <v>2017</v>
       </c>
-      <c r="F109" s="56" t="s">
+      <c r="F109" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G109" s="56">
+      <c r="G109" s="55">
         <v>2</v>
       </c>
       <c r="H109" s="15">
         <v>0</v>
       </c>
-      <c r="I109" s="56" t="s">
+      <c r="I109" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="J109" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="K109" s="56" t="s">
+      <c r="J109" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="K109" s="55" t="s">
         <v>0</v>
       </c>
       <c r="L109" s="46"/>
@@ -7713,14 +7710,14 @@
       <c r="Z109" s="46"/>
     </row>
     <row r="110" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A110" s="56">
-        <f t="shared" ref="A110:A121" si="5">SUM(A109+1)</f>
+      <c r="A110" s="55">
+        <f t="shared" ref="A110:A122" si="5">SUM(A109+1)</f>
         <v>108</v>
       </c>
-      <c r="B110" s="56" t="s">
+      <c r="B110" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="C110" s="56" t="s">
+      <c r="C110" s="55" t="s">
         <v>31</v>
       </c>
       <c r="D110" s="1">
@@ -7729,22 +7726,22 @@
       <c r="E110" s="15">
         <v>2017</v>
       </c>
-      <c r="F110" s="56" t="s">
+      <c r="F110" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G110" s="56">
+      <c r="G110" s="55">
         <v>1</v>
       </c>
       <c r="H110" s="15">
         <v>0</v>
       </c>
-      <c r="I110" s="56" t="s">
+      <c r="I110" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J110" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="K110" s="56" t="s">
+      <c r="J110" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="K110" s="55" t="s">
         <v>0</v>
       </c>
       <c r="L110" s="46"/>
@@ -7764,14 +7761,14 @@
       <c r="Z110" s="46"/>
     </row>
     <row r="111" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A111" s="56">
+      <c r="A111" s="55">
         <f t="shared" si="5"/>
         <v>109</v>
       </c>
-      <c r="B111" s="56" t="s">
+      <c r="B111" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C111" s="56" t="s">
+      <c r="C111" s="55" t="s">
         <v>10</v>
       </c>
       <c r="D111" s="1">
@@ -7780,22 +7777,22 @@
       <c r="E111" s="15">
         <v>2017</v>
       </c>
-      <c r="F111" s="56" t="s">
+      <c r="F111" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="G111" s="56">
+      <c r="G111" s="55">
         <v>0</v>
       </c>
       <c r="H111" s="15">
         <v>0</v>
       </c>
-      <c r="I111" s="56" t="s">
+      <c r="I111" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="J111" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="K111" s="56" t="s">
+      <c r="J111" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="K111" s="55" t="s">
         <v>0</v>
       </c>
       <c r="L111" s="46"/>
@@ -7815,14 +7812,14 @@
       <c r="Z111" s="46"/>
     </row>
     <row r="112" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A112" s="55">
+      <c r="A112" s="54">
         <f t="shared" si="5"/>
         <v>110</v>
       </c>
-      <c r="B112" s="55" t="s">
+      <c r="B112" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="C112" s="55" t="s">
+      <c r="C112" s="54" t="s">
         <v>13</v>
       </c>
       <c r="D112" s="18">
@@ -7831,22 +7828,22 @@
       <c r="E112" s="20">
         <v>2017</v>
       </c>
-      <c r="F112" s="55" t="s">
+      <c r="F112" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="G112" s="55">
+      <c r="G112" s="54">
         <v>0</v>
       </c>
       <c r="H112" s="20">
         <v>1</v>
       </c>
-      <c r="I112" s="55" t="s">
+      <c r="I112" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="J112" s="55" t="s">
+      <c r="J112" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="K112" s="55" t="s">
+      <c r="K112" s="54" t="s">
         <v>0</v>
       </c>
       <c r="L112" s="46"/>
@@ -7866,14 +7863,14 @@
       <c r="Z112" s="46"/>
     </row>
     <row r="113" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A113" s="56">
+      <c r="A113" s="55">
         <f t="shared" si="5"/>
         <v>111</v>
       </c>
-      <c r="B113" s="56" t="s">
+      <c r="B113" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C113" s="56" t="s">
+      <c r="C113" s="55" t="s">
         <v>19</v>
       </c>
       <c r="D113" s="1">
@@ -7882,22 +7879,22 @@
       <c r="E113" s="15">
         <v>2017</v>
       </c>
-      <c r="F113" s="56" t="s">
+      <c r="F113" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G113" s="56">
+      <c r="G113" s="55">
         <v>2</v>
       </c>
       <c r="H113" s="15">
         <v>0</v>
       </c>
-      <c r="I113" s="56" t="s">
+      <c r="I113" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J113" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="K113" s="56" t="s">
+      <c r="J113" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="K113" s="55" t="s">
         <v>0</v>
       </c>
       <c r="L113" s="46"/>
@@ -7917,14 +7914,14 @@
       <c r="Z113" s="46"/>
     </row>
     <row r="114" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A114" s="56">
+      <c r="A114" s="55">
         <f t="shared" si="5"/>
         <v>112</v>
       </c>
-      <c r="B114" s="56" t="s">
+      <c r="B114" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="C114" s="56" t="s">
+      <c r="C114" s="55" t="s">
         <v>10</v>
       </c>
       <c r="D114" s="1">
@@ -7933,22 +7930,22 @@
       <c r="E114" s="15">
         <v>2017</v>
       </c>
-      <c r="F114" s="56" t="s">
+      <c r="F114" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="G114" s="56">
+      <c r="G114" s="55">
         <v>0</v>
       </c>
       <c r="H114" s="15">
         <v>0</v>
       </c>
-      <c r="I114" s="56" t="s">
+      <c r="I114" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="J114" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="K114" s="56" t="s">
+      <c r="J114" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="K114" s="55" t="s">
         <v>0</v>
       </c>
       <c r="L114" s="46"/>
@@ -7968,14 +7965,14 @@
       <c r="Z114" s="46"/>
     </row>
     <row r="115" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A115" s="57">
+      <c r="A115" s="56">
         <f t="shared" si="5"/>
         <v>113</v>
       </c>
-      <c r="B115" s="57" t="s">
+      <c r="B115" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="C115" s="57" t="s">
+      <c r="C115" s="56" t="s">
         <v>19</v>
       </c>
       <c r="D115" s="1">
@@ -7984,22 +7981,22 @@
       <c r="E115" s="15">
         <v>2017</v>
       </c>
-      <c r="F115" s="57" t="s">
+      <c r="F115" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="G115" s="57">
+      <c r="G115" s="56">
         <v>2</v>
       </c>
       <c r="H115" s="15">
         <v>0</v>
       </c>
-      <c r="I115" s="57" t="s">
+      <c r="I115" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="J115" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="K115" s="57" t="s">
+      <c r="J115" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="K115" s="56" t="s">
         <v>49</v>
       </c>
       <c r="L115" s="46"/>
@@ -8019,38 +8016,38 @@
       <c r="Z115" s="46"/>
     </row>
     <row r="116" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A116" s="57">
+      <c r="A116" s="56">
         <f t="shared" si="5"/>
         <v>114</v>
       </c>
-      <c r="B116" s="57" t="s">
+      <c r="B116" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="C116" s="57" t="s">
+      <c r="C116" s="56" t="s">
         <v>8</v>
       </c>
       <c r="D116" s="1">
         <v>43009</v>
       </c>
-      <c r="E116" s="57">
+      <c r="E116" s="56">
         <v>2017</v>
       </c>
-      <c r="F116" s="57" t="s">
+      <c r="F116" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="G116" s="57">
+      <c r="G116" s="56">
         <v>2</v>
       </c>
-      <c r="H116" s="57">
+      <c r="H116" s="56">
         <v>3</v>
       </c>
-      <c r="I116" s="57" t="s">
+      <c r="I116" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="J116" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="K116" s="57" t="s">
+      <c r="J116" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="K116" s="56" t="s">
         <v>0</v>
       </c>
       <c r="L116" s="46"/>
@@ -8070,38 +8067,38 @@
       <c r="Z116" s="46"/>
     </row>
     <row r="117" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A117" s="57">
+      <c r="A117" s="56">
         <f t="shared" si="5"/>
         <v>115</v>
       </c>
-      <c r="B117" s="57" t="s">
+      <c r="B117" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C117" s="57" t="s">
+      <c r="C117" s="56" t="s">
         <v>107</v>
       </c>
       <c r="D117" s="1">
         <v>43019</v>
       </c>
-      <c r="E117" s="57">
+      <c r="E117" s="56">
         <v>2017</v>
       </c>
-      <c r="F117" s="57" t="s">
+      <c r="F117" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="G117" s="57">
+      <c r="G117" s="56">
         <v>2</v>
       </c>
-      <c r="H117" s="57">
-        <v>1</v>
-      </c>
-      <c r="I117" s="57" t="s">
+      <c r="H117" s="56">
+        <v>1</v>
+      </c>
+      <c r="I117" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="J117" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="K117" s="57" t="s">
+      <c r="J117" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="K117" s="56" t="s">
         <v>49</v>
       </c>
       <c r="L117" s="46"/>
@@ -8121,38 +8118,38 @@
       <c r="Z117" s="46"/>
     </row>
     <row r="118" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A118" s="57">
+      <c r="A118" s="56">
         <f t="shared" si="5"/>
         <v>116</v>
       </c>
-      <c r="B118" s="57" t="s">
+      <c r="B118" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="C118" s="57" t="s">
+      <c r="C118" s="56" t="s">
         <v>13</v>
       </c>
       <c r="D118" s="1">
         <v>43022</v>
       </c>
-      <c r="E118" s="57">
+      <c r="E118" s="56">
         <v>2017</v>
       </c>
-      <c r="F118" s="57" t="s">
+      <c r="F118" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="G118" s="57">
-        <v>0</v>
-      </c>
-      <c r="H118" s="57">
-        <v>1</v>
-      </c>
-      <c r="I118" s="57" t="s">
+      <c r="G118" s="56">
+        <v>0</v>
+      </c>
+      <c r="H118" s="56">
+        <v>1</v>
+      </c>
+      <c r="I118" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="J118" s="57" t="s">
+      <c r="J118" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="K118" s="57" t="s">
+      <c r="K118" s="56" t="s">
         <v>0</v>
       </c>
       <c r="L118" s="46"/>
@@ -8172,38 +8169,38 @@
       <c r="Z118" s="46"/>
     </row>
     <row r="119" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A119" s="57">
+      <c r="A119" s="56">
         <f t="shared" si="5"/>
         <v>117</v>
       </c>
-      <c r="B119" s="57" t="s">
+      <c r="B119" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="C119" s="57" t="s">
+      <c r="C119" s="56" t="s">
         <v>33</v>
       </c>
       <c r="D119" s="1">
         <v>43031</v>
       </c>
-      <c r="E119" s="57">
+      <c r="E119" s="56">
         <v>2017</v>
       </c>
-      <c r="F119" s="57" t="s">
+      <c r="F119" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="G119" s="57">
+      <c r="G119" s="56">
         <v>2</v>
       </c>
-      <c r="H119" s="57">
-        <v>1</v>
-      </c>
-      <c r="I119" s="57" t="s">
+      <c r="H119" s="56">
+        <v>1</v>
+      </c>
+      <c r="I119" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="J119" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="K119" s="57" t="s">
+      <c r="J119" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="K119" s="56" t="s">
         <v>0</v>
       </c>
       <c r="L119" s="46"/>
@@ -8223,38 +8220,38 @@
       <c r="Z119" s="46"/>
     </row>
     <row r="120" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A120" s="58">
+      <c r="A120" s="57">
         <f t="shared" si="5"/>
         <v>118</v>
       </c>
-      <c r="B120" s="58" t="s">
+      <c r="B120" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="C120" s="58" t="s">
+      <c r="C120" s="57" t="s">
         <v>25</v>
       </c>
       <c r="D120" s="1">
         <v>43043</v>
       </c>
-      <c r="E120" s="58">
+      <c r="E120" s="57">
         <v>2017</v>
       </c>
-      <c r="F120" s="58" t="s">
+      <c r="F120" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="G120" s="58">
-        <v>1</v>
-      </c>
-      <c r="H120" s="58">
+      <c r="G120" s="57">
+        <v>1</v>
+      </c>
+      <c r="H120" s="57">
         <v>2</v>
       </c>
-      <c r="I120" s="58" t="s">
+      <c r="I120" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="J120" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="K120" s="58" t="s">
+      <c r="J120" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="K120" s="57" t="s">
         <v>49</v>
       </c>
       <c r="L120" s="46"/>
@@ -8274,38 +8271,38 @@
       <c r="Z120" s="46"/>
     </row>
     <row r="121" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A121" s="59">
+      <c r="A121" s="58">
         <f t="shared" si="5"/>
         <v>119</v>
       </c>
-      <c r="B121" s="59" t="s">
+      <c r="B121" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="C121" s="59" t="s">
+      <c r="C121" s="58" t="s">
         <v>13</v>
       </c>
       <c r="D121" s="1">
         <v>43050</v>
       </c>
-      <c r="E121" s="59">
+      <c r="E121" s="58">
         <v>2017</v>
       </c>
-      <c r="F121" s="59" t="s">
+      <c r="F121" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="G121" s="59">
-        <v>0</v>
-      </c>
-      <c r="H121" s="59">
-        <v>1</v>
-      </c>
-      <c r="I121" s="59" t="s">
+      <c r="G121" s="58">
+        <v>0</v>
+      </c>
+      <c r="H121" s="58">
+        <v>1</v>
+      </c>
+      <c r="I121" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="J121" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="K121" s="59" t="s">
+      <c r="J121" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="K121" s="58" t="s">
         <v>0</v>
       </c>
       <c r="L121" s="46"/>
@@ -8325,17 +8322,40 @@
       <c r="Z121" s="46"/>
     </row>
     <row r="122" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A122" s="46"/>
-      <c r="B122" s="46"/>
-      <c r="C122" s="46"/>
-      <c r="D122" s="46"/>
-      <c r="E122" s="46"/>
-      <c r="F122" s="46"/>
-      <c r="G122" s="46"/>
-      <c r="H122" s="46"/>
-      <c r="I122" s="46"/>
-      <c r="J122" s="46"/>
-      <c r="K122" s="46"/>
+      <c r="A122" s="59">
+        <f t="shared" si="5"/>
+        <v>120</v>
+      </c>
+      <c r="B122" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="C122" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="D122" s="1">
+        <v>43055</v>
+      </c>
+      <c r="E122" s="59">
+        <v>2017</v>
+      </c>
+      <c r="F122" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="G122" s="59">
+        <v>1</v>
+      </c>
+      <c r="H122" s="59">
+        <v>2</v>
+      </c>
+      <c r="I122" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="J122" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="K122" s="59" t="s">
+        <v>49</v>
+      </c>
       <c r="L122" s="46"/>
       <c r="M122" s="46"/>
       <c r="N122" s="46"/>

</xml_diff>

<commit_message>
Botafogo x Cruzeiro 03122017
</commit_message>
<xml_diff>
--- a/Jogos do Botafogo que já fui.xlsx
+++ b/Jogos do Botafogo que já fui.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="116">
   <si>
     <t>Sim</t>
   </si>
@@ -369,6 +369,9 @@
   </si>
   <si>
     <t>Atlético Goianiense</t>
+  </si>
+  <si>
+    <t>Cruzeiro</t>
   </si>
 </sst>
 </file>
@@ -753,7 +756,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -915,6 +918,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1220,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,34 +1260,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="61"/>
-      <c r="T1" s="61"/>
-      <c r="U1" s="61"/>
-      <c r="V1" s="61"/>
-      <c r="W1" s="61"/>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="60"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="62"/>
+      <c r="X1" s="62"/>
+      <c r="Y1" s="62"/>
+      <c r="Z1" s="61"/>
       <c r="AA1" s="46"/>
       <c r="AB1" s="46"/>
       <c r="AC1" s="46"/>
@@ -1419,14 +1425,14 @@
       </c>
       <c r="O3" s="6">
         <f>COUNTIF(I3:I1007,"Série A")</f>
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="Q3" s="6">
         <f>COUNTIF(J2:J1004,"Nilton Santos")</f>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="R3" s="21">
         <v>2004</v>
@@ -1441,7 +1447,7 @@
       </c>
       <c r="U3" s="11">
         <f>COUNTIF(F3:F1007, "Empate")</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="V3" s="41">
         <f>COUNTIF(F3:F1007, "Derrota")</f>
@@ -1449,15 +1455,15 @@
       </c>
       <c r="W3" s="36">
         <f>SUM(G3:G1001)</f>
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="X3" s="42">
         <f>SUM(H3:H1001)</f>
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="Y3" s="43">
         <f>COUNTIF(K3:K1006,"Sim")</f>
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Z3" s="41">
         <f>COUNTIF(K3:K1006,"Não")</f>
@@ -2366,7 +2372,7 @@
       </c>
       <c r="S16" s="30">
         <f>COUNTIF(E3:E1060, "2017")</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="T16" s="47"/>
       <c r="U16" s="48"/>
@@ -4429,8 +4435,13 @@
       <c r="K50" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L50" s="47"/>
-      <c r="M50" s="51"/>
+      <c r="L50" s="51" t="s">
+        <v>115</v>
+      </c>
+      <c r="M50" s="60">
+        <f>COUNTIF(B5:B1002,"Cruzeiro")</f>
+        <v>1</v>
+      </c>
       <c r="N50" s="47"/>
       <c r="O50" s="47"/>
       <c r="P50" s="47"/>
@@ -7711,7 +7722,7 @@
     </row>
     <row r="110" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A110" s="55">
-        <f t="shared" ref="A110:A122" si="5">SUM(A109+1)</f>
+        <f t="shared" ref="A110:A123" si="5">SUM(A109+1)</f>
         <v>108</v>
       </c>
       <c r="B110" s="55" t="s">
@@ -8373,17 +8384,40 @@
       <c r="Z122" s="46"/>
     </row>
     <row r="123" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A123" s="46"/>
-      <c r="B123" s="46"/>
-      <c r="C123" s="46"/>
-      <c r="D123" s="46"/>
-      <c r="E123" s="46"/>
-      <c r="F123" s="46"/>
-      <c r="G123" s="46"/>
-      <c r="H123" s="46"/>
-      <c r="I123" s="46"/>
-      <c r="J123" s="46"/>
-      <c r="K123" s="46"/>
+      <c r="A123" s="60">
+        <f t="shared" si="5"/>
+        <v>121</v>
+      </c>
+      <c r="B123" s="60" t="s">
+        <v>115</v>
+      </c>
+      <c r="C123" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="D123" s="1">
+        <v>43072</v>
+      </c>
+      <c r="E123" s="60">
+        <v>2017</v>
+      </c>
+      <c r="F123" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="G123" s="60">
+        <v>2</v>
+      </c>
+      <c r="H123" s="60">
+        <v>2</v>
+      </c>
+      <c r="I123" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="J123" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="K123" s="60" t="s">
+        <v>0</v>
+      </c>
       <c r="L123" s="46"/>
       <c r="M123" s="46"/>
       <c r="N123" s="46"/>

</xml_diff>

<commit_message>
Botafogo x Madureira 03022018
</commit_message>
<xml_diff>
--- a/Jogos do Botafogo que já fui.xlsx
+++ b/Jogos do Botafogo que já fui.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="116">
   <si>
     <t>Sim</t>
   </si>
@@ -736,7 +736,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -918,13 +918,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1213,10 +1210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE126"/>
+  <dimension ref="A1:AE128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G120" sqref="G120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1249,34 +1246,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="64"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
+      <c r="S1" s="64"/>
+      <c r="T1" s="64"/>
+      <c r="U1" s="64"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="64"/>
+      <c r="X1" s="64"/>
+      <c r="Y1" s="64"/>
+      <c r="Z1" s="63"/>
       <c r="AA1" s="35"/>
       <c r="AB1" s="35"/>
       <c r="AC1" s="35"/>
@@ -1421,7 +1418,7 @@
       </c>
       <c r="Q3" s="6">
         <f>COUNTIF(J2:J1005,"Nilton Santos")</f>
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="R3" s="24">
         <v>2002</v>
@@ -1432,11 +1429,11 @@
       </c>
       <c r="T3" s="56">
         <f>COUNTIF(F3:F1008, "Vitória")</f>
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U3" s="55">
         <f>COUNTIF(F3:F1008, "Empate")</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V3" s="56">
         <f>COUNTIF(F3:F1008, "Derrota")</f>
@@ -1444,7 +1441,7 @@
       </c>
       <c r="W3" s="57">
         <f>SUM(G4:G1002)</f>
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="X3" s="58">
         <f>SUM(H4:H1002)</f>
@@ -1452,7 +1449,7 @@
       </c>
       <c r="Y3" s="59">
         <f>COUNTIF(K4:K1007,"Sim")</f>
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="Z3" s="56">
         <f>COUNTIF(K4:K1007,"Não")</f>
@@ -1510,7 +1507,7 @@
       </c>
       <c r="O4" s="7">
         <f>COUNTIF(I4:I1008,"Carioca")</f>
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="P4" s="8" t="s">
         <v>23</v>
@@ -1800,7 +1797,7 @@
       </c>
       <c r="M8" s="17">
         <f>COUNTIF(B4:B1004,"Boavista")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>78</v>
@@ -2471,7 +2468,7 @@
       </c>
       <c r="M18" s="17">
         <f>COUNTIF(B4:B1009,"Madureira")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N18" s="36"/>
       <c r="O18" s="36"/>
@@ -2482,7 +2479,7 @@
       </c>
       <c r="S18" s="49">
         <f>COUNTIF(E125:E160, "2018")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T18" s="41"/>
       <c r="U18" s="37"/>
@@ -4240,7 +4237,7 @@
       <c r="K47" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L47" s="63" t="s">
+      <c r="L47" s="61" t="s">
         <v>111</v>
       </c>
       <c r="M47" s="50">
@@ -4301,7 +4298,7 @@
       <c r="K48" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L48" s="63" t="s">
+      <c r="L48" s="61" t="s">
         <v>113</v>
       </c>
       <c r="M48" s="50">
@@ -4362,7 +4359,7 @@
       <c r="K49" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L49" s="63" t="s">
+      <c r="L49" s="61" t="s">
         <v>114</v>
       </c>
       <c r="M49" s="50">
@@ -4423,7 +4420,7 @@
       <c r="K50" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L50" s="63" t="s">
+      <c r="L50" s="61" t="s">
         <v>115</v>
       </c>
       <c r="M50" s="50">
@@ -7713,7 +7710,7 @@
     </row>
     <row r="110" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A110" s="43">
-        <f t="shared" ref="A110:A126" si="5">SUM(A109+1)</f>
+        <f t="shared" ref="A110:A128" si="5">SUM(A109+1)</f>
         <v>108</v>
       </c>
       <c r="B110" s="43" t="s">
@@ -8477,38 +8474,38 @@
       <c r="Z124" s="35"/>
     </row>
     <row r="125" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A125" s="49">
+      <c r="A125" s="62">
         <f t="shared" si="5"/>
         <v>123</v>
       </c>
-      <c r="B125" s="49" t="s">
+      <c r="B125" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="C125" s="50" t="s">
+      <c r="C125" s="62" t="s">
         <v>47</v>
       </c>
       <c r="D125" s="1">
         <v>43116</v>
       </c>
-      <c r="E125" s="49">
+      <c r="E125" s="62">
         <v>2018</v>
       </c>
-      <c r="F125" s="50" t="s">
+      <c r="F125" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="G125" s="49">
+      <c r="G125" s="62">
         <v>2</v>
       </c>
-      <c r="H125" s="49">
+      <c r="H125" s="62">
         <v>2</v>
       </c>
-      <c r="I125" s="49" t="s">
+      <c r="I125" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="J125" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="K125" s="49" t="s">
+      <c r="J125" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="K125" s="62" t="s">
         <v>0</v>
       </c>
       <c r="L125" s="35"/>
@@ -8528,38 +8525,38 @@
       <c r="Z125" s="35"/>
     </row>
     <row r="126" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A126" s="61">
+      <c r="A126" s="62">
         <f t="shared" si="5"/>
         <v>124</v>
       </c>
-      <c r="B126" s="61" t="s">
+      <c r="B126" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="C126" s="61" t="s">
+      <c r="C126" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="D126" s="62">
+      <c r="D126" s="1">
         <v>43120</v>
       </c>
-      <c r="E126" s="61">
+      <c r="E126" s="62">
         <v>2018</v>
       </c>
-      <c r="F126" s="61" t="s">
+      <c r="F126" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="G126" s="61">
-        <v>0</v>
-      </c>
-      <c r="H126" s="61">
-        <v>0</v>
-      </c>
-      <c r="I126" s="61" t="s">
+      <c r="G126" s="62">
+        <v>0</v>
+      </c>
+      <c r="H126" s="62">
+        <v>0</v>
+      </c>
+      <c r="I126" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="J126" s="61" t="s">
+      <c r="J126" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="K126" s="61" t="s">
+      <c r="K126" s="62" t="s">
         <v>0</v>
       </c>
       <c r="L126" s="35"/>
@@ -8578,6 +8575,78 @@
       <c r="Y126" s="35"/>
       <c r="Z126" s="35"/>
     </row>
+    <row r="127" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A127" s="62">
+        <f t="shared" si="5"/>
+        <v>125</v>
+      </c>
+      <c r="B127" s="62" t="s">
+        <v>37</v>
+      </c>
+      <c r="C127" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="D127" s="1">
+        <v>42763</v>
+      </c>
+      <c r="E127" s="62">
+        <v>2018</v>
+      </c>
+      <c r="F127" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="G127" s="62">
+        <v>1</v>
+      </c>
+      <c r="H127" s="62">
+        <v>0</v>
+      </c>
+      <c r="I127" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="J127" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="K127" s="62" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A128" s="62">
+        <f t="shared" si="5"/>
+        <v>126</v>
+      </c>
+      <c r="B128" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="C128" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="D128" s="1">
+        <v>43134</v>
+      </c>
+      <c r="E128" s="62">
+        <v>2018</v>
+      </c>
+      <c r="F128" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="G128" s="62">
+        <v>0</v>
+      </c>
+      <c r="H128" s="62">
+        <v>0</v>
+      </c>
+      <c r="I128" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="J128" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="K128" s="62" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="N3:O7">
     <sortCondition descending="1" ref="O3:O7"/>

</xml_diff>

<commit_message>
Botafogo x vasco 18032018
</commit_message>
<xml_diff>
--- a/Jogos do Botafogo que já fui.xlsx
+++ b/Jogos do Botafogo que já fui.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="116">
   <si>
     <t>Sim</t>
   </si>
@@ -1204,10 +1204,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE128"/>
+  <dimension ref="A1:AE129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D129" sqref="D129"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J123" sqref="J123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,7 +1363,7 @@
       </c>
       <c r="M2" s="16">
         <f>COUNTIF(B3:B1005,"Vasco")</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>38</v>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="Q2" s="6">
         <f>COUNTIF(J1:J1004,"Nilton Santos")</f>
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R2" s="24">
         <v>2002</v>
@@ -1396,19 +1396,19 @@
       </c>
       <c r="V2" s="56">
         <f>COUNTIF(F2:F1007, "Derrota")</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="W2" s="57">
         <f>SUM(G3:G1001)</f>
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="X2" s="58">
         <f>SUM(H3:H1001)</f>
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="Y2" s="59">
         <f>COUNTIF(K3:K1006,"Sim")</f>
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Z2" s="56">
         <f>COUNTIF(K3:K1006,"Não")</f>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="O3" s="7">
         <f>COUNTIF(I3:I1007,"Carioca")</f>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>23</v>
@@ -2438,7 +2438,7 @@
       </c>
       <c r="S17" s="49">
         <f>COUNTIF(E124:E159, "2018")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T17" s="41"/>
       <c r="U17" s="37"/>
@@ -7669,7 +7669,7 @@
     </row>
     <row r="109" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A109" s="43">
-        <f t="shared" ref="A109:A128" si="5">SUM(A108+1)</f>
+        <f t="shared" ref="A109:A129" si="5">SUM(A108+1)</f>
         <v>108</v>
       </c>
       <c r="B109" s="43" t="s">
@@ -8642,6 +8642,42 @@
         <v>0</v>
       </c>
     </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A129" s="62">
+        <f t="shared" si="5"/>
+        <v>128</v>
+      </c>
+      <c r="B129" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C129" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D129" s="1">
+        <v>43177</v>
+      </c>
+      <c r="E129" s="25">
+        <v>2018</v>
+      </c>
+      <c r="F129" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="G129" s="25">
+        <v>2</v>
+      </c>
+      <c r="H129" s="25">
+        <v>3</v>
+      </c>
+      <c r="I129" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="J129" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="K129" s="25" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="N3:O7">
     <sortCondition descending="1" ref="O3:O7"/>

</xml_diff>

<commit_message>
Botafogo x vasco 21032018
</commit_message>
<xml_diff>
--- a/Jogos do Botafogo que já fui.xlsx
+++ b/Jogos do Botafogo que já fui.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="116">
   <si>
     <t>Sim</t>
   </si>
@@ -420,7 +420,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -629,15 +629,6 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color theme="0"/>
       </left>
       <right/>
@@ -674,19 +665,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color theme="6"/>
@@ -697,15 +675,6 @@
       <bottom style="thin">
         <color theme="6"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -732,11 +701,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -825,7 +805,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -843,22 +823,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -888,40 +868,28 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1204,10 +1172,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE129"/>
+  <dimension ref="A1:AE130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J123" sqref="J123"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1300,22 +1268,22 @@
       <c r="T1" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="U1" s="25" t="s">
+      <c r="U1" s="54" t="s">
         <v>89</v>
       </c>
       <c r="V1" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="W1" s="25" t="s">
+      <c r="W1" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="X1" s="51" t="s">
+      <c r="X1" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="Y1" s="52" t="s">
+      <c r="Y1" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="Z1" s="53" t="s">
+      <c r="Z1" s="57" t="s">
         <v>98</v>
       </c>
       <c r="AA1" s="35"/>
@@ -1363,7 +1331,7 @@
       </c>
       <c r="M2" s="16">
         <f>COUNTIF(B3:B1005,"Vasco")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>38</v>
@@ -1377,7 +1345,7 @@
       </c>
       <c r="Q2" s="6">
         <f>COUNTIF(J1:J1004,"Nilton Santos")</f>
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R2" s="24">
         <v>2002</v>
@@ -1386,31 +1354,31 @@
         <f>COUNTIF(E2, "2002")</f>
         <v>1</v>
       </c>
-      <c r="T2" s="56">
+      <c r="T2" s="21">
         <f>COUNTIF(F2:F1007, "Vitória")</f>
-        <v>67</v>
-      </c>
-      <c r="U2" s="55">
+        <v>68</v>
+      </c>
+      <c r="U2" s="54">
         <f>COUNTIF(F2:F1007, "Empate")</f>
         <v>26</v>
       </c>
-      <c r="V2" s="56">
+      <c r="V2" s="23">
         <f>COUNTIF(F2:F1007, "Derrota")</f>
         <v>35</v>
       </c>
-      <c r="W2" s="57">
+      <c r="W2" s="15">
         <f>SUM(G3:G1001)</f>
-        <v>201</v>
-      </c>
-      <c r="X2" s="58">
+        <v>204</v>
+      </c>
+      <c r="X2" s="56">
         <f>SUM(H3:H1001)</f>
-        <v>127</v>
-      </c>
-      <c r="Y2" s="59">
+        <v>129</v>
+      </c>
+      <c r="Y2" s="58">
         <f>COUNTIF(K3:K1006,"Sim")</f>
-        <v>75</v>
-      </c>
-      <c r="Z2" s="56">
+        <v>76</v>
+      </c>
+      <c r="Z2" s="55">
         <f>COUNTIF(K3:K1006,"Não")</f>
         <v>52</v>
       </c>
@@ -1466,7 +1434,7 @@
       </c>
       <c r="O3" s="7">
         <f>COUNTIF(I3:I1007,"Carioca")</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>23</v>
@@ -1613,7 +1581,7 @@
         <f>COUNTIF(I1:I1007,"Libertadores")</f>
         <v>7</v>
       </c>
-      <c r="P5" s="60" t="s">
+      <c r="P5" s="52" t="s">
         <v>36</v>
       </c>
       <c r="Q5" s="17">
@@ -1689,7 +1657,7 @@
         <f>COUNTIF(I3:I1009,"Copa do Brasil")</f>
         <v>6</v>
       </c>
-      <c r="P6" s="60" t="s">
+      <c r="P6" s="52" t="s">
         <v>62</v>
       </c>
       <c r="Q6" s="17">
@@ -2438,7 +2406,7 @@
       </c>
       <c r="S17" s="49">
         <f>COUNTIF(E124:E159, "2018")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="T17" s="41"/>
       <c r="U17" s="37"/>
@@ -2500,7 +2468,7 @@
       <c r="P18" s="36"/>
       <c r="Q18" s="36"/>
       <c r="R18" s="36"/>
-      <c r="S18" s="54"/>
+      <c r="S18" s="51"/>
       <c r="T18" s="36"/>
       <c r="U18" s="37"/>
       <c r="V18" s="36"/>
@@ -4196,7 +4164,7 @@
       <c r="K46" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L46" s="61" t="s">
+      <c r="L46" s="53" t="s">
         <v>110</v>
       </c>
       <c r="M46" s="50">
@@ -4257,7 +4225,7 @@
       <c r="K47" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L47" s="61" t="s">
+      <c r="L47" s="53" t="s">
         <v>112</v>
       </c>
       <c r="M47" s="50">
@@ -4318,7 +4286,7 @@
       <c r="K48" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L48" s="61" t="s">
+      <c r="L48" s="53" t="s">
         <v>113</v>
       </c>
       <c r="M48" s="50">
@@ -4379,7 +4347,7 @@
       <c r="K49" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L49" s="61" t="s">
+      <c r="L49" s="53" t="s">
         <v>114</v>
       </c>
       <c r="M49" s="50">
@@ -7669,7 +7637,7 @@
     </row>
     <row r="109" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A109" s="43">
-        <f t="shared" ref="A109:A129" si="5">SUM(A108+1)</f>
+        <f t="shared" ref="A109:A130" si="5">SUM(A108+1)</f>
         <v>108</v>
       </c>
       <c r="B109" s="43" t="s">
@@ -8433,38 +8401,38 @@
       <c r="Z123" s="35"/>
     </row>
     <row r="124" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A124" s="62">
+      <c r="A124" s="54">
         <f t="shared" si="5"/>
         <v>123</v>
       </c>
-      <c r="B124" s="62" t="s">
+      <c r="B124" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="C124" s="62" t="s">
+      <c r="C124" s="54" t="s">
         <v>47</v>
       </c>
       <c r="D124" s="1">
         <v>43116</v>
       </c>
-      <c r="E124" s="62">
+      <c r="E124" s="54">
         <v>2018</v>
       </c>
-      <c r="F124" s="62" t="s">
+      <c r="F124" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="G124" s="62">
+      <c r="G124" s="54">
         <v>2</v>
       </c>
-      <c r="H124" s="62">
+      <c r="H124" s="54">
         <v>2</v>
       </c>
-      <c r="I124" s="62" t="s">
+      <c r="I124" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="J124" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="K124" s="62" t="s">
+      <c r="J124" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="K124" s="54" t="s">
         <v>0</v>
       </c>
       <c r="L124" s="35"/>
@@ -8484,38 +8452,38 @@
       <c r="Z124" s="35"/>
     </row>
     <row r="125" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A125" s="62">
+      <c r="A125" s="54">
         <f t="shared" si="5"/>
         <v>124</v>
       </c>
-      <c r="B125" s="62" t="s">
+      <c r="B125" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="C125" s="62" t="s">
+      <c r="C125" s="54" t="s">
         <v>10</v>
       </c>
       <c r="D125" s="1">
         <v>43120</v>
       </c>
-      <c r="E125" s="62">
+      <c r="E125" s="54">
         <v>2018</v>
       </c>
-      <c r="F125" s="62" t="s">
+      <c r="F125" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="G125" s="62">
-        <v>0</v>
-      </c>
-      <c r="H125" s="62">
-        <v>0</v>
-      </c>
-      <c r="I125" s="62" t="s">
+      <c r="G125" s="54">
+        <v>0</v>
+      </c>
+      <c r="H125" s="54">
+        <v>0</v>
+      </c>
+      <c r="I125" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="J125" s="62" t="s">
+      <c r="J125" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="K125" s="62" t="s">
+      <c r="K125" s="54" t="s">
         <v>0</v>
       </c>
       <c r="L125" s="35"/>
@@ -8535,146 +8503,182 @@
       <c r="Z125" s="35"/>
     </row>
     <row r="126" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A126" s="62">
+      <c r="A126" s="54">
         <f t="shared" si="5"/>
         <v>125</v>
       </c>
-      <c r="B126" s="62" t="s">
+      <c r="B126" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="C126" s="62" t="s">
+      <c r="C126" s="54" t="s">
         <v>31</v>
       </c>
       <c r="D126" s="1">
         <v>42763</v>
       </c>
-      <c r="E126" s="62">
+      <c r="E126" s="54">
         <v>2018</v>
       </c>
-      <c r="F126" s="62" t="s">
+      <c r="F126" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G126" s="62">
-        <v>1</v>
-      </c>
-      <c r="H126" s="62">
-        <v>0</v>
-      </c>
-      <c r="I126" s="62" t="s">
+      <c r="G126" s="54">
+        <v>1</v>
+      </c>
+      <c r="H126" s="54">
+        <v>0</v>
+      </c>
+      <c r="I126" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="J126" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="K126" s="62" t="s">
+      <c r="J126" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="K126" s="54" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A127" s="62">
+      <c r="A127" s="54">
         <f t="shared" si="5"/>
         <v>126</v>
       </c>
-      <c r="B127" s="62" t="s">
+      <c r="B127" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C127" s="62" t="s">
+      <c r="C127" s="54" t="s">
         <v>10</v>
       </c>
       <c r="D127" s="1">
         <v>43134</v>
       </c>
-      <c r="E127" s="62">
+      <c r="E127" s="54">
         <v>2018</v>
       </c>
-      <c r="F127" s="62" t="s">
+      <c r="F127" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="G127" s="62">
-        <v>0</v>
-      </c>
-      <c r="H127" s="62">
-        <v>0</v>
-      </c>
-      <c r="I127" s="62" t="s">
+      <c r="G127" s="54">
+        <v>0</v>
+      </c>
+      <c r="H127" s="54">
+        <v>0</v>
+      </c>
+      <c r="I127" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="J127" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="K127" s="62" t="s">
+      <c r="J127" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="K127" s="54" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A128" s="62">
+      <c r="A128" s="42">
         <f t="shared" si="5"/>
         <v>127</v>
       </c>
-      <c r="B128" s="62" t="s">
+      <c r="B128" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="C128" s="62" t="s">
+      <c r="C128" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="D128" s="1">
+      <c r="D128" s="18">
         <v>43165</v>
       </c>
-      <c r="E128" s="62">
+      <c r="E128" s="42">
         <v>2018</v>
       </c>
-      <c r="F128" s="62" t="s">
+      <c r="F128" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="G128" s="62">
-        <v>1</v>
-      </c>
-      <c r="H128" s="62">
-        <v>0</v>
-      </c>
-      <c r="I128" s="62" t="s">
+      <c r="G128" s="42">
+        <v>1</v>
+      </c>
+      <c r="H128" s="42">
+        <v>0</v>
+      </c>
+      <c r="I128" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J128" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="K128" s="62" t="s">
+      <c r="J128" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="K128" s="42" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A129" s="62">
+      <c r="A129" s="54">
         <f t="shared" si="5"/>
         <v>128</v>
       </c>
-      <c r="B129" s="25" t="s">
+      <c r="B129" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C129" s="25" t="s">
+      <c r="C129" s="54" t="s">
         <v>8</v>
       </c>
       <c r="D129" s="1">
         <v>43177</v>
       </c>
-      <c r="E129" s="25">
+      <c r="E129" s="54">
         <v>2018</v>
       </c>
-      <c r="F129" s="25" t="s">
+      <c r="F129" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="G129" s="25">
+      <c r="G129" s="54">
         <v>2</v>
       </c>
-      <c r="H129" s="25">
+      <c r="H129" s="54">
         <v>3</v>
       </c>
-      <c r="I129" s="25" t="s">
+      <c r="I129" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="J129" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="K129" s="25" t="s">
+      <c r="J129" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="K129" s="54" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A130" s="54">
+        <f t="shared" si="5"/>
+        <v>129</v>
+      </c>
+      <c r="B130" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="C130" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="D130" s="1">
+        <v>43180</v>
+      </c>
+      <c r="E130" s="54">
+        <v>2018</v>
+      </c>
+      <c r="F130" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="G130" s="54">
+        <v>3</v>
+      </c>
+      <c r="H130" s="54">
+        <v>2</v>
+      </c>
+      <c r="I130" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="J130" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="K130" s="54" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Botafogo x fluminense 25032018
</commit_message>
<xml_diff>
--- a/Jogos do Botafogo que já fui.xlsx
+++ b/Jogos do Botafogo que já fui.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="116">
   <si>
     <t>Sim</t>
   </si>
@@ -1172,10 +1172,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE130"/>
+  <dimension ref="A1:AE131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,7 +1345,7 @@
       </c>
       <c r="Q2" s="6">
         <f>COUNTIF(J1:J1004,"Nilton Santos")</f>
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R2" s="24">
         <v>2002</v>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="V2" s="23">
         <f>COUNTIF(F2:F1007, "Derrota")</f>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="W2" s="15">
         <f>SUM(G3:G1001)</f>
@@ -1372,11 +1372,11 @@
       </c>
       <c r="X2" s="56">
         <f>SUM(H3:H1001)</f>
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="Y2" s="58">
         <f>COUNTIF(K3:K1006,"Sim")</f>
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Z2" s="55">
         <f>COUNTIF(K3:K1006,"Não")</f>
@@ -1427,14 +1427,14 @@
       </c>
       <c r="M3" s="17">
         <f>COUNTIF(B3:B1005,"Fluminense")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>24</v>
       </c>
       <c r="O3" s="7">
         <f>COUNTIF(I3:I1007,"Carioca")</f>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>23</v>
@@ -2406,7 +2406,7 @@
       </c>
       <c r="S17" s="49">
         <f>COUNTIF(E124:E159, "2018")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="T17" s="41"/>
       <c r="U17" s="37"/>
@@ -7637,7 +7637,7 @@
     </row>
     <row r="109" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A109" s="43">
-        <f t="shared" ref="A109:A130" si="5">SUM(A108+1)</f>
+        <f t="shared" ref="A109:A131" si="5">SUM(A108+1)</f>
         <v>108</v>
       </c>
       <c r="B109" s="43" t="s">
@@ -8682,6 +8682,42 @@
         <v>0</v>
       </c>
     </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A131" s="54">
+        <f t="shared" si="5"/>
+        <v>130</v>
+      </c>
+      <c r="B131" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="C131" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="D131" s="1">
+        <v>43181</v>
+      </c>
+      <c r="E131" s="54">
+        <v>2018</v>
+      </c>
+      <c r="F131" s="54" t="s">
+        <v>86</v>
+      </c>
+      <c r="G131" s="54">
+        <v>0</v>
+      </c>
+      <c r="H131" s="54">
+        <v>3</v>
+      </c>
+      <c r="I131" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="J131" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="K131" s="54" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="N3:O7">
     <sortCondition descending="1" ref="O3:O7"/>

</xml_diff>

<commit_message>
BOTAFOGO x flamento 28032018
</commit_message>
<xml_diff>
--- a/Jogos do Botafogo que já fui.xlsx
+++ b/Jogos do Botafogo que já fui.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="116">
   <si>
     <t>Sim</t>
   </si>
@@ -716,7 +716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -842,30 +842,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1172,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE131"/>
+  <dimension ref="A1:AE132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,37 +1184,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="43" t="s">
+      <c r="I1" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="43" t="s">
+      <c r="J1" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="43" t="s">
+      <c r="K1" s="46" t="s">
         <v>66</v>
       </c>
       <c r="L1" s="24" t="s">
@@ -1268,22 +1244,22 @@
       <c r="T1" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="U1" s="54" t="s">
+      <c r="U1" s="46" t="s">
         <v>89</v>
       </c>
       <c r="V1" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="W1" s="54" t="s">
+      <c r="W1" s="46" t="s">
         <v>92</v>
       </c>
       <c r="X1" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="Y1" s="54" t="s">
+      <c r="Y1" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="Z1" s="57" t="s">
+      <c r="Z1" s="49" t="s">
         <v>98</v>
       </c>
       <c r="AA1" s="35"/>
@@ -1345,7 +1321,7 @@
       </c>
       <c r="Q2" s="6">
         <f>COUNTIF(J1:J1004,"Nilton Santos")</f>
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="R2" s="24">
         <v>2002</v>
@@ -1356,9 +1332,9 @@
       </c>
       <c r="T2" s="21">
         <f>COUNTIF(F2:F1007, "Vitória")</f>
-        <v>68</v>
-      </c>
-      <c r="U2" s="54">
+        <v>69</v>
+      </c>
+      <c r="U2" s="46">
         <f>COUNTIF(F2:F1007, "Empate")</f>
         <v>26</v>
       </c>
@@ -1368,17 +1344,17 @@
       </c>
       <c r="W2" s="15">
         <f>SUM(G3:G1001)</f>
-        <v>204</v>
-      </c>
-      <c r="X2" s="56">
+        <v>205</v>
+      </c>
+      <c r="X2" s="48">
         <f>SUM(H3:H1001)</f>
         <v>132</v>
       </c>
-      <c r="Y2" s="58">
+      <c r="Y2" s="50">
         <f>COUNTIF(K3:K1006,"Sim")</f>
-        <v>77</v>
-      </c>
-      <c r="Z2" s="55">
+        <v>78</v>
+      </c>
+      <c r="Z2" s="47">
         <f>COUNTIF(K3:K1006,"Não")</f>
         <v>52</v>
       </c>
@@ -1434,14 +1410,14 @@
       </c>
       <c r="O3" s="7">
         <f>COUNTIF(I3:I1007,"Carioca")</f>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>23</v>
       </c>
       <c r="Q3" s="7">
         <f>COUNTIF(J3:J1008,"Maracanã")</f>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="R3" s="21">
         <v>2004</v>
@@ -1450,6 +1426,13 @@
         <f>COUNTIF(E3:E9, "2004")</f>
         <v>7</v>
       </c>
+      <c r="T3" s="35"/>
+      <c r="U3" s="35"/>
+      <c r="V3" s="35"/>
+      <c r="W3" s="35"/>
+      <c r="X3" s="35"/>
+      <c r="Y3" s="35"/>
+      <c r="Z3" s="35"/>
       <c r="AA3" s="35"/>
       <c r="AB3" s="35"/>
       <c r="AC3" s="35"/>
@@ -1457,7 +1440,7 @@
       <c r="AE3" s="35"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="43">
+      <c r="A4" s="46">
         <f>SUM(A3+1)</f>
         <v>3</v>
       </c>
@@ -1496,7 +1479,7 @@
       </c>
       <c r="M4" s="17">
         <f>COUNTIF(B3:B1008,"Flamengo")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N4" s="8" t="s">
         <v>2</v>
@@ -1533,14 +1516,14 @@
       <c r="AE4" s="35"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="43">
+      <c r="A5" s="46">
         <f t="shared" ref="A5:A6" si="0">SUM(A4+1)</f>
         <v>4</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="46" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="1">
@@ -1558,10 +1541,10 @@
       <c r="H5" s="15">
         <v>1</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="43" t="s">
+      <c r="J5" s="46" t="s">
         <v>62</v>
       </c>
       <c r="K5" s="7" t="s">
@@ -1577,11 +1560,11 @@
       <c r="N5" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="49">
+      <c r="O5" s="46">
         <f>COUNTIF(I1:I1007,"Libertadores")</f>
         <v>7</v>
       </c>
-      <c r="P5" s="52" t="s">
+      <c r="P5" s="44" t="s">
         <v>36</v>
       </c>
       <c r="Q5" s="17">
@@ -1609,14 +1592,14 @@
       <c r="AE5" s="35"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A6" s="43">
+      <c r="A6" s="46">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="46" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="1">
@@ -1634,10 +1617,10 @@
       <c r="H6" s="15">
         <v>1</v>
       </c>
-      <c r="I6" s="43" t="s">
+      <c r="I6" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="43" t="s">
+      <c r="J6" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K6" s="7" t="s">
@@ -1653,11 +1636,11 @@
       <c r="N6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O6" s="49">
+      <c r="O6" s="46">
         <f>COUNTIF(I3:I1009,"Copa do Brasil")</f>
         <v>6</v>
       </c>
-      <c r="P6" s="52" t="s">
+      <c r="P6" s="44" t="s">
         <v>62</v>
       </c>
       <c r="Q6" s="17">
@@ -1685,14 +1668,14 @@
       <c r="AE6" s="35"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" s="43">
+      <c r="A7" s="46">
         <f t="shared" ref="A7:A17" si="1">SUM(A6+1)</f>
         <v>6</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="46" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="1">
@@ -1710,10 +1693,10 @@
       <c r="H7" s="15">
         <v>1</v>
       </c>
-      <c r="I7" s="43" t="s">
+      <c r="I7" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="43" t="s">
+      <c r="J7" s="46" t="s">
         <v>62</v>
       </c>
       <c r="K7" s="7" t="s">
@@ -1726,6 +1709,8 @@
         <f>COUNTIF(B3:B1003,"Boavista")</f>
         <v>4</v>
       </c>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
       <c r="P7" s="5" t="s">
         <v>77</v>
       </c>
@@ -1754,14 +1739,14 @@
       <c r="AE7" s="35"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="43">
+      <c r="A8" s="46">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="46" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="1">
@@ -1779,10 +1764,10 @@
       <c r="H8" s="15">
         <v>0</v>
       </c>
-      <c r="I8" s="43" t="s">
+      <c r="I8" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="43" t="s">
+      <c r="J8" s="46" t="s">
         <v>62</v>
       </c>
       <c r="K8" s="7" t="s">
@@ -1800,7 +1785,7 @@
       <c r="P8" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="Q8" s="49">
+      <c r="Q8" s="46">
         <f>COUNTIF(J3:J1008,"Raulino de Oliveira")</f>
         <v>2</v>
       </c>
@@ -1825,14 +1810,14 @@
       <c r="AE8" s="35"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A9" s="43">
+      <c r="A9" s="46">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="46" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="1">
@@ -1850,10 +1835,10 @@
       <c r="H9" s="15">
         <v>2</v>
       </c>
-      <c r="I9" s="43" t="s">
+      <c r="I9" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="43" t="s">
+      <c r="J9" s="46" t="s">
         <v>62</v>
       </c>
       <c r="K9" s="7" t="s">
@@ -1871,7 +1856,7 @@
       <c r="P9" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="Q9" s="49">
+      <c r="Q9" s="46">
         <f>COUNTIF(J3:J1008,"Mário Helênio")</f>
         <v>1</v>
       </c>
@@ -1896,14 +1881,14 @@
       <c r="AE9" s="35"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A10" s="43">
+      <c r="A10" s="46">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="46" t="s">
         <v>104</v>
       </c>
       <c r="D10" s="1">
@@ -1921,10 +1906,10 @@
       <c r="H10" s="15">
         <v>2</v>
       </c>
-      <c r="I10" s="43" t="s">
+      <c r="I10" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="43" t="s">
+      <c r="J10" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K10" s="7" t="s">
@@ -1939,6 +1924,8 @@
       </c>
       <c r="N10" s="36"/>
       <c r="O10" s="36"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
       <c r="R10" s="23">
         <v>2011</v>
       </c>
@@ -1960,14 +1947,14 @@
       <c r="AE10" s="35"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A11" s="43">
+      <c r="A11" s="46">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="46" t="s">
         <v>61</v>
       </c>
       <c r="D11" s="1">
@@ -1985,10 +1972,10 @@
       <c r="H11" s="15">
         <v>4</v>
       </c>
-      <c r="I11" s="43" t="s">
+      <c r="I11" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="43" t="s">
+      <c r="J11" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K11" s="7" t="s">
@@ -2026,14 +2013,14 @@
       <c r="AE11" s="35"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="43">
+      <c r="A12" s="46">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="46" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="1">
@@ -2051,7 +2038,7 @@
       <c r="H12" s="15">
         <v>0</v>
       </c>
-      <c r="I12" s="43" t="s">
+      <c r="I12" s="46" t="s">
         <v>38</v>
       </c>
       <c r="J12" s="2" t="s">
@@ -2092,14 +2079,14 @@
       <c r="AE12" s="35"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="43">
+      <c r="A13" s="46">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="46" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="1">
@@ -2117,7 +2104,7 @@
       <c r="H13" s="15">
         <v>1</v>
       </c>
-      <c r="I13" s="43" t="s">
+      <c r="I13" s="46" t="s">
         <v>38</v>
       </c>
       <c r="J13" s="2" t="s">
@@ -2158,14 +2145,14 @@
       <c r="AE13" s="35"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A14" s="43">
+      <c r="A14" s="46">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="46" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="1">
@@ -2183,7 +2170,7 @@
       <c r="H14" s="15">
         <v>2</v>
       </c>
-      <c r="I14" s="43" t="s">
+      <c r="I14" s="46" t="s">
         <v>38</v>
       </c>
       <c r="J14" s="2" t="s">
@@ -2224,14 +2211,14 @@
       <c r="AE14" s="35"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A15" s="43">
+      <c r="A15" s="46">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="46" t="s">
         <v>33</v>
       </c>
       <c r="D15" s="1">
@@ -2249,10 +2236,10 @@
       <c r="H15" s="15">
         <v>1</v>
       </c>
-      <c r="I15" s="43" t="s">
+      <c r="I15" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J15" s="43" t="s">
+      <c r="J15" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K15" s="7" t="s">
@@ -2290,14 +2277,14 @@
       <c r="AE15" s="35"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="43">
+      <c r="A16" s="46">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="46" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="1">
@@ -2315,10 +2302,10 @@
       <c r="H16" s="15">
         <v>0</v>
       </c>
-      <c r="I16" s="43" t="s">
+      <c r="I16" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J16" s="43" t="s">
+      <c r="J16" s="46" t="s">
         <v>77</v>
       </c>
       <c r="K16" s="7" t="s">
@@ -2338,7 +2325,7 @@
       <c r="R16" s="34">
         <v>2017</v>
       </c>
-      <c r="S16" s="49">
+      <c r="S16" s="46">
         <f>COUNTIF(E86:E123, "2017")</f>
         <v>38</v>
       </c>
@@ -2356,14 +2343,14 @@
       <c r="AE16" s="35"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A17" s="43">
+      <c r="A17" s="46">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="46" t="s">
         <v>58</v>
       </c>
       <c r="D17" s="1">
@@ -2381,10 +2368,10 @@
       <c r="H17" s="15">
         <v>3</v>
       </c>
-      <c r="I17" s="43" t="s">
+      <c r="I17" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="43" t="s">
+      <c r="J17" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K17" s="7" t="s">
@@ -2404,9 +2391,9 @@
       <c r="R17" s="40">
         <v>2018</v>
       </c>
-      <c r="S17" s="49">
+      <c r="S17" s="46">
         <f>COUNTIF(E124:E159, "2018")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="T17" s="41"/>
       <c r="U17" s="37"/>
@@ -2422,14 +2409,14 @@
       <c r="AE17" s="35"/>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A18" s="43">
+      <c r="A18" s="46">
         <f t="shared" ref="A18:A23" si="2">SUM(A17+1)</f>
         <v>17</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="46" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="1">
@@ -2447,10 +2434,10 @@
       <c r="H18" s="15">
         <v>1</v>
       </c>
-      <c r="I18" s="43" t="s">
+      <c r="I18" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="43" t="s">
+      <c r="J18" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K18" s="7" t="s">
@@ -2468,7 +2455,7 @@
       <c r="P18" s="36"/>
       <c r="Q18" s="36"/>
       <c r="R18" s="36"/>
-      <c r="S18" s="51"/>
+      <c r="S18" s="43"/>
       <c r="T18" s="36"/>
       <c r="U18" s="37"/>
       <c r="V18" s="36"/>
@@ -2483,14 +2470,14 @@
       <c r="AE18" s="35"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A19" s="43">
+      <c r="A19" s="46">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="43" t="s">
+      <c r="C19" s="46" t="s">
         <v>29</v>
       </c>
       <c r="D19" s="1">
@@ -2508,10 +2495,10 @@
       <c r="H19" s="15">
         <v>1</v>
       </c>
-      <c r="I19" s="43" t="s">
+      <c r="I19" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J19" s="43" t="s">
+      <c r="J19" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K19" s="7" t="s">
@@ -2544,14 +2531,14 @@
       <c r="AE19" s="35"/>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A20" s="43">
+      <c r="A20" s="46">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="43" t="s">
+      <c r="C20" s="46" t="s">
         <v>47</v>
       </c>
       <c r="D20" s="1">
@@ -2569,10 +2556,10 @@
       <c r="H20" s="15">
         <v>2</v>
       </c>
-      <c r="I20" s="43" t="s">
+      <c r="I20" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J20" s="43" t="s">
+      <c r="J20" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K20" s="7" t="s">
@@ -2605,14 +2592,14 @@
       <c r="AE20" s="35"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A21" s="43">
+      <c r="A21" s="46">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="43" t="s">
+      <c r="C21" s="46" t="s">
         <v>57</v>
       </c>
       <c r="D21" s="1">
@@ -2630,10 +2617,10 @@
       <c r="H21" s="15">
         <v>3</v>
       </c>
-      <c r="I21" s="43" t="s">
+      <c r="I21" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J21" s="43" t="s">
+      <c r="J21" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K21" s="7" t="s">
@@ -2666,14 +2653,14 @@
       <c r="AE21" s="35"/>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A22" s="43">
+      <c r="A22" s="46">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="43" t="s">
+      <c r="C22" s="46" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="1">
@@ -2691,10 +2678,10 @@
       <c r="H22" s="15">
         <v>1</v>
       </c>
-      <c r="I22" s="43" t="s">
+      <c r="I22" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J22" s="43" t="s">
+      <c r="J22" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K22" s="7" t="s">
@@ -2727,14 +2714,14 @@
       <c r="AE22" s="35"/>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A23" s="43">
+      <c r="A23" s="46">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="43" t="s">
+      <c r="C23" s="46" t="s">
         <v>47</v>
       </c>
       <c r="D23" s="1">
@@ -2752,10 +2739,10 @@
       <c r="H23" s="15">
         <v>2</v>
       </c>
-      <c r="I23" s="43" t="s">
+      <c r="I23" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J23" s="43" t="s">
+      <c r="J23" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K23" s="7" t="s">
@@ -2788,14 +2775,14 @@
       <c r="AE23" s="35"/>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A24" s="43">
+      <c r="A24" s="46">
         <f t="shared" ref="A24:A38" si="3">SUM(A23+1)</f>
         <v>23</v>
       </c>
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="43" t="s">
+      <c r="C24" s="46" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="1">
@@ -2813,10 +2800,10 @@
       <c r="H24" s="15">
         <v>1</v>
       </c>
-      <c r="I24" s="43" t="s">
+      <c r="I24" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="J24" s="43" t="s">
+      <c r="J24" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K24" s="7" t="s">
@@ -2849,14 +2836,14 @@
       <c r="AE24" s="35"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A25" s="43">
+      <c r="A25" s="46">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="B25" s="43" t="s">
+      <c r="B25" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="43" t="s">
+      <c r="C25" s="46" t="s">
         <v>17</v>
       </c>
       <c r="D25" s="1">
@@ -2874,10 +2861,10 @@
       <c r="H25" s="15">
         <v>0</v>
       </c>
-      <c r="I25" s="43" t="s">
+      <c r="I25" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J25" s="43" t="s">
+      <c r="J25" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K25" s="7" t="s">
@@ -2910,14 +2897,14 @@
       <c r="AE25" s="35"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A26" s="43">
+      <c r="A26" s="46">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="43" t="s">
+      <c r="C26" s="46" t="s">
         <v>29</v>
       </c>
       <c r="D26" s="1">
@@ -2935,10 +2922,10 @@
       <c r="H26" s="15">
         <v>1</v>
       </c>
-      <c r="I26" s="43" t="s">
+      <c r="I26" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J26" s="43" t="s">
+      <c r="J26" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K26" s="7" t="s">
@@ -2971,14 +2958,14 @@
       <c r="AE26" s="35"/>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A27" s="43">
+      <c r="A27" s="46">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="43" t="s">
+      <c r="C27" s="46" t="s">
         <v>15</v>
       </c>
       <c r="D27" s="1">
@@ -2996,10 +2983,10 @@
       <c r="H27" s="15">
         <v>1</v>
       </c>
-      <c r="I27" s="43" t="s">
+      <c r="I27" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J27" s="43" t="s">
+      <c r="J27" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K27" s="7" t="s">
@@ -3032,7 +3019,7 @@
       <c r="AE27" s="35"/>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A28" s="43">
+      <c r="A28" s="46">
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
@@ -3093,14 +3080,14 @@
       <c r="AE28" s="35"/>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A29" s="43">
+      <c r="A29" s="46">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="43" t="s">
+      <c r="C29" s="46" t="s">
         <v>29</v>
       </c>
       <c r="D29" s="1">
@@ -3118,10 +3105,10 @@
       <c r="H29" s="15">
         <v>1</v>
       </c>
-      <c r="I29" s="43" t="s">
+      <c r="I29" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J29" s="43" t="s">
+      <c r="J29" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K29" s="7" t="s">
@@ -3154,14 +3141,14 @@
       <c r="AE29" s="35"/>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A30" s="43">
+      <c r="A30" s="46">
         <f t="shared" si="3"/>
         <v>29</v>
       </c>
-      <c r="B30" s="43" t="s">
+      <c r="B30" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="43" t="s">
+      <c r="C30" s="46" t="s">
         <v>19</v>
       </c>
       <c r="D30" s="1">
@@ -3179,10 +3166,10 @@
       <c r="H30" s="15">
         <v>0</v>
       </c>
-      <c r="I30" s="43" t="s">
+      <c r="I30" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="J30" s="43" t="s">
+      <c r="J30" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K30" s="7" t="s">
@@ -3215,14 +3202,14 @@
       <c r="AE30" s="35"/>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A31" s="43">
+      <c r="A31" s="46">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="B31" s="43" t="s">
+      <c r="B31" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="43" t="s">
+      <c r="C31" s="46" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="1">
@@ -3240,10 +3227,10 @@
       <c r="H31" s="15">
         <v>1</v>
       </c>
-      <c r="I31" s="43" t="s">
+      <c r="I31" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J31" s="43" t="s">
+      <c r="J31" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K31" s="7" t="s">
@@ -3276,14 +3263,14 @@
       <c r="AE31" s="35"/>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A32" s="43">
+      <c r="A32" s="46">
         <f t="shared" si="3"/>
         <v>31</v>
       </c>
-      <c r="B32" s="43" t="s">
+      <c r="B32" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="43" t="s">
+      <c r="C32" s="46" t="s">
         <v>15</v>
       </c>
       <c r="D32" s="1">
@@ -3301,10 +3288,10 @@
       <c r="H32" s="15">
         <v>1</v>
       </c>
-      <c r="I32" s="43" t="s">
+      <c r="I32" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J32" s="43" t="s">
+      <c r="J32" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K32" s="7" t="s">
@@ -3337,14 +3324,14 @@
       <c r="AE32" s="35"/>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A33" s="43">
+      <c r="A33" s="46">
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="B33" s="43" t="s">
+      <c r="B33" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="43" t="s">
+      <c r="C33" s="46" t="s">
         <v>25</v>
       </c>
       <c r="D33" s="1">
@@ -3362,10 +3349,10 @@
       <c r="H33" s="15">
         <v>2</v>
       </c>
-      <c r="I33" s="43" t="s">
+      <c r="I33" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J33" s="43" t="s">
+      <c r="J33" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K33" s="7" t="s">
@@ -3398,14 +3385,14 @@
       <c r="AE33" s="35"/>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A34" s="43">
+      <c r="A34" s="46">
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="B34" s="43" t="s">
+      <c r="B34" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="43" t="s">
+      <c r="C34" s="46" t="s">
         <v>21</v>
       </c>
       <c r="D34" s="1">
@@ -3423,10 +3410,10 @@
       <c r="H34" s="15">
         <v>1</v>
       </c>
-      <c r="I34" s="43" t="s">
+      <c r="I34" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J34" s="43" t="s">
+      <c r="J34" s="46" t="s">
         <v>36</v>
       </c>
       <c r="K34" s="7" t="s">
@@ -3459,14 +3446,14 @@
       <c r="AE34" s="35"/>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A35" s="43">
+      <c r="A35" s="46">
         <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="43" t="s">
+      <c r="C35" s="46" t="s">
         <v>17</v>
       </c>
       <c r="D35" s="1">
@@ -3484,10 +3471,10 @@
       <c r="H35" s="15">
         <v>0</v>
       </c>
-      <c r="I35" s="43" t="s">
+      <c r="I35" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J35" s="43" t="s">
+      <c r="J35" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K35" s="7" t="s">
@@ -3520,14 +3507,14 @@
       <c r="AE35" s="35"/>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A36" s="43">
+      <c r="A36" s="46">
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="B36" s="43" t="s">
+      <c r="B36" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="43" t="s">
+      <c r="C36" s="46" t="s">
         <v>31</v>
       </c>
       <c r="D36" s="1">
@@ -3545,10 +3532,10 @@
       <c r="H36" s="15">
         <v>0</v>
       </c>
-      <c r="I36" s="43" t="s">
+      <c r="I36" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J36" s="43" t="s">
+      <c r="J36" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K36" s="7" t="s">
@@ -3581,14 +3568,14 @@
       <c r="AE36" s="35"/>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A37" s="43">
+      <c r="A37" s="46">
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="B37" s="43" t="s">
+      <c r="B37" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="43" t="s">
+      <c r="C37" s="46" t="s">
         <v>51</v>
       </c>
       <c r="D37" s="1">
@@ -3606,10 +3593,10 @@
       <c r="H37" s="15">
         <v>2</v>
       </c>
-      <c r="I37" s="43" t="s">
+      <c r="I37" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J37" s="43" t="s">
+      <c r="J37" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K37" s="7" t="s">
@@ -3642,14 +3629,14 @@
       <c r="AE37" s="35"/>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A38" s="43">
+      <c r="A38" s="46">
         <f t="shared" si="3"/>
         <v>37</v>
       </c>
-      <c r="B38" s="43" t="s">
+      <c r="B38" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="43" t="s">
+      <c r="C38" s="46" t="s">
         <v>50</v>
       </c>
       <c r="D38" s="1">
@@ -3667,10 +3654,10 @@
       <c r="H38" s="15">
         <v>2</v>
       </c>
-      <c r="I38" s="43" t="s">
+      <c r="I38" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J38" s="43" t="s">
+      <c r="J38" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K38" s="7" t="s">
@@ -3703,14 +3690,14 @@
       <c r="AE38" s="35"/>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A39" s="43">
+      <c r="A39" s="46">
         <f t="shared" ref="A39:A108" si="4">SUM(A38+1)</f>
         <v>38</v>
       </c>
-      <c r="B39" s="43" t="s">
+      <c r="B39" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="43" t="s">
+      <c r="C39" s="46" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="1">
@@ -3728,10 +3715,10 @@
       <c r="H39" s="15">
         <v>0</v>
       </c>
-      <c r="I39" s="43" t="s">
+      <c r="I39" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J39" s="43" t="s">
+      <c r="J39" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K39" s="7" t="s">
@@ -3764,14 +3751,14 @@
       <c r="AE39" s="35"/>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A40" s="43">
+      <c r="A40" s="46">
         <f t="shared" si="4"/>
         <v>39</v>
       </c>
-      <c r="B40" s="43" t="s">
+      <c r="B40" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="43" t="s">
+      <c r="C40" s="46" t="s">
         <v>47</v>
       </c>
       <c r="D40" s="1">
@@ -3789,10 +3776,10 @@
       <c r="H40" s="15">
         <v>2</v>
       </c>
-      <c r="I40" s="43" t="s">
+      <c r="I40" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J40" s="43" t="s">
+      <c r="J40" s="46" t="s">
         <v>36</v>
       </c>
       <c r="K40" s="7" t="s">
@@ -3825,14 +3812,14 @@
       <c r="AE40" s="35"/>
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A41" s="43">
+      <c r="A41" s="46">
         <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="B41" s="43" t="s">
+      <c r="B41" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C41" s="43" t="s">
+      <c r="C41" s="46" t="s">
         <v>29</v>
       </c>
       <c r="D41" s="1">
@@ -3850,10 +3837,10 @@
       <c r="H41" s="15">
         <v>1</v>
       </c>
-      <c r="I41" s="43" t="s">
+      <c r="I41" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J41" s="43" t="s">
+      <c r="J41" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K41" s="7" t="s">
@@ -3886,14 +3873,14 @@
       <c r="AE41" s="35"/>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A42" s="43">
+      <c r="A42" s="46">
         <f t="shared" si="4"/>
         <v>41</v>
       </c>
-      <c r="B42" s="43" t="s">
+      <c r="B42" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="43" t="s">
+      <c r="C42" s="46" t="s">
         <v>13</v>
       </c>
       <c r="D42" s="1">
@@ -3911,10 +3898,10 @@
       <c r="H42" s="15">
         <v>1</v>
       </c>
-      <c r="I42" s="43" t="s">
+      <c r="I42" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J42" s="43" t="s">
+      <c r="J42" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K42" s="7" t="s">
@@ -3947,14 +3934,14 @@
       <c r="AE42" s="35"/>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A43" s="43">
+      <c r="A43" s="46">
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="B43" s="43" t="s">
+      <c r="B43" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C43" s="43" t="s">
+      <c r="C43" s="46" t="s">
         <v>31</v>
       </c>
       <c r="D43" s="1">
@@ -3972,7 +3959,7 @@
       <c r="H43" s="15">
         <v>0</v>
       </c>
-      <c r="I43" s="43" t="s">
+      <c r="I43" s="46" t="s">
         <v>24</v>
       </c>
       <c r="J43" s="2" t="s">
@@ -4008,14 +3995,14 @@
       <c r="AE43" s="35"/>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A44" s="43">
+      <c r="A44" s="46">
         <f t="shared" si="4"/>
         <v>43</v>
       </c>
-      <c r="B44" s="43" t="s">
+      <c r="B44" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="43" t="s">
+      <c r="C44" s="46" t="s">
         <v>13</v>
       </c>
       <c r="D44" s="1">
@@ -4033,10 +4020,10 @@
       <c r="H44" s="15">
         <v>1</v>
       </c>
-      <c r="I44" s="43" t="s">
+      <c r="I44" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J44" s="43" t="s">
+      <c r="J44" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K44" s="7" t="s">
@@ -4045,7 +4032,7 @@
       <c r="L44" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="M44" s="50">
+      <c r="M44" s="46">
         <f>COUNTIF(B3:B1013,"São Paulo")</f>
         <v>2</v>
       </c>
@@ -4069,14 +4056,14 @@
       <c r="AE44" s="35"/>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A45" s="43">
+      <c r="A45" s="46">
         <f t="shared" si="4"/>
         <v>44</v>
       </c>
-      <c r="B45" s="43" t="s">
+      <c r="B45" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="C45" s="43" t="s">
+      <c r="C45" s="46" t="s">
         <v>17</v>
       </c>
       <c r="D45" s="1">
@@ -4094,10 +4081,10 @@
       <c r="H45" s="15">
         <v>0</v>
       </c>
-      <c r="I45" s="43" t="s">
+      <c r="I45" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J45" s="43" t="s">
+      <c r="J45" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K45" s="7" t="s">
@@ -4106,7 +4093,7 @@
       <c r="L45" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="M45" s="50">
+      <c r="M45" s="46">
         <f>COUNTIF(B3:B1037,"Paraná")</f>
         <v>1</v>
       </c>
@@ -4130,14 +4117,14 @@
       <c r="AE45" s="35"/>
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A46" s="43">
+      <c r="A46" s="46">
         <f t="shared" si="4"/>
         <v>45</v>
       </c>
-      <c r="B46" s="43" t="s">
+      <c r="B46" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="43" t="s">
+      <c r="C46" s="46" t="s">
         <v>6</v>
       </c>
       <c r="D46" s="1">
@@ -4155,19 +4142,19 @@
       <c r="H46" s="15">
         <v>0</v>
       </c>
-      <c r="I46" s="43" t="s">
+      <c r="I46" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="J46" s="43" t="s">
+      <c r="J46" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K46" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L46" s="53" t="s">
+      <c r="L46" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="M46" s="50">
+      <c r="M46" s="46">
         <f>COUNTIF(B3:B1037,"Avaí")</f>
         <v>1</v>
       </c>
@@ -4191,14 +4178,14 @@
       <c r="AE46" s="35"/>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A47" s="43">
+      <c r="A47" s="46">
         <f t="shared" si="4"/>
         <v>46</v>
       </c>
-      <c r="B47" s="43" t="s">
+      <c r="B47" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="C47" s="43" t="s">
+      <c r="C47" s="46" t="s">
         <v>31</v>
       </c>
       <c r="D47" s="1">
@@ -4216,19 +4203,19 @@
       <c r="H47" s="15">
         <v>0</v>
       </c>
-      <c r="I47" s="43" t="s">
+      <c r="I47" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="J47" s="43" t="s">
+      <c r="J47" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K47" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L47" s="53" t="s">
+      <c r="L47" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="M47" s="50">
+      <c r="M47" s="46">
         <f>COUNTIF(B3:B1000,"Nacional-URU")</f>
         <v>1</v>
       </c>
@@ -4256,10 +4243,10 @@
         <f t="shared" si="4"/>
         <v>47</v>
       </c>
-      <c r="B48" s="43" t="s">
+      <c r="B48" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C48" s="43" t="s">
+      <c r="C48" s="46" t="s">
         <v>13</v>
       </c>
       <c r="D48" s="1">
@@ -4277,19 +4264,19 @@
       <c r="H48" s="15">
         <v>1</v>
       </c>
-      <c r="I48" s="43" t="s">
+      <c r="I48" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J48" s="43" t="s">
+      <c r="J48" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K48" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L48" s="53" t="s">
+      <c r="L48" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="M48" s="50">
+      <c r="M48" s="46">
         <f>COUNTIF(B4:B1001,"Atlético Goianiense")</f>
         <v>1</v>
       </c>
@@ -4313,14 +4300,14 @@
       <c r="AE48" s="35"/>
     </row>
     <row r="49" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A49" s="43">
+      <c r="A49" s="46">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="B49" s="43" t="s">
+      <c r="B49" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="C49" s="43" t="s">
+      <c r="C49" s="46" t="s">
         <v>31</v>
       </c>
       <c r="D49" s="1">
@@ -4338,19 +4325,19 @@
       <c r="H49" s="15">
         <v>0</v>
       </c>
-      <c r="I49" s="43" t="s">
+      <c r="I49" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J49" s="43" t="s">
+      <c r="J49" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K49" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L49" s="53" t="s">
+      <c r="L49" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="M49" s="50">
+      <c r="M49" s="46">
         <f>COUNTIF(B5:B1002,"Cruzeiro")</f>
         <v>1</v>
       </c>
@@ -4374,14 +4361,14 @@
       <c r="AE49" s="35"/>
     </row>
     <row r="50" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A50" s="43">
+      <c r="A50" s="46">
         <f t="shared" si="4"/>
         <v>49</v>
       </c>
-      <c r="B50" s="43" t="s">
+      <c r="B50" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C50" s="43" t="s">
+      <c r="C50" s="46" t="s">
         <v>31</v>
       </c>
       <c r="D50" s="1">
@@ -4399,15 +4386,17 @@
       <c r="H50" s="15">
         <v>0</v>
       </c>
-      <c r="I50" s="43" t="s">
+      <c r="I50" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J50" s="43" t="s">
+      <c r="J50" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K50" s="7" t="s">
         <v>0</v>
       </c>
+      <c r="L50" s="35"/>
+      <c r="M50" s="35"/>
       <c r="N50" s="36"/>
       <c r="O50" s="36"/>
       <c r="P50" s="36"/>
@@ -4428,7 +4417,7 @@
       <c r="AE50" s="35"/>
     </row>
     <row r="51" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A51" s="43">
+      <c r="A51" s="46">
         <f t="shared" si="4"/>
         <v>50</v>
       </c>
@@ -4484,14 +4473,14 @@
       <c r="AE51" s="35"/>
     </row>
     <row r="52" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A52" s="43">
+      <c r="A52" s="46">
         <f t="shared" si="4"/>
         <v>51</v>
       </c>
-      <c r="B52" s="43" t="s">
+      <c r="B52" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="C52" s="43" t="s">
+      <c r="C52" s="46" t="s">
         <v>13</v>
       </c>
       <c r="D52" s="1">
@@ -4509,10 +4498,10 @@
       <c r="H52" s="15">
         <v>1</v>
       </c>
-      <c r="I52" s="43" t="s">
+      <c r="I52" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J52" s="43" t="s">
+      <c r="J52" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K52" s="7" t="s">
@@ -4540,14 +4529,14 @@
       <c r="AE52" s="35"/>
     </row>
     <row r="53" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A53" s="43">
+      <c r="A53" s="46">
         <f t="shared" si="4"/>
         <v>52</v>
       </c>
-      <c r="B53" s="43" t="s">
+      <c r="B53" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="C53" s="43" t="s">
+      <c r="C53" s="46" t="s">
         <v>31</v>
       </c>
       <c r="D53" s="1">
@@ -4565,10 +4554,10 @@
       <c r="H53" s="15">
         <v>0</v>
       </c>
-      <c r="I53" s="43" t="s">
+      <c r="I53" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J53" s="43" t="s">
+      <c r="J53" s="46" t="s">
         <v>36</v>
       </c>
       <c r="K53" s="7" t="s">
@@ -4596,14 +4585,14 @@
       <c r="AE53" s="35"/>
     </row>
     <row r="54" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A54" s="43">
+      <c r="A54" s="46">
         <f t="shared" si="4"/>
         <v>53</v>
       </c>
-      <c r="B54" s="43" t="s">
+      <c r="B54" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="C54" s="43" t="s">
+      <c r="C54" s="46" t="s">
         <v>6</v>
       </c>
       <c r="D54" s="1">
@@ -4621,10 +4610,10 @@
       <c r="H54" s="15">
         <v>0</v>
       </c>
-      <c r="I54" s="43" t="s">
+      <c r="I54" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J54" s="43" t="s">
+      <c r="J54" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K54" s="7" t="s">
@@ -4652,14 +4641,14 @@
       <c r="AE54" s="35"/>
     </row>
     <row r="55" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A55" s="43">
+      <c r="A55" s="46">
         <f t="shared" si="4"/>
         <v>54</v>
       </c>
-      <c r="B55" s="43" t="s">
+      <c r="B55" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C55" s="43" t="s">
+      <c r="C55" s="46" t="s">
         <v>33</v>
       </c>
       <c r="D55" s="1">
@@ -4677,10 +4666,10 @@
       <c r="H55" s="15">
         <v>1</v>
       </c>
-      <c r="I55" s="43" t="s">
+      <c r="I55" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J55" s="43" t="s">
+      <c r="J55" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K55" s="7" t="s">
@@ -4708,14 +4697,14 @@
       <c r="AE55" s="35"/>
     </row>
     <row r="56" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A56" s="43">
+      <c r="A56" s="46">
         <f t="shared" si="4"/>
         <v>55</v>
       </c>
-      <c r="B56" s="43" t="s">
+      <c r="B56" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C56" s="43" t="s">
+      <c r="C56" s="46" t="s">
         <v>31</v>
       </c>
       <c r="D56" s="1">
@@ -4733,10 +4722,10 @@
       <c r="H56" s="15">
         <v>0</v>
       </c>
-      <c r="I56" s="43" t="s">
+      <c r="I56" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J56" s="43" t="s">
+      <c r="J56" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K56" s="7" t="s">
@@ -4764,14 +4753,14 @@
       <c r="AE56" s="35"/>
     </row>
     <row r="57" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A57" s="43">
+      <c r="A57" s="46">
         <f t="shared" si="4"/>
         <v>56</v>
       </c>
-      <c r="B57" s="43" t="s">
+      <c r="B57" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C57" s="43" t="s">
+      <c r="C57" s="46" t="s">
         <v>75</v>
       </c>
       <c r="D57" s="1">
@@ -4789,10 +4778,10 @@
       <c r="H57" s="15">
         <v>3</v>
       </c>
-      <c r="I57" s="43" t="s">
+      <c r="I57" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J57" s="43" t="s">
+      <c r="J57" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K57" s="7" t="s">
@@ -4820,14 +4809,14 @@
       <c r="AE57" s="35"/>
     </row>
     <row r="58" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A58" s="43">
+      <c r="A58" s="46">
         <f t="shared" si="4"/>
         <v>57</v>
       </c>
-      <c r="B58" s="43" t="s">
+      <c r="B58" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C58" s="43" t="s">
+      <c r="C58" s="46" t="s">
         <v>17</v>
       </c>
       <c r="D58" s="1">
@@ -4845,10 +4834,10 @@
       <c r="H58" s="15">
         <v>0</v>
       </c>
-      <c r="I58" s="43" t="s">
+      <c r="I58" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J58" s="43" t="s">
+      <c r="J58" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K58" s="7" t="s">
@@ -4876,14 +4865,14 @@
       <c r="AE58" s="35"/>
     </row>
     <row r="59" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A59" s="43">
+      <c r="A59" s="46">
         <f t="shared" si="4"/>
         <v>58</v>
       </c>
-      <c r="B59" s="43" t="s">
+      <c r="B59" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C59" s="43" t="s">
+      <c r="C59" s="46" t="s">
         <v>15</v>
       </c>
       <c r="D59" s="1">
@@ -4901,10 +4890,10 @@
       <c r="H59" s="15">
         <v>1</v>
       </c>
-      <c r="I59" s="43" t="s">
+      <c r="I59" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J59" s="43" t="s">
+      <c r="J59" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K59" s="7" t="s">
@@ -4932,14 +4921,14 @@
       <c r="AE59" s="35"/>
     </row>
     <row r="60" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A60" s="43">
+      <c r="A60" s="46">
         <f t="shared" si="4"/>
         <v>59</v>
       </c>
-      <c r="B60" s="43" t="s">
+      <c r="B60" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C60" s="43" t="s">
+      <c r="C60" s="46" t="s">
         <v>21</v>
       </c>
       <c r="D60" s="1">
@@ -4957,10 +4946,10 @@
       <c r="H60" s="15">
         <v>1</v>
       </c>
-      <c r="I60" s="43" t="s">
+      <c r="I60" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J60" s="43" t="s">
+      <c r="J60" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K60" s="7" t="s">
@@ -4988,14 +4977,14 @@
       <c r="AE60" s="35"/>
     </row>
     <row r="61" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A61" s="43">
+      <c r="A61" s="46">
         <f t="shared" si="4"/>
         <v>60</v>
       </c>
-      <c r="B61" s="43" t="s">
+      <c r="B61" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C61" s="43" t="s">
+      <c r="C61" s="46" t="s">
         <v>25</v>
       </c>
       <c r="D61" s="1">
@@ -5013,10 +5002,10 @@
       <c r="H61" s="15">
         <v>2</v>
       </c>
-      <c r="I61" s="43" t="s">
+      <c r="I61" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J61" s="43" t="s">
+      <c r="J61" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K61" s="7" t="s">
@@ -5044,14 +5033,14 @@
       <c r="AE61" s="35"/>
     </row>
     <row r="62" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A62" s="43">
+      <c r="A62" s="46">
         <f t="shared" si="4"/>
         <v>61</v>
       </c>
-      <c r="B62" s="43" t="s">
+      <c r="B62" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="C62" s="43" t="s">
+      <c r="C62" s="46" t="s">
         <v>21</v>
       </c>
       <c r="D62" s="1">
@@ -5069,10 +5058,10 @@
       <c r="H62" s="15">
         <v>1</v>
       </c>
-      <c r="I62" s="43" t="s">
+      <c r="I62" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="J62" s="43" t="s">
+      <c r="J62" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K62" s="7" t="s">
@@ -5100,14 +5089,14 @@
       <c r="AE62" s="35"/>
     </row>
     <row r="63" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A63" s="43">
+      <c r="A63" s="46">
         <f t="shared" si="4"/>
         <v>62</v>
       </c>
-      <c r="B63" s="43" t="s">
+      <c r="B63" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C63" s="43" t="s">
+      <c r="C63" s="46" t="s">
         <v>19</v>
       </c>
       <c r="D63" s="1">
@@ -5125,10 +5114,10 @@
       <c r="H63" s="15">
         <v>0</v>
       </c>
-      <c r="I63" s="43" t="s">
+      <c r="I63" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="J63" s="43" t="s">
+      <c r="J63" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K63" s="7" t="s">
@@ -5156,14 +5145,14 @@
       <c r="AE63" s="35"/>
     </row>
     <row r="64" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A64" s="43">
+      <c r="A64" s="46">
         <f t="shared" si="4"/>
         <v>63</v>
       </c>
-      <c r="B64" s="43" t="s">
+      <c r="B64" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C64" s="43" t="s">
+      <c r="C64" s="46" t="s">
         <v>17</v>
       </c>
       <c r="D64" s="1">
@@ -5181,10 +5170,10 @@
       <c r="H64" s="15">
         <v>0</v>
       </c>
-      <c r="I64" s="43" t="s">
+      <c r="I64" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="J64" s="43" t="s">
+      <c r="J64" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K64" s="7" t="s">
@@ -5212,14 +5201,14 @@
       <c r="AE64" s="35"/>
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A65" s="43">
+      <c r="A65" s="46">
         <f t="shared" si="4"/>
         <v>64</v>
       </c>
-      <c r="B65" s="43" t="s">
+      <c r="B65" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C65" s="43" t="s">
+      <c r="C65" s="46" t="s">
         <v>15</v>
       </c>
       <c r="D65" s="1">
@@ -5237,10 +5226,10 @@
       <c r="H65" s="15">
         <v>1</v>
       </c>
-      <c r="I65" s="43" t="s">
+      <c r="I65" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="J65" s="43" t="s">
+      <c r="J65" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K65" s="7" t="s">
@@ -5268,14 +5257,14 @@
       <c r="AE65" s="35"/>
     </row>
     <row r="66" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A66" s="43">
+      <c r="A66" s="46">
         <f t="shared" si="4"/>
         <v>65</v>
       </c>
-      <c r="B66" s="43" t="s">
+      <c r="B66" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C66" s="43" t="s">
+      <c r="C66" s="46" t="s">
         <v>13</v>
       </c>
       <c r="D66" s="1">
@@ -5293,10 +5282,10 @@
       <c r="H66" s="15">
         <v>1</v>
       </c>
-      <c r="I66" s="43" t="s">
+      <c r="I66" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="J66" s="43" t="s">
+      <c r="J66" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K66" s="7" t="s">
@@ -5324,14 +5313,14 @@
       <c r="AE66" s="35"/>
     </row>
     <row r="67" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A67" s="43">
+      <c r="A67" s="46">
         <f t="shared" si="4"/>
         <v>66</v>
       </c>
-      <c r="B67" s="43" t="s">
+      <c r="B67" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="C67" s="43" t="s">
+      <c r="C67" s="46" t="s">
         <v>10</v>
       </c>
       <c r="D67" s="1">
@@ -5349,10 +5338,10 @@
       <c r="H67" s="15">
         <v>0</v>
       </c>
-      <c r="I67" s="43" t="s">
+      <c r="I67" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="J67" s="43" t="s">
+      <c r="J67" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K67" s="7" t="s">
@@ -5380,14 +5369,14 @@
       <c r="AE67" s="35"/>
     </row>
     <row r="68" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A68" s="43">
+      <c r="A68" s="46">
         <f t="shared" si="4"/>
         <v>67</v>
       </c>
-      <c r="B68" s="43" t="s">
+      <c r="B68" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C68" s="43" t="s">
+      <c r="C68" s="46" t="s">
         <v>8</v>
       </c>
       <c r="D68" s="1">
@@ -5405,10 +5394,10 @@
       <c r="H68" s="15">
         <v>3</v>
       </c>
-      <c r="I68" s="43" t="s">
+      <c r="I68" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="J68" s="43" t="s">
+      <c r="J68" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K68" s="7" t="s">
@@ -5436,14 +5425,14 @@
       <c r="AE68" s="35"/>
     </row>
     <row r="69" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A69" s="43">
+      <c r="A69" s="46">
         <f t="shared" si="4"/>
         <v>68</v>
       </c>
-      <c r="B69" s="43" t="s">
+      <c r="B69" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="43" t="s">
+      <c r="C69" s="46" t="s">
         <v>6</v>
       </c>
       <c r="D69" s="1">
@@ -5461,10 +5450,10 @@
       <c r="H69" s="15">
         <v>0</v>
       </c>
-      <c r="I69" s="43" t="s">
+      <c r="I69" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="J69" s="43" t="s">
+      <c r="J69" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K69" s="7" t="s">
@@ -5492,14 +5481,14 @@
       <c r="AE69" s="35"/>
     </row>
     <row r="70" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A70" s="43">
+      <c r="A70" s="46">
         <f t="shared" si="4"/>
         <v>69</v>
       </c>
-      <c r="B70" s="43" t="s">
+      <c r="B70" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="43" t="s">
+      <c r="C70" s="46" t="s">
         <v>4</v>
       </c>
       <c r="D70" s="1">
@@ -5517,10 +5506,10 @@
       <c r="H70" s="15">
         <v>3</v>
       </c>
-      <c r="I70" s="43" t="s">
+      <c r="I70" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="J70" s="43" t="s">
+      <c r="J70" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K70" s="7" t="s">
@@ -5548,14 +5537,14 @@
       <c r="AE70" s="35"/>
     </row>
     <row r="71" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A71" s="43">
+      <c r="A71" s="46">
         <f t="shared" si="4"/>
         <v>70</v>
       </c>
-      <c r="B71" s="43" t="s">
+      <c r="B71" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C71" s="43" t="s">
+      <c r="C71" s="46" t="s">
         <v>10</v>
       </c>
       <c r="D71" s="1">
@@ -5573,10 +5562,10 @@
       <c r="H71" s="15">
         <v>0</v>
       </c>
-      <c r="I71" s="43" t="s">
+      <c r="I71" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="J71" s="43" t="s">
+      <c r="J71" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K71" s="7" t="s">
@@ -5604,14 +5593,14 @@
       <c r="AE71" s="35"/>
     </row>
     <row r="72" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A72" s="43">
+      <c r="A72" s="46">
         <f t="shared" si="4"/>
         <v>71</v>
       </c>
-      <c r="B72" s="43" t="s">
+      <c r="B72" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="C72" s="43" t="s">
+      <c r="C72" s="46" t="s">
         <v>33</v>
       </c>
       <c r="D72" s="1">
@@ -5629,10 +5618,10 @@
       <c r="H72" s="15">
         <v>1</v>
       </c>
-      <c r="I72" s="43" t="s">
+      <c r="I72" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J72" s="43" t="s">
+      <c r="J72" s="46" t="s">
         <v>36</v>
       </c>
       <c r="K72" s="7" t="s">
@@ -5660,14 +5649,14 @@
       <c r="AE72" s="35"/>
     </row>
     <row r="73" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A73" s="43">
+      <c r="A73" s="46">
         <f t="shared" si="4"/>
         <v>72</v>
       </c>
-      <c r="B73" s="43" t="s">
+      <c r="B73" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="C73" s="43" t="s">
+      <c r="C73" s="46" t="s">
         <v>31</v>
       </c>
       <c r="D73" s="1">
@@ -5685,10 +5674,10 @@
       <c r="H73" s="15">
         <v>0</v>
       </c>
-      <c r="I73" s="43" t="s">
+      <c r="I73" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J73" s="43" t="s">
+      <c r="J73" s="46" t="s">
         <v>36</v>
       </c>
       <c r="K73" s="7" t="s">
@@ -5716,14 +5705,14 @@
       <c r="AE73" s="35"/>
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A74" s="43">
+      <c r="A74" s="46">
         <f t="shared" si="4"/>
         <v>73</v>
       </c>
-      <c r="B74" s="43" t="s">
+      <c r="B74" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C74" s="43" t="s">
+      <c r="C74" s="46" t="s">
         <v>13</v>
       </c>
       <c r="D74" s="1">
@@ -5741,10 +5730,10 @@
       <c r="H74" s="15">
         <v>1</v>
       </c>
-      <c r="I74" s="43" t="s">
+      <c r="I74" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J74" s="43" t="s">
+      <c r="J74" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K74" s="7" t="s">
@@ -5772,14 +5761,14 @@
       <c r="AE74" s="35"/>
     </row>
     <row r="75" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A75" s="43">
+      <c r="A75" s="46">
         <f t="shared" si="4"/>
         <v>74</v>
       </c>
-      <c r="B75" s="43" t="s">
+      <c r="B75" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C75" s="43" t="s">
+      <c r="C75" s="46" t="s">
         <v>74</v>
       </c>
       <c r="D75" s="1">
@@ -5797,10 +5786,10 @@
       <c r="H75" s="15">
         <v>1</v>
       </c>
-      <c r="I75" s="43" t="s">
+      <c r="I75" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J75" s="43" t="s">
+      <c r="J75" s="46" t="s">
         <v>23</v>
       </c>
       <c r="K75" s="7" t="s">
@@ -5828,14 +5817,14 @@
       <c r="AE75" s="35"/>
     </row>
     <row r="76" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A76" s="43">
+      <c r="A76" s="46">
         <f t="shared" si="4"/>
         <v>75</v>
       </c>
-      <c r="B76" s="43" t="s">
+      <c r="B76" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="C76" s="43" t="s">
+      <c r="C76" s="46" t="s">
         <v>76</v>
       </c>
       <c r="D76" s="1">
@@ -5853,7 +5842,7 @@
       <c r="H76" s="15">
         <v>1</v>
       </c>
-      <c r="I76" s="43" t="s">
+      <c r="I76" s="46" t="s">
         <v>38</v>
       </c>
       <c r="J76" s="2" t="s">
@@ -5884,14 +5873,14 @@
       <c r="AE76" s="35"/>
     </row>
     <row r="77" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A77" s="43">
+      <c r="A77" s="46">
         <f t="shared" si="4"/>
         <v>76</v>
       </c>
-      <c r="B77" s="43" t="s">
+      <c r="B77" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C77" s="43" t="s">
+      <c r="C77" s="46" t="s">
         <v>33</v>
       </c>
       <c r="D77" s="1">
@@ -5909,10 +5898,10 @@
       <c r="H77" s="15">
         <v>1</v>
       </c>
-      <c r="I77" s="43" t="s">
+      <c r="I77" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J77" s="43" t="s">
+      <c r="J77" s="46" t="s">
         <v>79</v>
       </c>
       <c r="K77" s="7" t="s">
@@ -5940,14 +5929,14 @@
       <c r="AE77" s="35"/>
     </row>
     <row r="78" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A78" s="43">
+      <c r="A78" s="46">
         <f t="shared" si="4"/>
         <v>77</v>
       </c>
-      <c r="B78" s="43" t="s">
+      <c r="B78" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="C78" s="43" t="s">
+      <c r="C78" s="46" t="s">
         <v>29</v>
       </c>
       <c r="D78" s="1">
@@ -5965,10 +5954,10 @@
       <c r="H78" s="15">
         <v>1</v>
       </c>
-      <c r="I78" s="43" t="s">
+      <c r="I78" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J78" s="43" t="s">
+      <c r="J78" s="46" t="s">
         <v>94</v>
       </c>
       <c r="K78" s="7" t="s">
@@ -5996,35 +5985,35 @@
       <c r="AE78" s="35"/>
     </row>
     <row r="79" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A79" s="43">
+      <c r="A79" s="46">
         <f t="shared" si="4"/>
         <v>78</v>
       </c>
-      <c r="B79" s="43" t="s">
+      <c r="B79" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="C79" s="43" t="s">
+      <c r="C79" s="46" t="s">
         <v>33</v>
       </c>
       <c r="D79" s="1">
         <v>42617</v>
       </c>
-      <c r="E79" s="43">
+      <c r="E79" s="46">
         <v>2016</v>
       </c>
-      <c r="F79" s="43" t="s">
+      <c r="F79" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G79" s="43">
+      <c r="G79" s="46">
         <v>2</v>
       </c>
       <c r="H79" s="15">
         <v>1</v>
       </c>
-      <c r="I79" s="43" t="s">
+      <c r="I79" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J79" s="43" t="s">
+      <c r="J79" s="46" t="s">
         <v>94</v>
       </c>
       <c r="K79" s="7" t="s">
@@ -6052,35 +6041,35 @@
       <c r="AE79" s="35"/>
     </row>
     <row r="80" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A80" s="43">
+      <c r="A80" s="46">
         <f t="shared" si="4"/>
         <v>79</v>
       </c>
-      <c r="B80" s="43" t="s">
+      <c r="B80" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C80" s="43" t="s">
+      <c r="C80" s="46" t="s">
         <v>31</v>
       </c>
       <c r="D80" s="1">
         <v>42620</v>
       </c>
-      <c r="E80" s="43">
+      <c r="E80" s="46">
         <v>2016</v>
       </c>
-      <c r="F80" s="43" t="s">
+      <c r="F80" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G80" s="43">
+      <c r="G80" s="46">
         <v>1</v>
       </c>
       <c r="H80" s="15">
         <v>0</v>
       </c>
-      <c r="I80" s="43" t="s">
+      <c r="I80" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J80" s="43" t="s">
+      <c r="J80" s="46" t="s">
         <v>94</v>
       </c>
       <c r="K80" s="7" t="s">
@@ -6108,14 +6097,14 @@
       <c r="AE80" s="35"/>
     </row>
     <row r="81" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A81" s="43">
+      <c r="A81" s="46">
         <f t="shared" si="4"/>
         <v>80</v>
       </c>
-      <c r="B81" s="43" t="s">
+      <c r="B81" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="C81" s="43" t="s">
+      <c r="C81" s="46" t="s">
         <v>31</v>
       </c>
       <c r="D81" s="1">
@@ -6124,19 +6113,19 @@
       <c r="E81" s="15">
         <v>2016</v>
       </c>
-      <c r="F81" s="43" t="s">
+      <c r="F81" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G81" s="43">
+      <c r="G81" s="46">
         <v>1</v>
       </c>
       <c r="H81" s="15">
         <v>0</v>
       </c>
-      <c r="I81" s="43" t="s">
+      <c r="I81" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J81" s="43" t="s">
+      <c r="J81" s="46" t="s">
         <v>94</v>
       </c>
       <c r="K81" s="7" t="s">
@@ -6164,14 +6153,14 @@
       <c r="AE81" s="35"/>
     </row>
     <row r="82" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A82" s="43">
+      <c r="A82" s="46">
         <f t="shared" si="4"/>
         <v>81</v>
       </c>
-      <c r="B82" s="43" t="s">
+      <c r="B82" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="C82" s="43" t="s">
+      <c r="C82" s="46" t="s">
         <v>95</v>
       </c>
       <c r="D82" s="1">
@@ -6180,19 +6169,19 @@
       <c r="E82" s="15">
         <v>2016</v>
       </c>
-      <c r="F82" s="43" t="s">
+      <c r="F82" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G82" s="43">
+      <c r="G82" s="46">
         <v>3</v>
       </c>
       <c r="H82" s="15">
         <v>2</v>
       </c>
-      <c r="I82" s="43" t="s">
+      <c r="I82" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J82" s="43" t="s">
+      <c r="J82" s="46" t="s">
         <v>94</v>
       </c>
       <c r="K82" s="7" t="s">
@@ -6220,14 +6209,14 @@
       <c r="AE82" s="35"/>
     </row>
     <row r="83" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A83" s="43">
+      <c r="A83" s="46">
         <f t="shared" si="4"/>
         <v>82</v>
       </c>
-      <c r="B83" s="43" t="s">
+      <c r="B83" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="C83" s="43" t="s">
+      <c r="C83" s="46" t="s">
         <v>10</v>
       </c>
       <c r="D83" s="1">
@@ -6236,19 +6225,19 @@
       <c r="E83" s="15">
         <v>2016</v>
       </c>
-      <c r="F83" s="43" t="s">
+      <c r="F83" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="G83" s="43">
+      <c r="G83" s="46">
         <v>0</v>
       </c>
       <c r="H83" s="15">
         <v>0</v>
       </c>
-      <c r="I83" s="43" t="s">
+      <c r="I83" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J83" s="43" t="s">
+      <c r="J83" s="46" t="s">
         <v>94</v>
       </c>
       <c r="K83" s="7" t="s">
@@ -6276,14 +6265,14 @@
       <c r="AE83" s="35"/>
     </row>
     <row r="84" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A84" s="43">
+      <c r="A84" s="46">
         <f t="shared" si="4"/>
         <v>83</v>
       </c>
-      <c r="B84" s="43" t="s">
+      <c r="B84" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="C84" s="43" t="s">
+      <c r="C84" s="46" t="s">
         <v>50</v>
       </c>
       <c r="D84" s="1">
@@ -6292,19 +6281,19 @@
       <c r="E84" s="15">
         <v>2016</v>
       </c>
-      <c r="F84" s="43" t="s">
+      <c r="F84" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="G84" s="43">
+      <c r="G84" s="46">
         <v>0</v>
       </c>
       <c r="H84" s="15">
         <v>2</v>
       </c>
-      <c r="I84" s="43" t="s">
+      <c r="I84" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J84" s="43" t="s">
+      <c r="J84" s="46" t="s">
         <v>94</v>
       </c>
       <c r="K84" s="7" t="s">
@@ -6332,14 +6321,14 @@
       <c r="AE84" s="35"/>
     </row>
     <row r="85" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A85" s="43">
+      <c r="A85" s="46">
         <f t="shared" si="4"/>
         <v>84</v>
       </c>
-      <c r="B85" s="43" t="s">
+      <c r="B85" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="C85" s="43" t="s">
+      <c r="C85" s="46" t="s">
         <v>74</v>
       </c>
       <c r="D85" s="1">
@@ -6348,19 +6337,19 @@
       <c r="E85" s="15">
         <v>2016</v>
       </c>
-      <c r="F85" s="43" t="s">
+      <c r="F85" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="G85" s="43">
+      <c r="G85" s="46">
         <v>1</v>
       </c>
       <c r="H85" s="15">
         <v>1</v>
       </c>
-      <c r="I85" s="43" t="s">
+      <c r="I85" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J85" s="43" t="s">
+      <c r="J85" s="46" t="s">
         <v>94</v>
       </c>
       <c r="K85" s="7" t="s">
@@ -6388,7 +6377,7 @@
       <c r="AE85" s="35"/>
     </row>
     <row r="86" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A86" s="43">
+      <c r="A86" s="46">
         <f t="shared" si="4"/>
         <v>85</v>
       </c>
@@ -6404,19 +6393,19 @@
       <c r="E86" s="26">
         <v>2017</v>
       </c>
-      <c r="F86" s="43" t="s">
+      <c r="F86" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="G86" s="43">
+      <c r="G86" s="46">
         <v>1</v>
       </c>
       <c r="H86" s="15">
         <v>1</v>
       </c>
-      <c r="I86" s="43" t="s">
+      <c r="I86" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J86" s="43" t="s">
+      <c r="J86" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K86" s="7" t="s">
@@ -6444,14 +6433,14 @@
       <c r="AE86" s="35"/>
     </row>
     <row r="87" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A87" s="43">
+      <c r="A87" s="46">
         <f t="shared" si="4"/>
         <v>86</v>
       </c>
-      <c r="B87" s="43" t="s">
+      <c r="B87" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="C87" s="43" t="s">
+      <c r="C87" s="46" t="s">
         <v>33</v>
       </c>
       <c r="D87" s="1">
@@ -6460,19 +6449,19 @@
       <c r="E87" s="15">
         <v>2017</v>
       </c>
-      <c r="F87" s="43" t="s">
+      <c r="F87" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G87" s="43">
+      <c r="G87" s="46">
         <v>2</v>
       </c>
       <c r="H87" s="15">
         <v>1</v>
       </c>
-      <c r="I87" s="43" t="s">
+      <c r="I87" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="J87" s="43" t="s">
+      <c r="J87" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K87" s="7" t="s">
@@ -6504,31 +6493,31 @@
         <f t="shared" si="4"/>
         <v>87</v>
       </c>
-      <c r="B88" s="43" t="s">
+      <c r="B88" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="C88" s="43" t="s">
+      <c r="C88" s="46" t="s">
         <v>33</v>
       </c>
       <c r="D88" s="1">
         <v>42770</v>
       </c>
-      <c r="E88" s="43">
+      <c r="E88" s="46">
         <v>2017</v>
       </c>
-      <c r="F88" s="43" t="s">
+      <c r="F88" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G88" s="43">
+      <c r="G88" s="46">
         <v>2</v>
       </c>
-      <c r="H88" s="43">
-        <v>1</v>
-      </c>
-      <c r="I88" s="43" t="s">
+      <c r="H88" s="46">
+        <v>1</v>
+      </c>
+      <c r="I88" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J88" s="43" t="s">
+      <c r="J88" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K88" s="7" t="s">
@@ -6556,7 +6545,7 @@
       <c r="AE88" s="35"/>
     </row>
     <row r="89" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A89" s="43">
+      <c r="A89" s="46">
         <f t="shared" si="4"/>
         <v>88</v>
       </c>
@@ -6612,14 +6601,14 @@
       <c r="AE89" s="35"/>
     </row>
     <row r="90" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A90" s="43">
+      <c r="A90" s="46">
         <f t="shared" si="4"/>
         <v>89</v>
       </c>
-      <c r="B90" s="43" t="s">
+      <c r="B90" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="C90" s="43" t="s">
+      <c r="C90" s="46" t="s">
         <v>31</v>
       </c>
       <c r="D90" s="1">
@@ -6628,19 +6617,19 @@
       <c r="E90" s="15">
         <v>2017</v>
       </c>
-      <c r="F90" s="43" t="s">
+      <c r="F90" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G90" s="43">
+      <c r="G90" s="46">
         <v>1</v>
       </c>
       <c r="H90" s="15">
         <v>0</v>
       </c>
-      <c r="I90" s="43" t="s">
+      <c r="I90" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J90" s="43" t="s">
+      <c r="J90" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K90" s="7" t="s">
@@ -6668,14 +6657,14 @@
       <c r="AE90" s="35"/>
     </row>
     <row r="91" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A91" s="43">
+      <c r="A91" s="46">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
-      <c r="B91" s="43" t="s">
+      <c r="B91" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C91" s="43" t="s">
+      <c r="C91" s="46" t="s">
         <v>10</v>
       </c>
       <c r="D91" s="1">
@@ -6684,19 +6673,19 @@
       <c r="E91" s="15">
         <v>2017</v>
       </c>
-      <c r="F91" s="43" t="s">
+      <c r="F91" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="G91" s="43">
+      <c r="G91" s="46">
         <v>0</v>
       </c>
       <c r="H91" s="15">
         <v>0</v>
       </c>
-      <c r="I91" s="43" t="s">
+      <c r="I91" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J91" s="43" t="s">
+      <c r="J91" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K91" s="7" t="s">
@@ -6724,14 +6713,14 @@
       <c r="AE91" s="35"/>
     </row>
     <row r="92" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A92" s="43">
+      <c r="A92" s="46">
         <f t="shared" si="4"/>
         <v>91</v>
       </c>
-      <c r="B92" s="43" t="s">
+      <c r="B92" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C92" s="43" t="s">
+      <c r="C92" s="46" t="s">
         <v>8</v>
       </c>
       <c r="D92" s="1">
@@ -6740,19 +6729,19 @@
       <c r="E92" s="15">
         <v>2017</v>
       </c>
-      <c r="F92" s="43" t="s">
+      <c r="F92" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="G92" s="43">
+      <c r="G92" s="46">
         <v>2</v>
       </c>
       <c r="H92" s="15">
         <v>3</v>
       </c>
-      <c r="I92" s="43" t="s">
+      <c r="I92" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J92" s="43" t="s">
+      <c r="J92" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K92" s="7" t="s">
@@ -6780,14 +6769,14 @@
       <c r="AE92" s="35"/>
     </row>
     <row r="93" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A93" s="43">
+      <c r="A93" s="46">
         <f t="shared" si="4"/>
         <v>92</v>
       </c>
-      <c r="B93" s="43" t="s">
+      <c r="B93" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C93" s="43" t="s">
+      <c r="C93" s="46" t="s">
         <v>29</v>
       </c>
       <c r="D93" s="1">
@@ -6796,19 +6785,19 @@
       <c r="E93" s="15">
         <v>2017</v>
       </c>
-      <c r="F93" s="43" t="s">
+      <c r="F93" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G93" s="43">
+      <c r="G93" s="46">
         <v>3</v>
       </c>
       <c r="H93" s="15">
         <v>1</v>
       </c>
-      <c r="I93" s="43" t="s">
+      <c r="I93" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J93" s="43" t="s">
+      <c r="J93" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K93" s="7" t="s">
@@ -6836,14 +6825,14 @@
       <c r="AE93" s="35"/>
     </row>
     <row r="94" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A94" s="43">
+      <c r="A94" s="46">
         <f t="shared" si="4"/>
         <v>93</v>
       </c>
-      <c r="B94" s="43" t="s">
+      <c r="B94" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C94" s="43" t="s">
+      <c r="C94" s="46" t="s">
         <v>50</v>
       </c>
       <c r="D94" s="1">
@@ -6852,19 +6841,19 @@
       <c r="E94" s="15">
         <v>2017</v>
       </c>
-      <c r="F94" s="43" t="s">
+      <c r="F94" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="G94" s="43">
+      <c r="G94" s="46">
         <v>0</v>
       </c>
       <c r="H94" s="15">
         <v>2</v>
       </c>
-      <c r="I94" s="43" t="s">
+      <c r="I94" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J94" s="43" t="s">
+      <c r="J94" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K94" s="7" t="s">
@@ -6892,14 +6881,14 @@
       <c r="AE94" s="35"/>
     </row>
     <row r="95" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A95" s="43">
+      <c r="A95" s="46">
         <f t="shared" si="4"/>
         <v>94</v>
       </c>
-      <c r="B95" s="43" t="s">
+      <c r="B95" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="C95" s="43" t="s">
+      <c r="C95" s="46" t="s">
         <v>106</v>
       </c>
       <c r="D95" s="1">
@@ -6908,19 +6897,19 @@
       <c r="E95" s="15">
         <v>2017</v>
       </c>
-      <c r="F95" s="43" t="s">
+      <c r="F95" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G95" s="43">
+      <c r="G95" s="46">
         <v>2</v>
       </c>
       <c r="H95" s="15">
         <v>1</v>
       </c>
-      <c r="I95" s="43" t="s">
+      <c r="I95" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="J95" s="43" t="s">
+      <c r="J95" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K95" s="7" t="s">
@@ -6948,14 +6937,14 @@
       <c r="AE95" s="35"/>
     </row>
     <row r="96" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A96" s="43">
+      <c r="A96" s="46">
         <f t="shared" si="4"/>
         <v>95</v>
       </c>
-      <c r="B96" s="43" t="s">
+      <c r="B96" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="C96" s="43" t="s">
+      <c r="C96" s="46" t="s">
         <v>50</v>
       </c>
       <c r="D96" s="1">
@@ -6964,19 +6953,19 @@
       <c r="E96" s="15">
         <v>2017</v>
       </c>
-      <c r="F96" s="43" t="s">
+      <c r="F96" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="G96" s="43">
+      <c r="G96" s="46">
         <v>0</v>
       </c>
       <c r="H96" s="15">
         <v>2</v>
       </c>
-      <c r="I96" s="43" t="s">
+      <c r="I96" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="J96" s="43" t="s">
+      <c r="J96" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K96" s="7" t="s">
@@ -7004,14 +6993,14 @@
       <c r="AE96" s="35"/>
     </row>
     <row r="97" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A97" s="43">
+      <c r="A97" s="46">
         <f t="shared" si="4"/>
         <v>96</v>
       </c>
-      <c r="B97" s="43" t="s">
+      <c r="B97" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="C97" s="43" t="s">
+      <c r="C97" s="46" t="s">
         <v>109</v>
       </c>
       <c r="D97" s="1">
@@ -7020,19 +7009,19 @@
       <c r="E97" s="15">
         <v>2017</v>
       </c>
-      <c r="F97" s="43" t="s">
+      <c r="F97" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G97" s="43">
+      <c r="G97" s="46">
         <v>1</v>
       </c>
       <c r="H97" s="15">
         <v>0</v>
       </c>
-      <c r="I97" s="43" t="s">
+      <c r="I97" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="J97" s="43" t="s">
+      <c r="J97" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K97" s="7" t="s">
@@ -7060,14 +7049,14 @@
       <c r="AE97" s="35"/>
     </row>
     <row r="98" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A98" s="43">
+      <c r="A98" s="46">
         <f t="shared" si="4"/>
         <v>97</v>
       </c>
-      <c r="B98" s="43" t="s">
+      <c r="B98" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="C98" s="43" t="s">
+      <c r="C98" s="46" t="s">
         <v>19</v>
       </c>
       <c r="D98" s="1">
@@ -7076,19 +7065,19 @@
       <c r="E98" s="15">
         <v>2017</v>
       </c>
-      <c r="F98" s="43" t="s">
+      <c r="F98" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G98" s="43">
+      <c r="G98" s="46">
         <v>2</v>
       </c>
       <c r="H98" s="15">
         <v>0</v>
       </c>
-      <c r="I98" s="43" t="s">
+      <c r="I98" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J98" s="43" t="s">
+      <c r="J98" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K98" s="7" t="s">
@@ -7120,10 +7109,10 @@
         <f t="shared" si="4"/>
         <v>98</v>
       </c>
-      <c r="B99" s="43" t="s">
+      <c r="B99" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="C99" s="43" t="s">
+      <c r="C99" s="46" t="s">
         <v>109</v>
       </c>
       <c r="D99" s="1">
@@ -7132,19 +7121,19 @@
       <c r="E99" s="15">
         <v>2017</v>
       </c>
-      <c r="F99" s="43" t="s">
+      <c r="F99" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G99" s="43">
+      <c r="G99" s="46">
         <v>1</v>
       </c>
       <c r="H99" s="15">
         <v>0</v>
       </c>
-      <c r="I99" s="43" t="s">
+      <c r="I99" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J99" s="43" t="s">
+      <c r="J99" s="46" t="s">
         <v>1</v>
       </c>
       <c r="K99" s="7" t="s">
@@ -7172,7 +7161,7 @@
       <c r="AE99" s="35"/>
     </row>
     <row r="100" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A100" s="43">
+      <c r="A100" s="46">
         <f t="shared" si="4"/>
         <v>99</v>
       </c>
@@ -7228,14 +7217,14 @@
       <c r="AE100" s="35"/>
     </row>
     <row r="101" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A101" s="43">
+      <c r="A101" s="46">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="B101" s="43" t="s">
+      <c r="B101" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C101" s="43" t="s">
+      <c r="C101" s="46" t="s">
         <v>29</v>
       </c>
       <c r="D101" s="1">
@@ -7244,22 +7233,22 @@
       <c r="E101" s="15">
         <v>2017</v>
       </c>
-      <c r="F101" s="43" t="s">
+      <c r="F101" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G101" s="43">
+      <c r="G101" s="46">
         <v>3</v>
       </c>
       <c r="H101" s="15">
         <v>1</v>
       </c>
-      <c r="I101" s="43" t="s">
+      <c r="I101" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J101" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="K101" s="43" t="s">
+      <c r="J101" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K101" s="46" t="s">
         <v>0</v>
       </c>
       <c r="L101" s="35"/>
@@ -7283,10 +7272,10 @@
         <f t="shared" si="4"/>
         <v>101</v>
       </c>
-      <c r="B102" s="43" t="s">
+      <c r="B102" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="C102" s="43" t="s">
+      <c r="C102" s="46" t="s">
         <v>50</v>
       </c>
       <c r="D102" s="1">
@@ -7295,22 +7284,22 @@
       <c r="E102" s="15">
         <v>2017</v>
       </c>
-      <c r="F102" s="43" t="s">
+      <c r="F102" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="G102" s="43">
+      <c r="G102" s="46">
         <v>0</v>
       </c>
       <c r="H102" s="15">
         <v>2</v>
       </c>
-      <c r="I102" s="43" t="s">
+      <c r="I102" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J102" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="K102" s="43" t="s">
+      <c r="J102" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K102" s="46" t="s">
         <v>0</v>
       </c>
       <c r="L102" s="35"/>
@@ -7381,7 +7370,7 @@
       <c r="Z103" s="35"/>
     </row>
     <row r="104" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A104" s="43">
+      <c r="A104" s="46">
         <f t="shared" si="4"/>
         <v>103</v>
       </c>
@@ -7436,10 +7425,10 @@
         <f t="shared" si="4"/>
         <v>104</v>
       </c>
-      <c r="B105" s="43" t="s">
+      <c r="B105" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="C105" s="43" t="s">
+      <c r="C105" s="46" t="s">
         <v>33</v>
       </c>
       <c r="D105" s="1">
@@ -7448,22 +7437,22 @@
       <c r="E105" s="15">
         <v>2017</v>
       </c>
-      <c r="F105" s="43" t="s">
+      <c r="F105" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G105" s="43">
+      <c r="G105" s="46">
         <v>2</v>
       </c>
       <c r="H105" s="15">
         <v>1</v>
       </c>
-      <c r="I105" s="43" t="s">
+      <c r="I105" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J105" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="K105" s="43" t="s">
+      <c r="J105" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K105" s="46" t="s">
         <v>0</v>
       </c>
       <c r="L105" s="35"/>
@@ -7483,7 +7472,7 @@
       <c r="Z105" s="35"/>
     </row>
     <row r="106" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A106" s="43">
+      <c r="A106" s="46">
         <f t="shared" si="4"/>
         <v>105</v>
       </c>
@@ -7538,10 +7527,10 @@
         <f t="shared" si="4"/>
         <v>106</v>
       </c>
-      <c r="B107" s="43" t="s">
+      <c r="B107" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="C107" s="43" t="s">
+      <c r="C107" s="46" t="s">
         <v>111</v>
       </c>
       <c r="D107" s="1">
@@ -7550,22 +7539,22 @@
       <c r="E107" s="15">
         <v>2017</v>
       </c>
-      <c r="F107" s="43" t="s">
+      <c r="F107" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="G107" s="43">
+      <c r="G107" s="46">
         <v>3</v>
       </c>
       <c r="H107" s="15">
         <v>4</v>
       </c>
-      <c r="I107" s="43" t="s">
+      <c r="I107" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J107" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="K107" s="43" t="s">
+      <c r="J107" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K107" s="46" t="s">
         <v>0</v>
       </c>
       <c r="L107" s="35"/>
@@ -7585,7 +7574,7 @@
       <c r="Z107" s="35"/>
     </row>
     <row r="108" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A108" s="43">
+      <c r="A108" s="46">
         <f t="shared" si="4"/>
         <v>107</v>
       </c>
@@ -7636,14 +7625,14 @@
       <c r="Z108" s="35"/>
     </row>
     <row r="109" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A109" s="43">
-        <f t="shared" ref="A109:A131" si="5">SUM(A108+1)</f>
+      <c r="A109" s="46">
+        <f t="shared" ref="A109:A132" si="5">SUM(A108+1)</f>
         <v>108</v>
       </c>
-      <c r="B109" s="43" t="s">
+      <c r="B109" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="C109" s="43" t="s">
+      <c r="C109" s="46" t="s">
         <v>19</v>
       </c>
       <c r="D109" s="1">
@@ -7652,22 +7641,22 @@
       <c r="E109" s="15">
         <v>2017</v>
       </c>
-      <c r="F109" s="43" t="s">
+      <c r="F109" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G109" s="43">
+      <c r="G109" s="46">
         <v>2</v>
       </c>
       <c r="H109" s="15">
         <v>0</v>
       </c>
-      <c r="I109" s="43" t="s">
+      <c r="I109" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="J109" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="K109" s="43" t="s">
+      <c r="J109" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K109" s="46" t="s">
         <v>0</v>
       </c>
       <c r="L109" s="35"/>
@@ -7687,14 +7676,14 @@
       <c r="Z109" s="35"/>
     </row>
     <row r="110" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A110" s="43">
+      <c r="A110" s="46">
         <f t="shared" si="5"/>
         <v>109</v>
       </c>
-      <c r="B110" s="43" t="s">
+      <c r="B110" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="C110" s="43" t="s">
+      <c r="C110" s="46" t="s">
         <v>31</v>
       </c>
       <c r="D110" s="1">
@@ -7703,22 +7692,22 @@
       <c r="E110" s="15">
         <v>2017</v>
       </c>
-      <c r="F110" s="43" t="s">
+      <c r="F110" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G110" s="43">
+      <c r="G110" s="46">
         <v>1</v>
       </c>
       <c r="H110" s="15">
         <v>0</v>
       </c>
-      <c r="I110" s="43" t="s">
+      <c r="I110" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J110" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="K110" s="43" t="s">
+      <c r="J110" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K110" s="46" t="s">
         <v>0</v>
       </c>
       <c r="L110" s="35"/>
@@ -7742,10 +7731,10 @@
         <f t="shared" si="5"/>
         <v>110</v>
       </c>
-      <c r="B111" s="43" t="s">
+      <c r="B111" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C111" s="43" t="s">
+      <c r="C111" s="46" t="s">
         <v>10</v>
       </c>
       <c r="D111" s="1">
@@ -7754,22 +7743,22 @@
       <c r="E111" s="15">
         <v>2017</v>
       </c>
-      <c r="F111" s="43" t="s">
+      <c r="F111" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="G111" s="43">
+      <c r="G111" s="46">
         <v>0</v>
       </c>
       <c r="H111" s="15">
         <v>0</v>
       </c>
-      <c r="I111" s="43" t="s">
+      <c r="I111" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="J111" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="K111" s="43" t="s">
+      <c r="J111" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K111" s="46" t="s">
         <v>0</v>
       </c>
       <c r="L111" s="35"/>
@@ -7789,7 +7778,7 @@
       <c r="Z111" s="35"/>
     </row>
     <row r="112" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A112" s="43">
+      <c r="A112" s="46">
         <f t="shared" si="5"/>
         <v>111</v>
       </c>
@@ -7840,14 +7829,14 @@
       <c r="Z112" s="35"/>
     </row>
     <row r="113" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A113" s="43">
+      <c r="A113" s="46">
         <f t="shared" si="5"/>
         <v>112</v>
       </c>
-      <c r="B113" s="43" t="s">
+      <c r="B113" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C113" s="43" t="s">
+      <c r="C113" s="46" t="s">
         <v>19</v>
       </c>
       <c r="D113" s="1">
@@ -7856,22 +7845,22 @@
       <c r="E113" s="15">
         <v>2017</v>
       </c>
-      <c r="F113" s="43" t="s">
+      <c r="F113" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G113" s="43">
+      <c r="G113" s="46">
         <v>2</v>
       </c>
       <c r="H113" s="15">
         <v>0</v>
       </c>
-      <c r="I113" s="43" t="s">
+      <c r="I113" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J113" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="K113" s="43" t="s">
+      <c r="J113" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K113" s="46" t="s">
         <v>0</v>
       </c>
       <c r="L113" s="35"/>
@@ -7891,14 +7880,14 @@
       <c r="Z113" s="35"/>
     </row>
     <row r="114" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A114" s="44">
+      <c r="A114" s="46">
         <f t="shared" si="5"/>
         <v>113</v>
       </c>
-      <c r="B114" s="43" t="s">
+      <c r="B114" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="C114" s="43" t="s">
+      <c r="C114" s="46" t="s">
         <v>10</v>
       </c>
       <c r="D114" s="1">
@@ -7907,22 +7896,22 @@
       <c r="E114" s="15">
         <v>2017</v>
       </c>
-      <c r="F114" s="43" t="s">
+      <c r="F114" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="G114" s="43">
+      <c r="G114" s="46">
         <v>0</v>
       </c>
       <c r="H114" s="15">
         <v>0</v>
       </c>
-      <c r="I114" s="43" t="s">
+      <c r="I114" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J114" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="K114" s="43" t="s">
+      <c r="J114" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K114" s="46" t="s">
         <v>0</v>
       </c>
       <c r="L114" s="35"/>
@@ -7942,14 +7931,14 @@
       <c r="Z114" s="35"/>
     </row>
     <row r="115" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A115" s="44">
+      <c r="A115" s="46">
         <f t="shared" si="5"/>
         <v>114</v>
       </c>
-      <c r="B115" s="44" t="s">
+      <c r="B115" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C115" s="44" t="s">
+      <c r="C115" s="46" t="s">
         <v>19</v>
       </c>
       <c r="D115" s="1">
@@ -7958,22 +7947,22 @@
       <c r="E115" s="15">
         <v>2017</v>
       </c>
-      <c r="F115" s="44" t="s">
+      <c r="F115" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G115" s="44">
+      <c r="G115" s="46">
         <v>2</v>
       </c>
       <c r="H115" s="15">
         <v>0</v>
       </c>
-      <c r="I115" s="44" t="s">
+      <c r="I115" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J115" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="K115" s="44" t="s">
+      <c r="J115" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K115" s="46" t="s">
         <v>49</v>
       </c>
       <c r="L115" s="35"/>
@@ -7993,38 +7982,38 @@
       <c r="Z115" s="35"/>
     </row>
     <row r="116" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A116" s="44">
+      <c r="A116" s="46">
         <f t="shared" si="5"/>
         <v>115</v>
       </c>
-      <c r="B116" s="44" t="s">
+      <c r="B116" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C116" s="44" t="s">
+      <c r="C116" s="46" t="s">
         <v>8</v>
       </c>
       <c r="D116" s="1">
         <v>43009</v>
       </c>
-      <c r="E116" s="44">
+      <c r="E116" s="46">
         <v>2017</v>
       </c>
-      <c r="F116" s="44" t="s">
+      <c r="F116" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="G116" s="44">
+      <c r="G116" s="46">
         <v>2</v>
       </c>
-      <c r="H116" s="44">
+      <c r="H116" s="46">
         <v>3</v>
       </c>
-      <c r="I116" s="44" t="s">
+      <c r="I116" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J116" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="K116" s="44" t="s">
+      <c r="J116" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K116" s="46" t="s">
         <v>0</v>
       </c>
       <c r="L116" s="35"/>
@@ -8044,38 +8033,38 @@
       <c r="Z116" s="35"/>
     </row>
     <row r="117" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A117" s="44">
+      <c r="A117" s="46">
         <f t="shared" si="5"/>
         <v>116</v>
       </c>
-      <c r="B117" s="44" t="s">
+      <c r="B117" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="C117" s="44" t="s">
+      <c r="C117" s="46" t="s">
         <v>106</v>
       </c>
       <c r="D117" s="1">
         <v>43019</v>
       </c>
-      <c r="E117" s="44">
+      <c r="E117" s="46">
         <v>2017</v>
       </c>
-      <c r="F117" s="44" t="s">
+      <c r="F117" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G117" s="44">
+      <c r="G117" s="46">
         <v>2</v>
       </c>
-      <c r="H117" s="44">
-        <v>1</v>
-      </c>
-      <c r="I117" s="44" t="s">
+      <c r="H117" s="46">
+        <v>1</v>
+      </c>
+      <c r="I117" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J117" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="K117" s="44" t="s">
+      <c r="J117" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K117" s="46" t="s">
         <v>49</v>
       </c>
       <c r="L117" s="35"/>
@@ -8095,38 +8084,38 @@
       <c r="Z117" s="35"/>
     </row>
     <row r="118" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A118" s="44">
+      <c r="A118" s="46">
         <f t="shared" si="5"/>
         <v>117</v>
       </c>
-      <c r="B118" s="44" t="s">
+      <c r="B118" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C118" s="44" t="s">
+      <c r="C118" s="46" t="s">
         <v>13</v>
       </c>
       <c r="D118" s="1">
         <v>43022</v>
       </c>
-      <c r="E118" s="44">
+      <c r="E118" s="46">
         <v>2017</v>
       </c>
-      <c r="F118" s="44" t="s">
+      <c r="F118" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="G118" s="44">
-        <v>0</v>
-      </c>
-      <c r="H118" s="44">
-        <v>1</v>
-      </c>
-      <c r="I118" s="44" t="s">
+      <c r="G118" s="46">
+        <v>0</v>
+      </c>
+      <c r="H118" s="46">
+        <v>1</v>
+      </c>
+      <c r="I118" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J118" s="44" t="s">
+      <c r="J118" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="K118" s="44" t="s">
+      <c r="K118" s="46" t="s">
         <v>0</v>
       </c>
       <c r="L118" s="35"/>
@@ -8146,38 +8135,38 @@
       <c r="Z118" s="35"/>
     </row>
     <row r="119" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A119" s="45">
+      <c r="A119" s="46">
         <f t="shared" si="5"/>
         <v>118</v>
       </c>
-      <c r="B119" s="44" t="s">
+      <c r="B119" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C119" s="44" t="s">
+      <c r="C119" s="46" t="s">
         <v>33</v>
       </c>
       <c r="D119" s="1">
         <v>43031</v>
       </c>
-      <c r="E119" s="44">
+      <c r="E119" s="46">
         <v>2017</v>
       </c>
-      <c r="F119" s="44" t="s">
+      <c r="F119" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G119" s="44">
+      <c r="G119" s="46">
         <v>2</v>
       </c>
-      <c r="H119" s="44">
-        <v>1</v>
-      </c>
-      <c r="I119" s="44" t="s">
+      <c r="H119" s="46">
+        <v>1</v>
+      </c>
+      <c r="I119" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J119" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="K119" s="44" t="s">
+      <c r="J119" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K119" s="46" t="s">
         <v>0</v>
       </c>
       <c r="L119" s="35"/>
@@ -8201,34 +8190,34 @@
         <f t="shared" si="5"/>
         <v>119</v>
       </c>
-      <c r="B120" s="45" t="s">
+      <c r="B120" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C120" s="45" t="s">
+      <c r="C120" s="46" t="s">
         <v>25</v>
       </c>
       <c r="D120" s="1">
         <v>43043</v>
       </c>
-      <c r="E120" s="45">
+      <c r="E120" s="46">
         <v>2017</v>
       </c>
-      <c r="F120" s="45" t="s">
+      <c r="F120" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="G120" s="45">
-        <v>1</v>
-      </c>
-      <c r="H120" s="45">
+      <c r="G120" s="46">
+        <v>1</v>
+      </c>
+      <c r="H120" s="46">
         <v>2</v>
       </c>
-      <c r="I120" s="45" t="s">
+      <c r="I120" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J120" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="K120" s="49" t="s">
+      <c r="J120" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K120" s="46" t="s">
         <v>0</v>
       </c>
       <c r="L120" s="35"/>
@@ -8248,7 +8237,7 @@
       <c r="Z120" s="35"/>
     </row>
     <row r="121" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A121" s="47">
+      <c r="A121" s="46">
         <f t="shared" si="5"/>
         <v>120</v>
       </c>
@@ -8279,7 +8268,7 @@
       <c r="J121" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="K121" s="49" t="s">
+      <c r="K121" s="46" t="s">
         <v>0</v>
       </c>
       <c r="L121" s="35"/>
@@ -8299,38 +8288,38 @@
       <c r="Z121" s="35"/>
     </row>
     <row r="122" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A122" s="48">
+      <c r="A122" s="46">
         <f t="shared" si="5"/>
         <v>121</v>
       </c>
-      <c r="B122" s="47" t="s">
+      <c r="B122" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="C122" s="47" t="s">
+      <c r="C122" s="46" t="s">
         <v>25</v>
       </c>
       <c r="D122" s="1">
         <v>43055</v>
       </c>
-      <c r="E122" s="47">
+      <c r="E122" s="46">
         <v>2017</v>
       </c>
-      <c r="F122" s="47" t="s">
+      <c r="F122" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="G122" s="47">
-        <v>1</v>
-      </c>
-      <c r="H122" s="47">
+      <c r="G122" s="46">
+        <v>1</v>
+      </c>
+      <c r="H122" s="46">
         <v>2</v>
       </c>
-      <c r="I122" s="47" t="s">
+      <c r="I122" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J122" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="K122" s="49" t="s">
+      <c r="J122" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K122" s="46" t="s">
         <v>0</v>
       </c>
       <c r="L122" s="35"/>
@@ -8350,38 +8339,38 @@
       <c r="Z122" s="35"/>
     </row>
     <row r="123" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A123" s="49">
+      <c r="A123" s="46">
         <f t="shared" si="5"/>
         <v>122</v>
       </c>
-      <c r="B123" s="48" t="s">
+      <c r="B123" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="C123" s="48" t="s">
+      <c r="C123" s="46" t="s">
         <v>47</v>
       </c>
       <c r="D123" s="1">
         <v>43072</v>
       </c>
-      <c r="E123" s="48">
+      <c r="E123" s="46">
         <v>2017</v>
       </c>
-      <c r="F123" s="48" t="s">
+      <c r="F123" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="G123" s="48">
+      <c r="G123" s="46">
         <v>2</v>
       </c>
-      <c r="H123" s="48">
+      <c r="H123" s="46">
         <v>2</v>
       </c>
-      <c r="I123" s="48" t="s">
+      <c r="I123" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J123" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="K123" s="49" t="s">
+      <c r="J123" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K123" s="46" t="s">
         <v>0</v>
       </c>
       <c r="L123" s="35"/>
@@ -8401,38 +8390,38 @@
       <c r="Z123" s="35"/>
     </row>
     <row r="124" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A124" s="54">
+      <c r="A124" s="46">
         <f t="shared" si="5"/>
         <v>123</v>
       </c>
-      <c r="B124" s="54" t="s">
+      <c r="B124" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="C124" s="54" t="s">
+      <c r="C124" s="46" t="s">
         <v>47</v>
       </c>
       <c r="D124" s="1">
         <v>43116</v>
       </c>
-      <c r="E124" s="54">
+      <c r="E124" s="46">
         <v>2018</v>
       </c>
-      <c r="F124" s="54" t="s">
+      <c r="F124" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="G124" s="54">
+      <c r="G124" s="46">
         <v>2</v>
       </c>
-      <c r="H124" s="54">
+      <c r="H124" s="46">
         <v>2</v>
       </c>
-      <c r="I124" s="54" t="s">
+      <c r="I124" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J124" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="K124" s="54" t="s">
+      <c r="J124" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K124" s="46" t="s">
         <v>0</v>
       </c>
       <c r="L124" s="35"/>
@@ -8452,38 +8441,38 @@
       <c r="Z124" s="35"/>
     </row>
     <row r="125" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A125" s="54">
+      <c r="A125" s="46">
         <f t="shared" si="5"/>
         <v>124</v>
       </c>
-      <c r="B125" s="54" t="s">
+      <c r="B125" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C125" s="54" t="s">
+      <c r="C125" s="46" t="s">
         <v>10</v>
       </c>
       <c r="D125" s="1">
         <v>43120</v>
       </c>
-      <c r="E125" s="54">
+      <c r="E125" s="46">
         <v>2018</v>
       </c>
-      <c r="F125" s="54" t="s">
+      <c r="F125" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="G125" s="54">
-        <v>0</v>
-      </c>
-      <c r="H125" s="54">
-        <v>0</v>
-      </c>
-      <c r="I125" s="54" t="s">
+      <c r="G125" s="46">
+        <v>0</v>
+      </c>
+      <c r="H125" s="46">
+        <v>0</v>
+      </c>
+      <c r="I125" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J125" s="54" t="s">
+      <c r="J125" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="K125" s="54" t="s">
+      <c r="K125" s="46" t="s">
         <v>0</v>
       </c>
       <c r="L125" s="35"/>
@@ -8503,76 +8492,106 @@
       <c r="Z125" s="35"/>
     </row>
     <row r="126" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A126" s="54">
+      <c r="A126" s="46">
         <f t="shared" si="5"/>
         <v>125</v>
       </c>
-      <c r="B126" s="54" t="s">
+      <c r="B126" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="C126" s="54" t="s">
+      <c r="C126" s="46" t="s">
         <v>31</v>
       </c>
       <c r="D126" s="1">
-        <v>42763</v>
-      </c>
-      <c r="E126" s="54">
+        <v>43128</v>
+      </c>
+      <c r="E126" s="46">
         <v>2018</v>
       </c>
-      <c r="F126" s="54" t="s">
+      <c r="F126" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G126" s="54">
-        <v>1</v>
-      </c>
-      <c r="H126" s="54">
-        <v>0</v>
-      </c>
-      <c r="I126" s="54" t="s">
+      <c r="G126" s="46">
+        <v>1</v>
+      </c>
+      <c r="H126" s="46">
+        <v>0</v>
+      </c>
+      <c r="I126" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J126" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="K126" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="J126" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K126" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="L126" s="35"/>
+      <c r="M126" s="35"/>
+      <c r="N126" s="35"/>
+      <c r="O126" s="35"/>
+      <c r="P126" s="35"/>
+      <c r="Q126" s="35"/>
+      <c r="R126" s="35"/>
+      <c r="S126" s="35"/>
+      <c r="T126" s="35"/>
+      <c r="U126" s="35"/>
+      <c r="V126" s="35"/>
+      <c r="W126" s="35"/>
+      <c r="X126" s="35"/>
+      <c r="Y126" s="35"/>
+      <c r="Z126" s="35"/>
     </row>
     <row r="127" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A127" s="54">
+      <c r="A127" s="46">
         <f t="shared" si="5"/>
         <v>126</v>
       </c>
-      <c r="B127" s="54" t="s">
+      <c r="B127" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C127" s="54" t="s">
+      <c r="C127" s="46" t="s">
         <v>10</v>
       </c>
       <c r="D127" s="1">
         <v>43134</v>
       </c>
-      <c r="E127" s="54">
+      <c r="E127" s="46">
         <v>2018</v>
       </c>
-      <c r="F127" s="54" t="s">
+      <c r="F127" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="G127" s="54">
-        <v>0</v>
-      </c>
-      <c r="H127" s="54">
-        <v>0</v>
-      </c>
-      <c r="I127" s="54" t="s">
+      <c r="G127" s="46">
+        <v>0</v>
+      </c>
+      <c r="H127" s="46">
+        <v>0</v>
+      </c>
+      <c r="I127" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J127" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="K127" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="J127" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K127" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="L127" s="35"/>
+      <c r="M127" s="35"/>
+      <c r="N127" s="35"/>
+      <c r="O127" s="35"/>
+      <c r="P127" s="35"/>
+      <c r="Q127" s="35"/>
+      <c r="R127" s="35"/>
+      <c r="S127" s="35"/>
+      <c r="T127" s="35"/>
+      <c r="U127" s="35"/>
+      <c r="V127" s="35"/>
+      <c r="W127" s="35"/>
+      <c r="X127" s="35"/>
+      <c r="Y127" s="35"/>
+      <c r="Z127" s="35"/>
     </row>
     <row r="128" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A128" s="42">
@@ -8609,114 +8628,225 @@
       <c r="K128" s="42" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A129" s="54">
+      <c r="L128" s="35"/>
+      <c r="M128" s="35"/>
+      <c r="N128" s="35"/>
+      <c r="O128" s="35"/>
+      <c r="P128" s="35"/>
+      <c r="Q128" s="35"/>
+      <c r="R128" s="35"/>
+      <c r="S128" s="35"/>
+      <c r="T128" s="35"/>
+      <c r="U128" s="35"/>
+      <c r="V128" s="35"/>
+      <c r="W128" s="35"/>
+      <c r="X128" s="35"/>
+      <c r="Y128" s="35"/>
+      <c r="Z128" s="35"/>
+    </row>
+    <row r="129" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A129" s="46">
         <f t="shared" si="5"/>
         <v>128</v>
       </c>
-      <c r="B129" s="54" t="s">
+      <c r="B129" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C129" s="54" t="s">
+      <c r="C129" s="46" t="s">
         <v>8</v>
       </c>
       <c r="D129" s="1">
         <v>43177</v>
       </c>
-      <c r="E129" s="54">
+      <c r="E129" s="46">
         <v>2018</v>
       </c>
-      <c r="F129" s="54" t="s">
+      <c r="F129" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="G129" s="54">
+      <c r="G129" s="46">
         <v>2</v>
       </c>
-      <c r="H129" s="54">
+      <c r="H129" s="46">
         <v>3</v>
       </c>
-      <c r="I129" s="54" t="s">
+      <c r="I129" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J129" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="K129" s="54" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A130" s="54">
+      <c r="J129" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K129" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="L129" s="35"/>
+      <c r="M129" s="35"/>
+      <c r="N129" s="35"/>
+      <c r="O129" s="35"/>
+      <c r="P129" s="35"/>
+      <c r="Q129" s="35"/>
+      <c r="R129" s="35"/>
+      <c r="S129" s="35"/>
+      <c r="T129" s="35"/>
+      <c r="U129" s="35"/>
+      <c r="V129" s="35"/>
+      <c r="W129" s="35"/>
+      <c r="X129" s="35"/>
+      <c r="Y129" s="35"/>
+      <c r="Z129" s="35"/>
+    </row>
+    <row r="130" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A130" s="46">
         <f t="shared" si="5"/>
         <v>129</v>
       </c>
-      <c r="B130" s="54" t="s">
+      <c r="B130" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C130" s="54" t="s">
+      <c r="C130" s="46" t="s">
         <v>95</v>
       </c>
       <c r="D130" s="1">
         <v>43180</v>
       </c>
-      <c r="E130" s="54">
+      <c r="E130" s="46">
         <v>2018</v>
       </c>
-      <c r="F130" s="54" t="s">
+      <c r="F130" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G130" s="54">
+      <c r="G130" s="46">
         <v>3</v>
       </c>
-      <c r="H130" s="54">
+      <c r="H130" s="46">
         <v>2</v>
       </c>
-      <c r="I130" s="54" t="s">
+      <c r="I130" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J130" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="K130" s="54" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A131" s="54">
+      <c r="J130" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K130" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="L130" s="35"/>
+      <c r="M130" s="35"/>
+      <c r="N130" s="35"/>
+      <c r="O130" s="35"/>
+      <c r="P130" s="35"/>
+      <c r="Q130" s="35"/>
+      <c r="R130" s="35"/>
+      <c r="S130" s="35"/>
+      <c r="T130" s="35"/>
+      <c r="U130" s="35"/>
+      <c r="V130" s="35"/>
+      <c r="W130" s="35"/>
+      <c r="X130" s="35"/>
+      <c r="Y130" s="35"/>
+      <c r="Z130" s="35"/>
+    </row>
+    <row r="131" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A131" s="46">
         <f t="shared" si="5"/>
         <v>130</v>
       </c>
-      <c r="B131" s="54" t="s">
+      <c r="B131" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C131" s="54" t="s">
+      <c r="C131" s="46" t="s">
         <v>4</v>
       </c>
       <c r="D131" s="1">
         <v>43181</v>
       </c>
-      <c r="E131" s="54">
+      <c r="E131" s="46">
         <v>2018</v>
       </c>
-      <c r="F131" s="54" t="s">
+      <c r="F131" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="G131" s="54">
-        <v>0</v>
-      </c>
-      <c r="H131" s="54">
+      <c r="G131" s="46">
+        <v>0</v>
+      </c>
+      <c r="H131" s="46">
         <v>3</v>
       </c>
-      <c r="I131" s="54" t="s">
+      <c r="I131" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J131" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="K131" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="J131" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="K131" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="L131" s="35"/>
+      <c r="M131" s="35"/>
+      <c r="N131" s="35"/>
+      <c r="O131" s="35"/>
+      <c r="P131" s="35"/>
+      <c r="Q131" s="35"/>
+      <c r="R131" s="35"/>
+      <c r="S131" s="35"/>
+      <c r="T131" s="35"/>
+      <c r="U131" s="35"/>
+      <c r="V131" s="35"/>
+      <c r="W131" s="35"/>
+      <c r="X131" s="35"/>
+      <c r="Y131" s="35"/>
+      <c r="Z131" s="35"/>
+    </row>
+    <row r="132" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A132" s="46">
+        <f t="shared" si="5"/>
+        <v>131</v>
+      </c>
+      <c r="B132" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="C132" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="D132" s="1">
+        <v>43187</v>
+      </c>
+      <c r="E132" s="46">
+        <v>2018</v>
+      </c>
+      <c r="F132" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="G132" s="46">
+        <v>1</v>
+      </c>
+      <c r="H132" s="46">
+        <v>0</v>
+      </c>
+      <c r="I132" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="J132" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="K132" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="L132" s="35"/>
+      <c r="M132" s="35"/>
+      <c r="N132" s="35"/>
+      <c r="O132" s="35"/>
+      <c r="P132" s="35"/>
+      <c r="Q132" s="35"/>
+      <c r="R132" s="35"/>
+      <c r="S132" s="35"/>
+      <c r="T132" s="35"/>
+      <c r="U132" s="35"/>
+      <c r="V132" s="35"/>
+      <c r="W132" s="35"/>
+      <c r="X132" s="35"/>
+      <c r="Y132" s="35"/>
+      <c r="Z132" s="35"/>
     </row>
   </sheetData>
   <sortState ref="N3:O7">

</xml_diff>

<commit_message>
Botafogo x vasco 01042018
</commit_message>
<xml_diff>
--- a/Jogos do Botafogo que já fui.xlsx
+++ b/Jogos do Botafogo que já fui.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="116">
   <si>
     <t>Sim</t>
   </si>
@@ -1148,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE132"/>
+  <dimension ref="A1:AE133"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E131" sqref="E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,7 +1307,7 @@
       </c>
       <c r="M2" s="16">
         <f>COUNTIF(B3:B1005,"Vasco")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>38</v>
@@ -1321,7 +1321,7 @@
       </c>
       <c r="Q2" s="6">
         <f>COUNTIF(J1:J1004,"Nilton Santos")</f>
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R2" s="24">
         <v>2002</v>
@@ -1340,19 +1340,19 @@
       </c>
       <c r="V2" s="23">
         <f>COUNTIF(F2:F1007, "Derrota")</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="W2" s="15">
         <f>SUM(G3:G1001)</f>
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="X2" s="48">
         <f>SUM(H3:H1001)</f>
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="Y2" s="50">
         <f>COUNTIF(K3:K1006,"Sim")</f>
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Z2" s="47">
         <f>COUNTIF(K3:K1006,"Não")</f>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="O3" s="7">
         <f>COUNTIF(I3:I1007,"Carioca")</f>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>23</v>
@@ -2393,7 +2393,7 @@
       </c>
       <c r="S17" s="46">
         <f>COUNTIF(E124:E159, "2018")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="T17" s="41"/>
       <c r="U17" s="37"/>
@@ -7626,7 +7626,7 @@
     </row>
     <row r="109" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A109" s="46">
-        <f t="shared" ref="A109:A132" si="5">SUM(A108+1)</f>
+        <f t="shared" ref="A109:A133" si="5">SUM(A108+1)</f>
         <v>108</v>
       </c>
       <c r="B109" s="46" t="s">
@@ -8848,6 +8848,42 @@
       <c r="Y132" s="35"/>
       <c r="Z132" s="35"/>
     </row>
+    <row r="133" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A133" s="46">
+        <f t="shared" si="5"/>
+        <v>132</v>
+      </c>
+      <c r="B133" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C133" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="D133" s="1">
+        <v>43191</v>
+      </c>
+      <c r="E133" s="46">
+        <v>2018</v>
+      </c>
+      <c r="F133" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="G133" s="46">
+        <v>2</v>
+      </c>
+      <c r="H133" s="46">
+        <v>3</v>
+      </c>
+      <c r="I133" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="J133" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K133" s="46" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="N3:O7">
     <sortCondition descending="1" ref="O3:O7"/>

</xml_diff>

<commit_message>
BOTAFOGO CAMPEÃO CARIOCA 2018
</commit_message>
<xml_diff>
--- a/Jogos do Botafogo que já fui.xlsx
+++ b/Jogos do Botafogo que já fui.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hfogo_000\Documents\GitHub\JogosDoBotafogo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="116">
   <si>
     <t>Sim</t>
   </si>
@@ -377,8 +372,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -389,6 +384,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -716,7 +719,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -868,6 +871,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -928,7 +932,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -963,7 +967,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1140,21 +1144,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE133"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AE135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E131" sqref="E131"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J135" sqref="J135"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
@@ -1183,7 +1187,7 @@
     <col min="25" max="26" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31">
       <c r="A1" s="46" t="s">
         <v>72</v>
       </c>
@@ -1268,7 +1272,7 @@
       <c r="AD1" s="35"/>
       <c r="AE1" s="35"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1307,7 +1311,7 @@
       </c>
       <c r="M2" s="16">
         <f>COUNTIF(B3:B1005,"Vasco")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>38</v>
@@ -1332,7 +1336,7 @@
       </c>
       <c r="T2" s="21">
         <f>COUNTIF(F2:F1007, "Vitória")</f>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="U2" s="46">
         <f>COUNTIF(F2:F1007, "Empate")</f>
@@ -1348,11 +1352,11 @@
       </c>
       <c r="X2" s="48">
         <f>SUM(H3:H1001)</f>
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Y2" s="50">
         <f>COUNTIF(K3:K1006,"Sim")</f>
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="Z2" s="47">
         <f>COUNTIF(K3:K1006,"Não")</f>
@@ -1364,7 +1368,7 @@
       <c r="AD2" s="35"/>
       <c r="AE2" s="35"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1410,14 +1414,14 @@
       </c>
       <c r="O3" s="7">
         <f>COUNTIF(I3:I1007,"Carioca")</f>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>23</v>
       </c>
       <c r="Q3" s="7">
         <f>COUNTIF(J3:J1008,"Maracanã")</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R3" s="21">
         <v>2004</v>
@@ -1439,7 +1443,7 @@
       <c r="AD3" s="35"/>
       <c r="AE3" s="35"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31">
       <c r="A4" s="46">
         <f>SUM(A3+1)</f>
         <v>3</v>
@@ -1515,7 +1519,7 @@
       <c r="AD4" s="35"/>
       <c r="AE4" s="35"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31">
       <c r="A5" s="46">
         <f t="shared" ref="A5:A6" si="0">SUM(A4+1)</f>
         <v>4</v>
@@ -1591,7 +1595,7 @@
       <c r="AD5" s="35"/>
       <c r="AE5" s="35"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31">
       <c r="A6" s="46">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1667,7 +1671,7 @@
       <c r="AD6" s="35"/>
       <c r="AE6" s="35"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31">
       <c r="A7" s="46">
         <f t="shared" ref="A7:A17" si="1">SUM(A6+1)</f>
         <v>6</v>
@@ -1738,7 +1742,7 @@
       <c r="AD7" s="35"/>
       <c r="AE7" s="35"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31">
       <c r="A8" s="46">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1809,7 +1813,7 @@
       <c r="AD8" s="35"/>
       <c r="AE8" s="35"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31">
       <c r="A9" s="46">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -1880,7 +1884,7 @@
       <c r="AD9" s="35"/>
       <c r="AE9" s="35"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31">
       <c r="A10" s="46">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1946,7 +1950,7 @@
       <c r="AD10" s="35"/>
       <c r="AE10" s="35"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31">
       <c r="A11" s="46">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -2012,7 +2016,7 @@
       <c r="AD11" s="35"/>
       <c r="AE11" s="35"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31">
       <c r="A12" s="46">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -2078,7 +2082,7 @@
       <c r="AD12" s="35"/>
       <c r="AE12" s="35"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31">
       <c r="A13" s="46">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -2144,7 +2148,7 @@
       <c r="AD13" s="35"/>
       <c r="AE13" s="35"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31">
       <c r="A14" s="46">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -2210,7 +2214,7 @@
       <c r="AD14" s="35"/>
       <c r="AE14" s="35"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31">
       <c r="A15" s="46">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -2276,7 +2280,7 @@
       <c r="AD15" s="35"/>
       <c r="AE15" s="35"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31">
       <c r="A16" s="46">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -2342,7 +2346,7 @@
       <c r="AD16" s="35"/>
       <c r="AE16" s="35"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31">
       <c r="A17" s="46">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -2393,7 +2397,7 @@
       </c>
       <c r="S17" s="46">
         <f>COUNTIF(E124:E159, "2018")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T17" s="41"/>
       <c r="U17" s="37"/>
@@ -2408,7 +2412,7 @@
       <c r="AD17" s="35"/>
       <c r="AE17" s="35"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31">
       <c r="A18" s="46">
         <f t="shared" ref="A18:A23" si="2">SUM(A17+1)</f>
         <v>17</v>
@@ -2469,7 +2473,7 @@
       <c r="AD18" s="35"/>
       <c r="AE18" s="35"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31">
       <c r="A19" s="46">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -2530,7 +2534,7 @@
       <c r="AD19" s="35"/>
       <c r="AE19" s="35"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31">
       <c r="A20" s="46">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -2591,7 +2595,7 @@
       <c r="AD20" s="35"/>
       <c r="AE20" s="35"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31">
       <c r="A21" s="46">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -2652,7 +2656,7 @@
       <c r="AD21" s="35"/>
       <c r="AE21" s="35"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31">
       <c r="A22" s="46">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -2713,7 +2717,7 @@
       <c r="AD22" s="35"/>
       <c r="AE22" s="35"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31">
       <c r="A23" s="46">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -2774,7 +2778,7 @@
       <c r="AD23" s="35"/>
       <c r="AE23" s="35"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31">
       <c r="A24" s="46">
         <f t="shared" ref="A24:A38" si="3">SUM(A23+1)</f>
         <v>23</v>
@@ -2835,7 +2839,7 @@
       <c r="AD24" s="35"/>
       <c r="AE24" s="35"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31">
       <c r="A25" s="46">
         <f t="shared" si="3"/>
         <v>24</v>
@@ -2896,7 +2900,7 @@
       <c r="AD25" s="35"/>
       <c r="AE25" s="35"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31">
       <c r="A26" s="46">
         <f t="shared" si="3"/>
         <v>25</v>
@@ -2957,7 +2961,7 @@
       <c r="AD26" s="35"/>
       <c r="AE26" s="35"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31">
       <c r="A27" s="46">
         <f t="shared" si="3"/>
         <v>26</v>
@@ -3018,7 +3022,7 @@
       <c r="AD27" s="35"/>
       <c r="AE27" s="35"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31">
       <c r="A28" s="46">
         <f t="shared" si="3"/>
         <v>27</v>
@@ -3079,7 +3083,7 @@
       <c r="AD28" s="35"/>
       <c r="AE28" s="35"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31">
       <c r="A29" s="46">
         <f t="shared" si="3"/>
         <v>28</v>
@@ -3140,7 +3144,7 @@
       <c r="AD29" s="35"/>
       <c r="AE29" s="35"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31">
       <c r="A30" s="46">
         <f t="shared" si="3"/>
         <v>29</v>
@@ -3201,7 +3205,7 @@
       <c r="AD30" s="35"/>
       <c r="AE30" s="35"/>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31">
       <c r="A31" s="46">
         <f t="shared" si="3"/>
         <v>30</v>
@@ -3262,7 +3266,7 @@
       <c r="AD31" s="35"/>
       <c r="AE31" s="35"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31">
       <c r="A32" s="46">
         <f t="shared" si="3"/>
         <v>31</v>
@@ -3323,7 +3327,7 @@
       <c r="AD32" s="35"/>
       <c r="AE32" s="35"/>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31">
       <c r="A33" s="46">
         <f t="shared" si="3"/>
         <v>32</v>
@@ -3384,7 +3388,7 @@
       <c r="AD33" s="35"/>
       <c r="AE33" s="35"/>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31">
       <c r="A34" s="46">
         <f t="shared" si="3"/>
         <v>33</v>
@@ -3445,7 +3449,7 @@
       <c r="AD34" s="35"/>
       <c r="AE34" s="35"/>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31">
       <c r="A35" s="46">
         <f t="shared" si="3"/>
         <v>34</v>
@@ -3506,7 +3510,7 @@
       <c r="AD35" s="35"/>
       <c r="AE35" s="35"/>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31">
       <c r="A36" s="46">
         <f t="shared" si="3"/>
         <v>35</v>
@@ -3567,7 +3571,7 @@
       <c r="AD36" s="35"/>
       <c r="AE36" s="35"/>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31">
       <c r="A37" s="46">
         <f t="shared" si="3"/>
         <v>36</v>
@@ -3628,7 +3632,7 @@
       <c r="AD37" s="35"/>
       <c r="AE37" s="35"/>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31">
       <c r="A38" s="46">
         <f t="shared" si="3"/>
         <v>37</v>
@@ -3689,7 +3693,7 @@
       <c r="AD38" s="35"/>
       <c r="AE38" s="35"/>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31">
       <c r="A39" s="46">
         <f t="shared" ref="A39:A108" si="4">SUM(A38+1)</f>
         <v>38</v>
@@ -3750,7 +3754,7 @@
       <c r="AD39" s="35"/>
       <c r="AE39" s="35"/>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31">
       <c r="A40" s="46">
         <f t="shared" si="4"/>
         <v>39</v>
@@ -3811,7 +3815,7 @@
       <c r="AD40" s="35"/>
       <c r="AE40" s="35"/>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:31">
       <c r="A41" s="46">
         <f t="shared" si="4"/>
         <v>40</v>
@@ -3872,7 +3876,7 @@
       <c r="AD41" s="35"/>
       <c r="AE41" s="35"/>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:31">
       <c r="A42" s="46">
         <f t="shared" si="4"/>
         <v>41</v>
@@ -3933,7 +3937,7 @@
       <c r="AD42" s="35"/>
       <c r="AE42" s="35"/>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:31">
       <c r="A43" s="46">
         <f t="shared" si="4"/>
         <v>42</v>
@@ -3994,7 +3998,7 @@
       <c r="AD43" s="35"/>
       <c r="AE43" s="35"/>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:31">
       <c r="A44" s="46">
         <f t="shared" si="4"/>
         <v>43</v>
@@ -4055,7 +4059,7 @@
       <c r="AD44" s="35"/>
       <c r="AE44" s="35"/>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:31">
       <c r="A45" s="46">
         <f t="shared" si="4"/>
         <v>44</v>
@@ -4116,7 +4120,7 @@
       <c r="AD45" s="35"/>
       <c r="AE45" s="35"/>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:31">
       <c r="A46" s="46">
         <f t="shared" si="4"/>
         <v>45</v>
@@ -4177,7 +4181,7 @@
       <c r="AD46" s="35"/>
       <c r="AE46" s="35"/>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:31">
       <c r="A47" s="46">
         <f t="shared" si="4"/>
         <v>46</v>
@@ -4238,7 +4242,7 @@
       <c r="AD47" s="35"/>
       <c r="AE47" s="35"/>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:31">
       <c r="A48" s="42">
         <f t="shared" si="4"/>
         <v>47</v>
@@ -4299,7 +4303,7 @@
       <c r="AD48" s="35"/>
       <c r="AE48" s="35"/>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:31">
       <c r="A49" s="46">
         <f t="shared" si="4"/>
         <v>48</v>
@@ -4360,7 +4364,7 @@
       <c r="AD49" s="35"/>
       <c r="AE49" s="35"/>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:31">
       <c r="A50" s="46">
         <f t="shared" si="4"/>
         <v>49</v>
@@ -4416,7 +4420,7 @@
       <c r="AD50" s="35"/>
       <c r="AE50" s="35"/>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:31">
       <c r="A51" s="46">
         <f t="shared" si="4"/>
         <v>50</v>
@@ -4472,7 +4476,7 @@
       <c r="AD51" s="35"/>
       <c r="AE51" s="35"/>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:31">
       <c r="A52" s="46">
         <f t="shared" si="4"/>
         <v>51</v>
@@ -4528,7 +4532,7 @@
       <c r="AD52" s="35"/>
       <c r="AE52" s="35"/>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:31">
       <c r="A53" s="46">
         <f t="shared" si="4"/>
         <v>52</v>
@@ -4584,7 +4588,7 @@
       <c r="AD53" s="35"/>
       <c r="AE53" s="35"/>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:31">
       <c r="A54" s="46">
         <f t="shared" si="4"/>
         <v>53</v>
@@ -4640,7 +4644,7 @@
       <c r="AD54" s="35"/>
       <c r="AE54" s="35"/>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:31">
       <c r="A55" s="46">
         <f t="shared" si="4"/>
         <v>54</v>
@@ -4696,7 +4700,7 @@
       <c r="AD55" s="35"/>
       <c r="AE55" s="35"/>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:31">
       <c r="A56" s="46">
         <f t="shared" si="4"/>
         <v>55</v>
@@ -4752,7 +4756,7 @@
       <c r="AD56" s="35"/>
       <c r="AE56" s="35"/>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:31">
       <c r="A57" s="46">
         <f t="shared" si="4"/>
         <v>56</v>
@@ -4808,7 +4812,7 @@
       <c r="AD57" s="35"/>
       <c r="AE57" s="35"/>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:31">
       <c r="A58" s="46">
         <f t="shared" si="4"/>
         <v>57</v>
@@ -4864,7 +4868,7 @@
       <c r="AD58" s="35"/>
       <c r="AE58" s="35"/>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:31">
       <c r="A59" s="46">
         <f t="shared" si="4"/>
         <v>58</v>
@@ -4920,7 +4924,7 @@
       <c r="AD59" s="35"/>
       <c r="AE59" s="35"/>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:31">
       <c r="A60" s="46">
         <f t="shared" si="4"/>
         <v>59</v>
@@ -4976,7 +4980,7 @@
       <c r="AD60" s="35"/>
       <c r="AE60" s="35"/>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:31">
       <c r="A61" s="46">
         <f t="shared" si="4"/>
         <v>60</v>
@@ -5032,7 +5036,7 @@
       <c r="AD61" s="35"/>
       <c r="AE61" s="35"/>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:31">
       <c r="A62" s="46">
         <f t="shared" si="4"/>
         <v>61</v>
@@ -5088,7 +5092,7 @@
       <c r="AD62" s="35"/>
       <c r="AE62" s="35"/>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:31">
       <c r="A63" s="46">
         <f t="shared" si="4"/>
         <v>62</v>
@@ -5144,7 +5148,7 @@
       <c r="AD63" s="35"/>
       <c r="AE63" s="35"/>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:31">
       <c r="A64" s="46">
         <f t="shared" si="4"/>
         <v>63</v>
@@ -5200,7 +5204,7 @@
       <c r="AD64" s="35"/>
       <c r="AE64" s="35"/>
     </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:31">
       <c r="A65" s="46">
         <f t="shared" si="4"/>
         <v>64</v>
@@ -5256,7 +5260,7 @@
       <c r="AD65" s="35"/>
       <c r="AE65" s="35"/>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:31">
       <c r="A66" s="46">
         <f t="shared" si="4"/>
         <v>65</v>
@@ -5312,7 +5316,7 @@
       <c r="AD66" s="35"/>
       <c r="AE66" s="35"/>
     </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:31">
       <c r="A67" s="46">
         <f t="shared" si="4"/>
         <v>66</v>
@@ -5368,7 +5372,7 @@
       <c r="AD67" s="35"/>
       <c r="AE67" s="35"/>
     </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:31">
       <c r="A68" s="46">
         <f t="shared" si="4"/>
         <v>67</v>
@@ -5424,7 +5428,7 @@
       <c r="AD68" s="35"/>
       <c r="AE68" s="35"/>
     </row>
-    <row r="69" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:31">
       <c r="A69" s="46">
         <f t="shared" si="4"/>
         <v>68</v>
@@ -5480,7 +5484,7 @@
       <c r="AD69" s="35"/>
       <c r="AE69" s="35"/>
     </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:31">
       <c r="A70" s="46">
         <f t="shared" si="4"/>
         <v>69</v>
@@ -5536,7 +5540,7 @@
       <c r="AD70" s="35"/>
       <c r="AE70" s="35"/>
     </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:31">
       <c r="A71" s="46">
         <f t="shared" si="4"/>
         <v>70</v>
@@ -5592,7 +5596,7 @@
       <c r="AD71" s="35"/>
       <c r="AE71" s="35"/>
     </row>
-    <row r="72" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:31">
       <c r="A72" s="46">
         <f t="shared" si="4"/>
         <v>71</v>
@@ -5648,7 +5652,7 @@
       <c r="AD72" s="35"/>
       <c r="AE72" s="35"/>
     </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:31">
       <c r="A73" s="46">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -5704,7 +5708,7 @@
       <c r="AD73" s="35"/>
       <c r="AE73" s="35"/>
     </row>
-    <row r="74" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:31">
       <c r="A74" s="46">
         <f t="shared" si="4"/>
         <v>73</v>
@@ -5760,7 +5764,7 @@
       <c r="AD74" s="35"/>
       <c r="AE74" s="35"/>
     </row>
-    <row r="75" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:31">
       <c r="A75" s="46">
         <f t="shared" si="4"/>
         <v>74</v>
@@ -5816,7 +5820,7 @@
       <c r="AD75" s="35"/>
       <c r="AE75" s="35"/>
     </row>
-    <row r="76" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:31">
       <c r="A76" s="46">
         <f t="shared" si="4"/>
         <v>75</v>
@@ -5872,7 +5876,7 @@
       <c r="AD76" s="35"/>
       <c r="AE76" s="35"/>
     </row>
-    <row r="77" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:31">
       <c r="A77" s="46">
         <f t="shared" si="4"/>
         <v>76</v>
@@ -5928,7 +5932,7 @@
       <c r="AD77" s="35"/>
       <c r="AE77" s="35"/>
     </row>
-    <row r="78" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:31">
       <c r="A78" s="46">
         <f t="shared" si="4"/>
         <v>77</v>
@@ -5984,7 +5988,7 @@
       <c r="AD78" s="35"/>
       <c r="AE78" s="35"/>
     </row>
-    <row r="79" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:31">
       <c r="A79" s="46">
         <f t="shared" si="4"/>
         <v>78</v>
@@ -6040,7 +6044,7 @@
       <c r="AD79" s="35"/>
       <c r="AE79" s="35"/>
     </row>
-    <row r="80" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:31">
       <c r="A80" s="46">
         <f t="shared" si="4"/>
         <v>79</v>
@@ -6096,7 +6100,7 @@
       <c r="AD80" s="35"/>
       <c r="AE80" s="35"/>
     </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:31">
       <c r="A81" s="46">
         <f t="shared" si="4"/>
         <v>80</v>
@@ -6152,7 +6156,7 @@
       <c r="AD81" s="35"/>
       <c r="AE81" s="35"/>
     </row>
-    <row r="82" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:31">
       <c r="A82" s="46">
         <f t="shared" si="4"/>
         <v>81</v>
@@ -6208,7 +6212,7 @@
       <c r="AD82" s="35"/>
       <c r="AE82" s="35"/>
     </row>
-    <row r="83" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:31">
       <c r="A83" s="46">
         <f t="shared" si="4"/>
         <v>82</v>
@@ -6264,7 +6268,7 @@
       <c r="AD83" s="35"/>
       <c r="AE83" s="35"/>
     </row>
-    <row r="84" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:31">
       <c r="A84" s="46">
         <f t="shared" si="4"/>
         <v>83</v>
@@ -6320,7 +6324,7 @@
       <c r="AD84" s="35"/>
       <c r="AE84" s="35"/>
     </row>
-    <row r="85" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:31">
       <c r="A85" s="46">
         <f t="shared" si="4"/>
         <v>84</v>
@@ -6376,7 +6380,7 @@
       <c r="AD85" s="35"/>
       <c r="AE85" s="35"/>
     </row>
-    <row r="86" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:31">
       <c r="A86" s="46">
         <f t="shared" si="4"/>
         <v>85</v>
@@ -6432,7 +6436,7 @@
       <c r="AD86" s="35"/>
       <c r="AE86" s="35"/>
     </row>
-    <row r="87" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:31">
       <c r="A87" s="46">
         <f t="shared" si="4"/>
         <v>86</v>
@@ -6488,7 +6492,7 @@
       <c r="AD87" s="35"/>
       <c r="AE87" s="35"/>
     </row>
-    <row r="88" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:31">
       <c r="A88" s="42">
         <f t="shared" si="4"/>
         <v>87</v>
@@ -6544,7 +6548,7 @@
       <c r="AD88" s="35"/>
       <c r="AE88" s="35"/>
     </row>
-    <row r="89" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:31">
       <c r="A89" s="46">
         <f t="shared" si="4"/>
         <v>88</v>
@@ -6600,7 +6604,7 @@
       <c r="AD89" s="35"/>
       <c r="AE89" s="35"/>
     </row>
-    <row r="90" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:31">
       <c r="A90" s="46">
         <f t="shared" si="4"/>
         <v>89</v>
@@ -6656,7 +6660,7 @@
       <c r="AD90" s="35"/>
       <c r="AE90" s="35"/>
     </row>
-    <row r="91" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:31">
       <c r="A91" s="46">
         <f t="shared" si="4"/>
         <v>90</v>
@@ -6712,7 +6716,7 @@
       <c r="AD91" s="35"/>
       <c r="AE91" s="35"/>
     </row>
-    <row r="92" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:31">
       <c r="A92" s="46">
         <f t="shared" si="4"/>
         <v>91</v>
@@ -6768,7 +6772,7 @@
       <c r="AD92" s="35"/>
       <c r="AE92" s="35"/>
     </row>
-    <row r="93" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:31">
       <c r="A93" s="46">
         <f t="shared" si="4"/>
         <v>92</v>
@@ -6824,7 +6828,7 @@
       <c r="AD93" s="35"/>
       <c r="AE93" s="35"/>
     </row>
-    <row r="94" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:31">
       <c r="A94" s="46">
         <f t="shared" si="4"/>
         <v>93</v>
@@ -6880,7 +6884,7 @@
       <c r="AD94" s="35"/>
       <c r="AE94" s="35"/>
     </row>
-    <row r="95" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:31">
       <c r="A95" s="46">
         <f t="shared" si="4"/>
         <v>94</v>
@@ -6936,7 +6940,7 @@
       <c r="AD95" s="35"/>
       <c r="AE95" s="35"/>
     </row>
-    <row r="96" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:31">
       <c r="A96" s="46">
         <f t="shared" si="4"/>
         <v>95</v>
@@ -6992,7 +6996,7 @@
       <c r="AD96" s="35"/>
       <c r="AE96" s="35"/>
     </row>
-    <row r="97" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:31">
       <c r="A97" s="46">
         <f t="shared" si="4"/>
         <v>96</v>
@@ -7048,7 +7052,7 @@
       <c r="AD97" s="35"/>
       <c r="AE97" s="35"/>
     </row>
-    <row r="98" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:31">
       <c r="A98" s="46">
         <f t="shared" si="4"/>
         <v>97</v>
@@ -7104,7 +7108,7 @@
       <c r="AD98" s="35"/>
       <c r="AE98" s="35"/>
     </row>
-    <row r="99" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:31">
       <c r="A99" s="42">
         <f t="shared" si="4"/>
         <v>98</v>
@@ -7160,7 +7164,7 @@
       <c r="AD99" s="35"/>
       <c r="AE99" s="35"/>
     </row>
-    <row r="100" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:31">
       <c r="A100" s="46">
         <f t="shared" si="4"/>
         <v>99</v>
@@ -7216,7 +7220,7 @@
       <c r="AD100" s="35"/>
       <c r="AE100" s="35"/>
     </row>
-    <row r="101" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:31">
       <c r="A101" s="46">
         <f t="shared" si="4"/>
         <v>100</v>
@@ -7267,7 +7271,7 @@
       <c r="Y101" s="35"/>
       <c r="Z101" s="35"/>
     </row>
-    <row r="102" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:31">
       <c r="A102" s="42">
         <f t="shared" si="4"/>
         <v>101</v>
@@ -7318,7 +7322,7 @@
       <c r="Y102" s="35"/>
       <c r="Z102" s="35"/>
     </row>
-    <row r="103" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:31">
       <c r="A103" s="42">
         <f t="shared" si="4"/>
         <v>102</v>
@@ -7369,7 +7373,7 @@
       <c r="Y103" s="35"/>
       <c r="Z103" s="35"/>
     </row>
-    <row r="104" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:31">
       <c r="A104" s="46">
         <f t="shared" si="4"/>
         <v>103</v>
@@ -7420,7 +7424,7 @@
       <c r="Y104" s="35"/>
       <c r="Z104" s="35"/>
     </row>
-    <row r="105" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:31">
       <c r="A105" s="42">
         <f t="shared" si="4"/>
         <v>104</v>
@@ -7471,7 +7475,7 @@
       <c r="Y105" s="35"/>
       <c r="Z105" s="35"/>
     </row>
-    <row r="106" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:31">
       <c r="A106" s="46">
         <f t="shared" si="4"/>
         <v>105</v>
@@ -7522,7 +7526,7 @@
       <c r="Y106" s="35"/>
       <c r="Z106" s="35"/>
     </row>
-    <row r="107" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:31">
       <c r="A107" s="42">
         <f t="shared" si="4"/>
         <v>106</v>
@@ -7573,7 +7577,7 @@
       <c r="Y107" s="35"/>
       <c r="Z107" s="35"/>
     </row>
-    <row r="108" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:31">
       <c r="A108" s="46">
         <f t="shared" si="4"/>
         <v>107</v>
@@ -7624,9 +7628,9 @@
       <c r="Y108" s="35"/>
       <c r="Z108" s="35"/>
     </row>
-    <row r="109" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:31">
       <c r="A109" s="46">
-        <f t="shared" ref="A109:A133" si="5">SUM(A108+1)</f>
+        <f t="shared" ref="A109:A134" si="5">SUM(A108+1)</f>
         <v>108</v>
       </c>
       <c r="B109" s="46" t="s">
@@ -7675,7 +7679,7 @@
       <c r="Y109" s="35"/>
       <c r="Z109" s="35"/>
     </row>
-    <row r="110" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:31">
       <c r="A110" s="46">
         <f t="shared" si="5"/>
         <v>109</v>
@@ -7726,7 +7730,7 @@
       <c r="Y110" s="35"/>
       <c r="Z110" s="35"/>
     </row>
-    <row r="111" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:31">
       <c r="A111" s="42">
         <f t="shared" si="5"/>
         <v>110</v>
@@ -7777,7 +7781,7 @@
       <c r="Y111" s="35"/>
       <c r="Z111" s="35"/>
     </row>
-    <row r="112" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:31">
       <c r="A112" s="46">
         <f t="shared" si="5"/>
         <v>111</v>
@@ -7828,7 +7832,7 @@
       <c r="Y112" s="35"/>
       <c r="Z112" s="35"/>
     </row>
-    <row r="113" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:26">
       <c r="A113" s="46">
         <f t="shared" si="5"/>
         <v>112</v>
@@ -7879,7 +7883,7 @@
       <c r="Y113" s="35"/>
       <c r="Z113" s="35"/>
     </row>
-    <row r="114" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:26">
       <c r="A114" s="46">
         <f t="shared" si="5"/>
         <v>113</v>
@@ -7930,7 +7934,7 @@
       <c r="Y114" s="35"/>
       <c r="Z114" s="35"/>
     </row>
-    <row r="115" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:26">
       <c r="A115" s="46">
         <f t="shared" si="5"/>
         <v>114</v>
@@ -7981,7 +7985,7 @@
       <c r="Y115" s="35"/>
       <c r="Z115" s="35"/>
     </row>
-    <row r="116" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:26">
       <c r="A116" s="46">
         <f t="shared" si="5"/>
         <v>115</v>
@@ -8032,7 +8036,7 @@
       <c r="Y116" s="35"/>
       <c r="Z116" s="35"/>
     </row>
-    <row r="117" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:26">
       <c r="A117" s="46">
         <f t="shared" si="5"/>
         <v>116</v>
@@ -8083,7 +8087,7 @@
       <c r="Y117" s="35"/>
       <c r="Z117" s="35"/>
     </row>
-    <row r="118" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:26">
       <c r="A118" s="46">
         <f t="shared" si="5"/>
         <v>117</v>
@@ -8134,7 +8138,7 @@
       <c r="Y118" s="35"/>
       <c r="Z118" s="35"/>
     </row>
-    <row r="119" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:26">
       <c r="A119" s="46">
         <f t="shared" si="5"/>
         <v>118</v>
@@ -8185,7 +8189,7 @@
       <c r="Y119" s="35"/>
       <c r="Z119" s="35"/>
     </row>
-    <row r="120" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:26">
       <c r="A120" s="46">
         <f t="shared" si="5"/>
         <v>119</v>
@@ -8236,7 +8240,7 @@
       <c r="Y120" s="35"/>
       <c r="Z120" s="35"/>
     </row>
-    <row r="121" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:26">
       <c r="A121" s="46">
         <f t="shared" si="5"/>
         <v>120</v>
@@ -8287,7 +8291,7 @@
       <c r="Y121" s="35"/>
       <c r="Z121" s="35"/>
     </row>
-    <row r="122" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:26">
       <c r="A122" s="46">
         <f t="shared" si="5"/>
         <v>121</v>
@@ -8338,7 +8342,7 @@
       <c r="Y122" s="35"/>
       <c r="Z122" s="35"/>
     </row>
-    <row r="123" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:26">
       <c r="A123" s="46">
         <f t="shared" si="5"/>
         <v>122</v>
@@ -8389,7 +8393,7 @@
       <c r="Y123" s="35"/>
       <c r="Z123" s="35"/>
     </row>
-    <row r="124" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:26">
       <c r="A124" s="46">
         <f t="shared" si="5"/>
         <v>123</v>
@@ -8440,7 +8444,7 @@
       <c r="Y124" s="35"/>
       <c r="Z124" s="35"/>
     </row>
-    <row r="125" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:26">
       <c r="A125" s="46">
         <f t="shared" si="5"/>
         <v>124</v>
@@ -8491,7 +8495,7 @@
       <c r="Y125" s="35"/>
       <c r="Z125" s="35"/>
     </row>
-    <row r="126" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:26">
       <c r="A126" s="46">
         <f t="shared" si="5"/>
         <v>125</v>
@@ -8542,7 +8546,7 @@
       <c r="Y126" s="35"/>
       <c r="Z126" s="35"/>
     </row>
-    <row r="127" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:26">
       <c r="A127" s="46">
         <f t="shared" si="5"/>
         <v>126</v>
@@ -8593,7 +8597,7 @@
       <c r="Y127" s="35"/>
       <c r="Z127" s="35"/>
     </row>
-    <row r="128" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:26">
       <c r="A128" s="42">
         <f t="shared" si="5"/>
         <v>127</v>
@@ -8644,7 +8648,7 @@
       <c r="Y128" s="35"/>
       <c r="Z128" s="35"/>
     </row>
-    <row r="129" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:26">
       <c r="A129" s="46">
         <f t="shared" si="5"/>
         <v>128</v>
@@ -8695,7 +8699,7 @@
       <c r="Y129" s="35"/>
       <c r="Z129" s="35"/>
     </row>
-    <row r="130" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:26">
       <c r="A130" s="46">
         <f t="shared" si="5"/>
         <v>129</v>
@@ -8746,7 +8750,7 @@
       <c r="Y130" s="35"/>
       <c r="Z130" s="35"/>
     </row>
-    <row r="131" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:26">
       <c r="A131" s="46">
         <f t="shared" si="5"/>
         <v>130</v>
@@ -8797,7 +8801,7 @@
       <c r="Y131" s="35"/>
       <c r="Z131" s="35"/>
     </row>
-    <row r="132" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:26">
       <c r="A132" s="46">
         <f t="shared" si="5"/>
         <v>131</v>
@@ -8848,7 +8852,7 @@
       <c r="Y132" s="35"/>
       <c r="Z132" s="35"/>
     </row>
-    <row r="133" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:26">
       <c r="A133" s="46">
         <f t="shared" si="5"/>
         <v>132</v>
@@ -8883,6 +8887,45 @@
       <c r="K133" s="46" t="s">
         <v>0</v>
       </c>
+    </row>
+    <row r="134" spans="1:26">
+      <c r="A134" s="46">
+        <f t="shared" si="5"/>
+        <v>133</v>
+      </c>
+      <c r="B134" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C134" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="D134" s="1">
+        <v>43198</v>
+      </c>
+      <c r="E134" s="46">
+        <v>2018</v>
+      </c>
+      <c r="F134" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="G134" s="46">
+        <v>0</v>
+      </c>
+      <c r="H134" s="46">
+        <v>1</v>
+      </c>
+      <c r="I134" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="J134" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="K134" s="46" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:26">
+      <c r="J135" s="51"/>
     </row>
   </sheetData>
   <sortState ref="N3:O7">

</xml_diff>

<commit_message>
Botafogo x Grêmio 28042018
</commit_message>
<xml_diff>
--- a/Jogos do Botafogo que já fui.xlsx
+++ b/Jogos do Botafogo que já fui.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="117">
   <si>
     <t>Sim</t>
   </si>
@@ -381,7 +381,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,14 +392,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -727,7 +719,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -879,7 +871,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1163,22 +1154,22 @@
   <dimension ref="A1:AE135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A107" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+      <selection activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" customWidth="1"/>
     <col min="12" max="12" width="24" customWidth="1"/>
     <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -1326,14 +1317,14 @@
       </c>
       <c r="O2" s="6">
         <f>COUNTIF(I3:I1007,"Série A")</f>
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="Q2" s="6">
         <f>COUNTIF(J1:J1004,"Nilton Santos")</f>
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R2" s="24">
         <v>2002</v>
@@ -1344,7 +1335,7 @@
       </c>
       <c r="T2" s="21">
         <f>COUNTIF(F2:F1007, "Vitória")</f>
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="U2" s="46">
         <f>COUNTIF(F2:F1007, "Empate")</f>
@@ -1356,15 +1347,15 @@
       </c>
       <c r="W2" s="15">
         <f>SUM(G3:G1001)</f>
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="X2" s="48">
         <f>SUM(H3:H1001)</f>
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Y2" s="50">
         <f>COUNTIF(K3:K1006,"Sim")</f>
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Z2" s="47">
         <f>COUNTIF(K3:K1006,"Não")</f>
@@ -1567,7 +1558,7 @@
       </c>
       <c r="M5" s="17">
         <f>COUNTIF(B3:B1005,"Grêmio")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N5" s="22" t="s">
         <v>43</v>
@@ -2405,7 +2396,7 @@
       </c>
       <c r="S17" s="46">
         <f>COUNTIF(E124:E159, "2018")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T17" s="41"/>
       <c r="U17" s="37"/>
@@ -7638,7 +7629,7 @@
     </row>
     <row r="109" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A109" s="46">
-        <f t="shared" ref="A109:A134" si="5">SUM(A108+1)</f>
+        <f t="shared" ref="A109:A135" si="5">SUM(A108+1)</f>
         <v>108</v>
       </c>
       <c r="B109" s="46" t="s">
@@ -8933,7 +8924,40 @@
       </c>
     </row>
     <row r="135" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="J135" s="51"/>
+      <c r="A135" s="46">
+        <f t="shared" si="5"/>
+        <v>134</v>
+      </c>
+      <c r="B135" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C135" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="D135" s="1">
+        <v>43218</v>
+      </c>
+      <c r="E135" s="46">
+        <v>2018</v>
+      </c>
+      <c r="F135" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="G135" s="46">
+        <v>2</v>
+      </c>
+      <c r="H135" s="46">
+        <v>1</v>
+      </c>
+      <c r="I135" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="J135" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K135" s="46" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="N3:O7">

</xml_diff>

<commit_message>
bota 2 x 1 flu 14052018
</commit_message>
<xml_diff>
--- a/Jogos do Botafogo que já fui.xlsx
+++ b/Jogos do Botafogo que já fui.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="119">
   <si>
     <t>Sim</t>
   </si>
@@ -1210,10 +1210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE136"/>
+  <dimension ref="A1:AE137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J147" sqref="J147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,14 +1376,14 @@
       </c>
       <c r="O2" s="6">
         <f>COUNTIF(I3:I1007,"Série A")</f>
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="P2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="Q2" s="6">
         <f>COUNTIF(J1:J1004,"Nilton Santos")</f>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R2" s="24">
         <v>2002</v>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="T2" s="21">
         <f>COUNTIF(F2:F1007, "Vitória")</f>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="U2" s="46">
         <f>COUNTIF(F2:F1007, "Empate")</f>
@@ -1406,15 +1406,15 @@
       </c>
       <c r="W2" s="15">
         <f>SUM(G3:G1001)</f>
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="X2" s="48">
         <f>SUM(H3:H1001)</f>
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="Y2" s="50">
         <f>COUNTIF(K3:K1006,"Sim")</f>
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Z2" s="47">
         <f>COUNTIF(K3:K1006,"Não")</f>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="M3" s="17">
         <f>COUNTIF(B3:B1005,"Fluminense")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>24</v>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="S17" s="46">
         <f>COUNTIF(E124:E159, "2018")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T17" s="41"/>
       <c r="U17" s="37"/>
@@ -7698,7 +7698,7 @@
     </row>
     <row r="109" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A109" s="46">
-        <f t="shared" ref="A109:A136" si="5">SUM(A108+1)</f>
+        <f t="shared" ref="A109:A137" si="5">SUM(A108+1)</f>
         <v>108</v>
       </c>
       <c r="B109" s="46" t="s">
@@ -9064,6 +9064,42 @@
         <v>0</v>
       </c>
     </row>
+    <row r="137" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A137" s="46">
+        <f t="shared" si="5"/>
+        <v>136</v>
+      </c>
+      <c r="B137" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="C137" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="D137" s="1">
+        <v>43234</v>
+      </c>
+      <c r="E137" s="46">
+        <v>2018</v>
+      </c>
+      <c r="F137" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="G137" s="46">
+        <v>2</v>
+      </c>
+      <c r="H137" s="46">
+        <v>1</v>
+      </c>
+      <c r="I137" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="J137" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K137" s="46" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="N3:O7">
     <sortCondition descending="1" ref="O3:O7"/>

</xml_diff>

<commit_message>
bota x santos com o santos depressivo e o cope
</commit_message>
<xml_diff>
--- a/Jogos do Botafogo que já fui.xlsx
+++ b/Jogos do Botafogo que já fui.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="120">
   <si>
     <t>Sim</t>
   </si>
@@ -7059,6 +7059,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1648115</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>1501805</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="148" name="Imagem 147"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId83" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2000250" y="220408500"/>
+          <a:ext cx="1362365" cy="1335118"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7325,10 +7369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF141"/>
+  <dimension ref="A1:AF142"/>
   <sheetViews>
-    <sheetView topLeftCell="A137" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="K141" sqref="K141"/>
+    <sheetView topLeftCell="A135" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="G142" sqref="G142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12875,7 +12919,7 @@
     </row>
     <row r="109" spans="1:32" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6">
-        <f t="shared" ref="A109:A141" si="4">SUM(A108+1)</f>
+        <f t="shared" ref="A109:A142" si="4">SUM(A108+1)</f>
         <v>108</v>
       </c>
       <c r="B109" s="15"/>
@@ -14517,6 +14561,43 @@
         <v>1</v>
       </c>
       <c r="L141" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:27" ht="123" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A142" s="6">
+        <f t="shared" si="4"/>
+        <v>141</v>
+      </c>
+      <c r="B142" s="48"/>
+      <c r="C142" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D142" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E142" s="22">
+        <v>43316</v>
+      </c>
+      <c r="F142" s="7">
+        <v>2018</v>
+      </c>
+      <c r="G142" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H142" s="7">
+        <v>0</v>
+      </c>
+      <c r="I142" s="7">
+        <v>0</v>
+      </c>
+      <c r="J142" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K142" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L142" s="6" t="s">
         <v>0</v>
       </c>
     </row>
@@ -14546,8 +14627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14613,14 +14694,14 @@
       </c>
       <c r="D2" s="14">
         <f>COUNTIF(Principal!J3:J1007,"Série A")</f>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="14">
         <f>COUNTIF(Principal!K1:K1004,"Nilton Santos")</f>
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G2" s="7">
         <v>2002</v>
@@ -14635,7 +14716,7 @@
       </c>
       <c r="J2" s="7">
         <f>COUNTIF(Principal!G2:G1007, "Empate")</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K2" s="7">
         <f>COUNTIF(Principal!G2:G1007, "Derrota")</f>
@@ -14851,7 +14932,7 @@
       </c>
       <c r="J8" s="50">
         <f>COUNTIF(Principal!L3:L1006,"Sim")</f>
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K8" s="25"/>
     </row>
@@ -15061,7 +15142,7 @@
       </c>
       <c r="H17" s="7">
         <f>COUNTIF(Principal!F124:F159, "2018")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I17" s="21"/>
       <c r="J17" s="29"/>
@@ -15163,7 +15244,7 @@
       </c>
       <c r="B23" s="18">
         <f>COUNTIF(Principal!C3:C1013,"Santos")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C23" s="25"/>
       <c r="D23" s="25"/>

</xml_diff>

<commit_message>
rumo aos 46 pontos
</commit_message>
<xml_diff>
--- a/Jogos do Botafogo que já fui.xlsx
+++ b/Jogos do Botafogo que já fui.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Principal" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="125">
   <si>
     <t>Sim</t>
   </si>
@@ -760,7 +760,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -920,6 +920,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7408,6 +7414,50 @@
         <a:xfrm>
           <a:off x="1985964" y="229704900"/>
           <a:ext cx="1333500" cy="1542249"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>309563</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>1546894</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="155" name="Imagem 154"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId56" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2024063" y="231362251"/>
+          <a:ext cx="1214437" cy="1427831"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7682,10 +7732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF148"/>
+  <dimension ref="A1:AF149"/>
   <sheetViews>
-    <sheetView topLeftCell="A143" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="K149" sqref="K149"/>
+    <sheetView tabSelected="1" topLeftCell="A143" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14531,24 +14581,24 @@
         <v>122</v>
       </c>
       <c r="B134" s="26"/>
-      <c r="C134" s="57" t="s">
+      <c r="C134" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="D134" s="56"/>
+      <c r="D134" s="58"/>
       <c r="E134" s="22">
         <v>43197</v>
       </c>
-      <c r="F134" s="54" t="s">
+      <c r="F134" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="G134" s="55"/>
-      <c r="H134" s="55"/>
-      <c r="I134" s="55"/>
-      <c r="J134" s="56"/>
-      <c r="K134" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="L134" s="55"/>
+      <c r="G134" s="57"/>
+      <c r="H134" s="57"/>
+      <c r="I134" s="57"/>
+      <c r="J134" s="58"/>
+      <c r="K134" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="L134" s="57"/>
       <c r="M134" s="19"/>
       <c r="N134" s="19"/>
       <c r="O134" s="19"/>
@@ -15099,7 +15149,7 @@
     </row>
     <row r="148" spans="1:12" ht="123" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A148" s="52">
-        <f t="shared" si="4"/>
+        <f>SUM(A147+1)</f>
         <v>146</v>
       </c>
       <c r="B148" s="48"/>
@@ -15119,10 +15169,10 @@
         <v>86</v>
       </c>
       <c r="H148" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I148" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J148" s="7" t="s">
         <v>38</v>
@@ -15131,6 +15181,43 @@
         <v>23</v>
       </c>
       <c r="L148" s="52" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" ht="123" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A149" s="54">
+        <f>SUM(A148+1)</f>
+        <v>147</v>
+      </c>
+      <c r="B149" s="48"/>
+      <c r="C149" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="D149" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E149" s="22">
+        <v>43359</v>
+      </c>
+      <c r="F149" s="7">
+        <v>2018</v>
+      </c>
+      <c r="G149" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H149" s="7">
+        <v>1</v>
+      </c>
+      <c r="I149" s="7">
+        <v>0</v>
+      </c>
+      <c r="J149" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K149" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L149" s="54" t="s">
         <v>0</v>
       </c>
     </row>
@@ -15165,7 +15252,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -15232,14 +15319,14 @@
       </c>
       <c r="D2" s="14">
         <f>COUNTIF(Principal!J3:J1008,"Série A")</f>
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="14">
         <f>COUNTIF(Principal!K1:K1005,"Nilton Santos")</f>
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G2" s="7">
         <v>2002</v>
@@ -15250,7 +15337,7 @@
       </c>
       <c r="I2" s="7">
         <f>COUNTIF(Principal!G2:G1008, "Vitória")</f>
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J2" s="7">
         <f>COUNTIF(Principal!G2:G1008, "Empate")</f>
@@ -15366,7 +15453,7 @@
       </c>
       <c r="J5" s="24">
         <f>SUM(Principal!I3:I1002)</f>
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K5" s="21"/>
     </row>
@@ -15470,7 +15557,7 @@
       </c>
       <c r="J8" s="50">
         <f>COUNTIF(Principal!L3:L1007,"Sim")</f>
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K8" s="25"/>
     </row>
@@ -15680,7 +15767,7 @@
       </c>
       <c r="H17" s="7">
         <f>COUNTIF(Principal!F124:F160, "2018")</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I17" s="21"/>
       <c r="J17" s="29"/>
@@ -15800,7 +15887,7 @@
       </c>
       <c r="B24" s="18">
         <f>COUNTIF(Principal!C3:C996,"América-MG")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" s="25"/>
       <c r="D24" s="25"/>

</xml_diff>

<commit_message>
é amigo... ta difícil
</commit_message>
<xml_diff>
--- a/Jogos do Botafogo que já fui.xlsx
+++ b/Jogos do Botafogo que já fui.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="126">
   <si>
     <t>Sim</t>
   </si>
@@ -763,7 +763,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -947,6 +947,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7611,6 +7617,50 @@
         <a:xfrm>
           <a:off x="1952625" y="236053313"/>
           <a:ext cx="1452562" cy="1452562"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>271462</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1652587</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>1485900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="159" name="Imagem 158"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1985962" y="237634463"/>
+          <a:ext cx="1381125" cy="1381125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7885,10 +7935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF152"/>
+  <dimension ref="A1:AF153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="B152" sqref="B152"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="C153" sqref="C153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14734,24 +14784,24 @@
         <v>122</v>
       </c>
       <c r="B134" s="26"/>
-      <c r="C134" s="65" t="s">
+      <c r="C134" s="67" t="s">
         <v>123</v>
       </c>
-      <c r="D134" s="64"/>
+      <c r="D134" s="66"/>
       <c r="E134" s="22">
         <v>43197</v>
       </c>
-      <c r="F134" s="62" t="s">
+      <c r="F134" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="G134" s="63"/>
-      <c r="H134" s="63"/>
-      <c r="I134" s="63"/>
-      <c r="J134" s="64"/>
-      <c r="K134" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="L134" s="63"/>
+      <c r="G134" s="65"/>
+      <c r="H134" s="65"/>
+      <c r="I134" s="65"/>
+      <c r="J134" s="66"/>
+      <c r="K134" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="L134" s="65"/>
       <c r="M134" s="19"/>
       <c r="N134" s="19"/>
       <c r="O134" s="19"/>
@@ -15482,6 +15532,43 @@
         <v>1</v>
       </c>
       <c r="L152" s="60" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" ht="123" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A153" s="62">
+        <f>SUM(A152+1)</f>
+        <v>151</v>
+      </c>
+      <c r="B153" s="48"/>
+      <c r="C153" s="63" t="s">
+        <v>40</v>
+      </c>
+      <c r="D153" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E153" s="22">
+        <v>43393</v>
+      </c>
+      <c r="F153" s="7">
+        <v>2018</v>
+      </c>
+      <c r="G153" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H153" s="7">
+        <v>0</v>
+      </c>
+      <c r="I153" s="7">
+        <v>1</v>
+      </c>
+      <c r="J153" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K153" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L153" s="62" t="s">
         <v>0</v>
       </c>
     </row>
@@ -15583,14 +15670,14 @@
       </c>
       <c r="D2" s="14">
         <f>COUNTIF(Principal!J3:J1008,"Série A")</f>
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="14">
         <f>COUNTIF(Principal!K1:K1005,"Nilton Santos")</f>
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G2" s="7">
         <v>2002</v>
@@ -15609,7 +15696,7 @@
       </c>
       <c r="K2" s="7">
         <f>COUNTIF(Principal!G2:G1008, "Derrota")</f>
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
@@ -15717,7 +15804,7 @@
       </c>
       <c r="J5" s="24">
         <f>SUM(Principal!I3:I1002)</f>
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K5" s="21"/>
     </row>
@@ -15821,7 +15908,7 @@
       </c>
       <c r="J8" s="50">
         <f>COUNTIF(Principal!L3:L1007,"Sim")</f>
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K8" s="25"/>
     </row>
@@ -15928,7 +16015,7 @@
       </c>
       <c r="B13" s="18">
         <f>COUNTIF(Principal!C3:C1000,"Bahia")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="25"/>
@@ -16031,7 +16118,7 @@
       </c>
       <c r="H17" s="7">
         <f>COUNTIF(Principal!F124:F160, "2018")</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I17" s="21"/>
       <c r="J17" s="29"/>

</xml_diff>

<commit_message>
troquei o são caetano de lugar pq a data tava errada
</commit_message>
<xml_diff>
--- a/Jogos do Botafogo que já fui.xlsx
+++ b/Jogos do Botafogo que já fui.xlsx
@@ -857,7 +857,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1074,6 +1074,9 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1681,13 +1684,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>266701</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1581151</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>12282</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1725,13 +1728,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1577318</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1769,13 +1772,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1657350</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>1504950</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1813,13 +1816,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1428750</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>1503199</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1857,13 +1860,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1600200</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>1507998</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1901,13 +1904,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>152401</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1657351</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>1543051</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1945,13 +1948,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>152401</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1714501</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>6858</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -8237,8 +8240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="F156" sqref="F156"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8576,7 +8579,7 @@
     </row>
     <row r="7" spans="1:34" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
-        <f t="shared" ref="A7:A17" si="0">SUM(A6+1)</f>
+        <f t="shared" ref="A7:A22" si="0">SUM(A6+1)</f>
         <v>6</v>
       </c>
       <c r="B7" s="15"/>
@@ -8991,19 +8994,19 @@
       <c r="AH14" s="1"/>
     </row>
     <row r="15" spans="1:34" ht="123" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="74">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="8" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E15" s="22">
-        <v>38647</v>
+        <v>38668</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>126</v>
@@ -9018,7 +9021,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" s="71" t="s">
         <v>157</v>
@@ -9027,14 +9030,11 @@
         <v>38</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="N15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="5"/>
-      <c r="AB15" s="3"/>
       <c r="AC15" s="2"/>
       <c r="AD15" s="1"/>
       <c r="AE15" s="1"/>
@@ -9043,43 +9043,43 @@
       <c r="AH15" s="1"/>
     </row>
     <row r="16" spans="1:34" ht="123" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="A16" s="74">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="8" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="E16" s="22">
-        <v>38668</v>
+        <v>38739</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G16" s="24">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="H16" s="22" t="s">
         <v>20</v>
       </c>
       <c r="I16" s="23">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J16" s="24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K16" s="71" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="N16" s="6" t="s">
         <v>49</v>
@@ -9095,19 +9095,19 @@
       <c r="AH16" s="1"/>
     </row>
     <row r="17" spans="1:34" ht="123" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="A17" s="74">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="8" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="E17" s="22">
-        <v>38739</v>
+        <v>38767</v>
       </c>
       <c r="F17" s="22" t="s">
         <v>127</v>
@@ -9116,13 +9116,13 @@
         <v>2006</v>
       </c>
       <c r="H17" s="22" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="I17" s="23">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J17" s="24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K17" s="71" t="s">
         <v>158</v>
@@ -9147,19 +9147,19 @@
       <c r="AH17" s="1"/>
     </row>
     <row r="18" spans="1:34" ht="123" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <f t="shared" ref="A18:A23" si="1">SUM(A17+1)</f>
+      <c r="A18" s="74">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="15"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="8" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="E18" s="22">
-        <v>38767</v>
+        <v>38816</v>
       </c>
       <c r="F18" s="22" t="s">
         <v>127</v>
@@ -9168,10 +9168,10 @@
         <v>2006</v>
       </c>
       <c r="H18" s="22" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="I18" s="23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J18" s="24">
         <v>1</v>
@@ -9199,40 +9199,40 @@
       <c r="AH18" s="1"/>
     </row>
     <row r="19" spans="1:34" ht="123" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="32">
-        <f t="shared" si="1"/>
+      <c r="A19" s="74">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="26"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="8" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="E19" s="22">
-        <v>38816</v>
+        <v>38850</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G19" s="24">
         <v>2006</v>
       </c>
       <c r="H19" s="22" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="I19" s="23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J19" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K19" s="71" t="s">
         <v>158</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="M19" s="7" t="s">
         <v>23</v>
@@ -9251,19 +9251,19 @@
       <c r="AH19" s="1"/>
     </row>
     <row r="20" spans="1:34" ht="123" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
-        <f t="shared" si="1"/>
+      <c r="A20" s="74">
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="E20" s="22">
-        <v>38850</v>
+        <v>39004</v>
       </c>
       <c r="F20" s="22" t="s">
         <v>126</v>
@@ -9272,16 +9272,16 @@
         <v>2006</v>
       </c>
       <c r="H20" s="22" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="I20" s="23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J20" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K20" s="71" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="L20" s="7" t="s">
         <v>38</v>
@@ -9303,19 +9303,19 @@
       <c r="AH20" s="1"/>
     </row>
     <row r="21" spans="1:34" ht="123" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <f t="shared" si="1"/>
+      <c r="A21" s="74">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="8" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="E21" s="22">
-        <v>39004</v>
+        <v>39012</v>
       </c>
       <c r="F21" s="22" t="s">
         <v>126</v>
@@ -9327,13 +9327,13 @@
         <v>20</v>
       </c>
       <c r="I21" s="23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J21" s="24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K21" s="71" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="L21" s="7" t="s">
         <v>38</v>
@@ -9355,8 +9355,8 @@
       <c r="AH21" s="1"/>
     </row>
     <row r="22" spans="1:34" ht="123" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
-        <f t="shared" si="1"/>
+      <c r="A22" s="74">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="15"/>
@@ -9408,7 +9408,7 @@
     </row>
     <row r="23" spans="1:34" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A18:A23" si="1">SUM(A22+1)</f>
         <v>22</v>
       </c>
       <c r="B23" s="15"/>
@@ -15883,26 +15883,26 @@
         <v>121</v>
       </c>
       <c r="B134" s="26"/>
-      <c r="C134" s="74" t="s">
+      <c r="C134" s="75" t="s">
         <v>122</v>
       </c>
-      <c r="D134" s="75"/>
+      <c r="D134" s="76"/>
       <c r="E134" s="22">
         <v>43197</v>
       </c>
-      <c r="F134" s="76" t="s">
+      <c r="F134" s="77" t="s">
         <v>123</v>
       </c>
-      <c r="G134" s="75"/>
-      <c r="H134" s="75"/>
-      <c r="I134" s="75"/>
-      <c r="J134" s="75"/>
-      <c r="K134" s="75"/>
-      <c r="L134" s="77"/>
-      <c r="M134" s="76" t="s">
-        <v>1</v>
-      </c>
-      <c r="N134" s="75"/>
+      <c r="G134" s="76"/>
+      <c r="H134" s="76"/>
+      <c r="I134" s="76"/>
+      <c r="J134" s="76"/>
+      <c r="K134" s="76"/>
+      <c r="L134" s="78"/>
+      <c r="M134" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="N134" s="76"/>
       <c r="O134" s="19"/>
       <c r="P134" s="19"/>
       <c r="Q134" s="19"/>
@@ -17158,8 +17158,8 @@
         <v>2005</v>
       </c>
       <c r="H4" s="6">
-        <f>COUNTIF(Principal!G10:G16, "2005")</f>
-        <v>7</v>
+        <f>COUNTIF(Principal!G10:G15, "2005")</f>
+        <v>6</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>92</v>
@@ -17202,8 +17202,8 @@
         <v>2006</v>
       </c>
       <c r="H5" s="6">
-        <f>COUNTIF(Principal!G17:G23, "2006")</f>
-        <v>7</v>
+        <f>COUNTIF(Principal!G16:G23, "2006")</f>
+        <v>8</v>
       </c>
       <c r="I5" s="48">
         <f>SUM(Principal!I3:I1002)</f>

</xml_diff>

<commit_message>
mudança em algumas datas
</commit_message>
<xml_diff>
--- a/Jogos do Botafogo que já fui.xlsx
+++ b/Jogos do Botafogo que já fui.xlsx
@@ -8240,8 +8240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8798,7 +8798,7 @@
         <v>61</v>
       </c>
       <c r="E11" s="22">
-        <v>38434</v>
+        <v>38424</v>
       </c>
       <c r="F11" s="22" t="s">
         <v>127</v>
@@ -9408,7 +9408,7 @@
     </row>
     <row r="23" spans="1:34" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
-        <f t="shared" ref="A18:A23" si="1">SUM(A22+1)</f>
+        <f t="shared" ref="A23" si="1">SUM(A22+1)</f>
         <v>22</v>
       </c>
       <c r="B23" s="15"/>

</xml_diff>